<commit_message>
token for localhost ignored
</commit_message>
<xml_diff>
--- a/results/publications.xlsx
+++ b/results/publications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="451">
   <si>
     <t>title</t>
   </si>
@@ -324,6 +324,33 @@
     <t>Correction to: Meeting report from the fourth meeting of the Computational Modeling in Biology Network (COMBINE).</t>
   </si>
   <si>
+    <t>Effect of alcohol on the interleukin 6-mediated inflammatory response in a new mouse model of acute-on-chronic liver injury.</t>
+  </si>
+  <si>
+    <t>Liver-specific Repin1 deficiency impairs transient hepatic steatosis in liver regeneration.</t>
+  </si>
+  <si>
+    <t>ABCB4 Gene Aberrations in Human Liver Disease: An Evolving Spectrum</t>
+  </si>
+  <si>
+    <t>Effects of Gene Variants Controlling Vitamin D Metabolism and Serum Levels on Hepatic Steatosis.</t>
+  </si>
+  <si>
+    <t>Analytical challenges in human plasma lipidomics: A winding path towards the truth</t>
+  </si>
+  <si>
+    <t>Epigenomic map of human liver reveals principles of zonated morphogenic and metabolic control</t>
+  </si>
+  <si>
+    <t>The Diurnal Timing of Starvation Differently Impacts Murine Hepatic Gene Expression and Lipid Metabolism – A Systems Biology Analysis Using Self-Organizing Maps</t>
+  </si>
+  <si>
+    <t>Clinical and Functional Relevance of the Monocarboxylate Transporter Family in Disease Pathophysiology and Drug Therapy.</t>
+  </si>
+  <si>
+    <t>The fruit fly Drosophila melanogaster as an innovative preclinical ADME model for solute carrier membrane transporters, with consequences for pharmacology and drug therapy.</t>
+  </si>
+  <si>
     <t>J Integr Bioinform</t>
   </si>
   <si>
@@ -519,6 +546,21 @@
     <t>Stand Genomic Sci</t>
   </si>
   <si>
+    <t>Biochim Biophys Acta Mol Basis Dis</t>
+  </si>
+  <si>
+    <t>Semin Liver Dis</t>
+  </si>
+  <si>
+    <t>TrAC Trends in Analytical Chemistry</t>
+  </si>
+  <si>
+    <t>Clin Transl Sci</t>
+  </si>
+  <si>
+    <t>Drug Discov Today</t>
+  </si>
+  <si>
     <t>2017-02-12</t>
   </si>
   <si>
@@ -657,6 +699,30 @@
     <t>2018-08-13</t>
   </si>
   <si>
+    <t>2018-01-18</t>
+  </si>
+  <si>
+    <t>2018-10-24</t>
+  </si>
+  <si>
+    <t>2018-03-08</t>
+  </si>
+  <si>
+    <t>2018-10-20</t>
+  </si>
+  <si>
+    <t>2018-12-01</t>
+  </si>
+  <si>
+    <t>2018-09-10</t>
+  </si>
+  <si>
+    <t>2018-04-17</t>
+  </si>
+  <si>
+    <t>2018-06-12</t>
+  </si>
+  <si>
     <t>J Integr Bioinform. 2016 Dec 18;13(3):289. doi: 10.2390/biecoll-jib-2016-289.</t>
   </si>
   <si>
@@ -918,6 +984,33 @@
     <t>Stand Genomic Sci. 2018 Aug 9;13:17. doi: 10.1186/s40793-018-0320-4. eCollection  2018.</t>
   </si>
   <si>
+    <t>Biochim Biophys Acta Mol Basis Dis. 2018 Nov 15;1865(2):298-307. doi: 10.1016/j.bbadis.2018.11.008.</t>
+  </si>
+  <si>
+    <t>Sci Rep. 2018 Nov 15;8(1):16858. doi: 10.1038/s41598-018-35325-3.</t>
+  </si>
+  <si>
+    <t>Semin Liver Dis 38(04) : 299</t>
+  </si>
+  <si>
+    <t>Digestion. 2018;97(4):298-308. doi: 10.1159/000485180. Epub 2018 Mar 7.</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S016599361830428X?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Nat Commun 9(1) : 416</t>
+  </si>
+  <si>
+    <t>Front. Physiol. 9 : 660</t>
+  </si>
+  <si>
+    <t>Clin Transl Sci. 2018 Jul;11(4):352-364. doi: 10.1111/cts.12551. Epub 2018 Apr 16.</t>
+  </si>
+  <si>
+    <t>Drug Discov Today. 2018 Oct;23(10):1746-1760. doi: 10.1016/j.drudis.2018.06.002.  Epub 2018 Jun 8.</t>
+  </si>
+  <si>
     <t>['F. Schreiber', 'G. D. Bader', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'N. Le Novere', 'C. Myers', 'D. Nickerson', 'B. Sommer', 'D. Walthemath']</t>
   </si>
   <si>
@@ -1203,6 +1296,30 @@
     <t>['D. Waltemath', 'F. T. Bergmann', 'C. Chaouiya', 'T. Czauderna', 'P. Gleeson', 'C. Goble', 'Martin Golebiewski', 'M. Hucka', 'N. Juty', 'O. Krebs', 'N. Le Novere', 'H. Mi', 'I. I. Moraru', 'C. J. Myers', 'D. Nickerson', 'B. G. Olivier', 'N. Rodriguez', 'F. Schreiber', 'L. Smith', 'F. Zhang', 'E. Bonnet']</t>
   </si>
   <si>
+    <t>['Ersin Karatayli', 'R. A. Hall', 'Susanne Weber', 'Steven Dooley', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['K. Abshagen', 'B. Degenhardt', 'M. Liebig', 'A. Wendt', 'B. Genz', 'U. Schaeper', 'M. Stumvoll', 'Ute Hofmann', 'M. Frank', 'B. Vollmar', 'N. Kloting']</t>
+  </si>
+  <si>
+    <t>['Matthias Reichert', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['M. Jamka', 'A. Arslanow', 'A. Bohner', 'M. Krawczyk', 'Susanne Weber', 'F. Grunhage', 'Frank Lammert', 'C. S. Stokes']</t>
+  </si>
+  <si>
+    <t>['Olga Vvedenskaya', 'Yuting Wang', 'Jacobo Miranda Ackerman', 'Oskar Knittelfelder', 'Andrej Shevchenko']</t>
+  </si>
+  <si>
+    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Thomas Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
+  </si>
+  <si>
+    <t>['Christiane Rennert', 'Sebastian Vlaic', 'Eugenia Marbach-Breitrück', 'Carlo Thiel', 'Susanne Sales', 'Andrej Shevchenko', 'Rolf Gebhardt', 'Madlen Matz-Soja']</t>
+  </si>
+  <si>
+    <t>['Y. Wang', 'B. Moussian', 'E. Schaeffeler', 'Matthias Schwab', 'A. T. Nies']</t>
+  </si>
+  <si>
     <t>{'data': [{'id': '2', 'type': 'projects'}]}</t>
   </si>
   <si>
@@ -1249,13 +1366,16 @@
   </si>
   <si>
     <t>{'data': [{'id': '10', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1270,6 +1390,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1304,16 +1431,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1606,7 +1739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1637,19 +1770,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="E2" t="s">
-        <v>300</v>
+        <v>331</v>
       </c>
       <c r="F2" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1657,19 +1790,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="E3" t="s">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="F3" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1677,19 +1810,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="E4" t="s">
-        <v>302</v>
+        <v>333</v>
       </c>
       <c r="F4" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1697,19 +1830,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="E5" t="s">
-        <v>303</v>
+        <v>334</v>
       </c>
       <c r="F5" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1717,19 +1850,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="E6" t="s">
-        <v>304</v>
+        <v>335</v>
       </c>
       <c r="F6" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1737,19 +1870,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="E7" t="s">
-        <v>305</v>
+        <v>336</v>
       </c>
       <c r="F7" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1757,19 +1890,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="E8" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="F8" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1777,19 +1910,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="E9" t="s">
-        <v>307</v>
+        <v>338</v>
       </c>
       <c r="F9" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1797,19 +1930,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="E10" t="s">
-        <v>308</v>
+        <v>339</v>
       </c>
       <c r="F10" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1817,19 +1950,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="E11" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="F11" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1837,19 +1970,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="E12" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="F12" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1857,19 +1990,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="E13" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="F13" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1877,19 +2010,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="E14" t="s">
-        <v>312</v>
+        <v>343</v>
       </c>
       <c r="F14" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1897,19 +2030,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="E15" t="s">
-        <v>313</v>
+        <v>344</v>
       </c>
       <c r="F15" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1917,19 +2050,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="E16" t="s">
-        <v>314</v>
+        <v>345</v>
       </c>
       <c r="F16" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1937,19 +2070,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="E17" t="s">
-        <v>315</v>
+        <v>346</v>
       </c>
       <c r="F17" t="s">
-        <v>400</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1957,19 +2090,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="E18" t="s">
-        <v>316</v>
+        <v>347</v>
       </c>
       <c r="F18" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1977,19 +2110,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="D19" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="E19" t="s">
-        <v>317</v>
+        <v>348</v>
       </c>
       <c r="F19" t="s">
-        <v>401</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1997,19 +2130,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="E20" t="s">
-        <v>318</v>
+        <v>349</v>
       </c>
       <c r="F20" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2017,19 +2150,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="E21" t="s">
-        <v>319</v>
+        <v>350</v>
       </c>
       <c r="F21" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2037,19 +2170,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="E22" t="s">
-        <v>320</v>
+        <v>351</v>
       </c>
       <c r="F22" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2057,19 +2190,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="E23" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
       <c r="F23" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2077,19 +2210,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="D24" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="E24" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
       <c r="F24" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2097,19 +2230,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="E25" t="s">
-        <v>323</v>
+        <v>354</v>
       </c>
       <c r="F25" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2117,19 +2250,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="D26" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="E26" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="F26" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2137,19 +2270,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="D27" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="E27" t="s">
-        <v>325</v>
+        <v>356</v>
       </c>
       <c r="F27" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2157,19 +2290,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="E28" t="s">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="F28" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2177,19 +2310,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D29" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="E29" t="s">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="F29" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2197,19 +2330,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="E30" t="s">
-        <v>327</v>
+        <v>358</v>
       </c>
       <c r="F30" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2217,19 +2350,19 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="D31" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="E31" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="F31" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2237,19 +2370,19 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D32" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="E32" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
       <c r="F32" t="s">
-        <v>401</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2257,19 +2390,19 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="D33" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="E33" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="F33" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2277,19 +2410,19 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="D34" t="s">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="E34" t="s">
-        <v>331</v>
+        <v>362</v>
       </c>
       <c r="F34" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2297,19 +2430,19 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="E35" t="s">
-        <v>332</v>
+        <v>363</v>
       </c>
       <c r="F35" t="s">
-        <v>403</v>
+        <v>442</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2317,19 +2450,19 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D36" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="E36" t="s">
-        <v>333</v>
+        <v>364</v>
       </c>
       <c r="F36" t="s">
-        <v>404</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2337,16 +2470,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="E37" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="F37" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2354,16 +2487,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="D38" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="E38" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="F38" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2371,16 +2504,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="E39" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="F39" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2388,16 +2521,16 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D40" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="E40" t="s">
-        <v>337</v>
+        <v>368</v>
       </c>
       <c r="F40" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2405,19 +2538,19 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D41" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="E41" t="s">
-        <v>338</v>
+        <v>369</v>
       </c>
       <c r="F41" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2425,19 +2558,19 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="D42" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="E42" t="s">
-        <v>339</v>
+        <v>370</v>
       </c>
       <c r="F42" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2445,16 +2578,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="E43" t="s">
-        <v>340</v>
+        <v>371</v>
       </c>
       <c r="F43" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2462,16 +2595,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D44" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="E44" t="s">
-        <v>341</v>
+        <v>372</v>
       </c>
       <c r="F44" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2479,16 +2612,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D45" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="E45" t="s">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="F45" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2496,16 +2629,16 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D46" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="E46" t="s">
-        <v>343</v>
+        <v>374</v>
       </c>
       <c r="F46" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2513,16 +2646,16 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="E47" t="s">
-        <v>344</v>
+        <v>375</v>
       </c>
       <c r="F47" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2530,16 +2663,16 @@
         <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="E48" t="s">
-        <v>312</v>
+        <v>343</v>
       </c>
       <c r="F48" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2547,16 +2680,16 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="E49" t="s">
-        <v>345</v>
+        <v>376</v>
       </c>
       <c r="F49" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2564,16 +2697,16 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="E50" t="s">
-        <v>346</v>
+        <v>377</v>
       </c>
       <c r="F50" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2581,19 +2714,19 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D51" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="E51" t="s">
-        <v>347</v>
+        <v>378</v>
       </c>
       <c r="F51" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2601,19 +2734,19 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D52" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="E52" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="F52" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2621,16 +2754,16 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="E53" t="s">
-        <v>349</v>
+        <v>380</v>
       </c>
       <c r="F53" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2638,19 +2771,19 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="E54" t="s">
-        <v>350</v>
+        <v>381</v>
       </c>
       <c r="F54" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2658,19 +2791,19 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C55" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="D55" t="s">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="E55" t="s">
-        <v>351</v>
+        <v>382</v>
       </c>
       <c r="F55" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2678,19 +2811,19 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D56" t="s">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="E56" t="s">
-        <v>352</v>
+        <v>383</v>
       </c>
       <c r="F56" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2698,19 +2831,19 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="D57" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="E57" t="s">
-        <v>353</v>
+        <v>384</v>
       </c>
       <c r="F57" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2718,19 +2851,19 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="D58" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="E58" t="s">
-        <v>354</v>
+        <v>385</v>
       </c>
       <c r="F58" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2738,19 +2871,19 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D59" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="E59" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="F59" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2758,19 +2891,19 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="D60" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="E60" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
       <c r="F60" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2778,19 +2911,19 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="D61" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="E61" t="s">
-        <v>357</v>
+        <v>388</v>
       </c>
       <c r="F61" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2798,19 +2931,19 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C62" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="D62" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="E62" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="F62" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2818,19 +2951,19 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="E63" t="s">
-        <v>359</v>
+        <v>390</v>
       </c>
       <c r="F63" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2838,19 +2971,19 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D64" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="E64" t="s">
-        <v>360</v>
+        <v>391</v>
       </c>
       <c r="F64" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2858,16 +2991,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D65" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="E65" t="s">
-        <v>361</v>
+        <v>392</v>
       </c>
       <c r="F65" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2875,16 +3008,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D66" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="E66" t="s">
-        <v>362</v>
+        <v>393</v>
       </c>
       <c r="F66" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2892,16 +3025,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D67" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="E67" t="s">
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="F67" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2909,16 +3042,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D68" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="E68" t="s">
-        <v>364</v>
+        <v>395</v>
       </c>
       <c r="F68" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2926,16 +3059,16 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D69" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="E69" t="s">
-        <v>365</v>
+        <v>396</v>
       </c>
       <c r="F69" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2943,16 +3076,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D70" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
       <c r="E70" t="s">
-        <v>366</v>
+        <v>397</v>
       </c>
       <c r="F70" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2960,13 +3093,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="E71" t="s">
-        <v>367</v>
+        <v>398</v>
       </c>
       <c r="F71" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2974,16 +3107,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D72" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="E72" t="s">
-        <v>368</v>
+        <v>399</v>
       </c>
       <c r="F72" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2991,16 +3124,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D73" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="E73" t="s">
-        <v>369</v>
+        <v>400</v>
       </c>
       <c r="F73" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3008,16 +3141,16 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C74" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E74" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
       <c r="F74" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3025,16 +3158,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E75" t="s">
-        <v>371</v>
+        <v>402</v>
       </c>
       <c r="F75" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3042,13 +3175,13 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E76" t="s">
-        <v>372</v>
+        <v>403</v>
       </c>
       <c r="F76" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3056,16 +3189,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D77" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="E77" t="s">
-        <v>373</v>
+        <v>404</v>
       </c>
       <c r="F77" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3073,16 +3206,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C78" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="E78" t="s">
-        <v>374</v>
+        <v>405</v>
       </c>
       <c r="F78" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3090,16 +3223,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="E79" t="s">
-        <v>375</v>
+        <v>406</v>
       </c>
       <c r="F79" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3107,16 +3240,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>281</v>
+        <v>303</v>
       </c>
       <c r="E80" t="s">
-        <v>376</v>
+        <v>407</v>
       </c>
       <c r="F80" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3124,16 +3257,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D81" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="E81" t="s">
-        <v>377</v>
+        <v>408</v>
       </c>
       <c r="F81" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3141,16 +3274,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="E82" t="s">
-        <v>378</v>
+        <v>409</v>
       </c>
       <c r="F82" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3158,16 +3291,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="D83" t="s">
-        <v>284</v>
+        <v>306</v>
       </c>
       <c r="E83" t="s">
-        <v>379</v>
+        <v>410</v>
       </c>
       <c r="F83" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3175,16 +3308,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D84" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="E84" t="s">
-        <v>380</v>
+        <v>411</v>
       </c>
       <c r="F84" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3192,16 +3325,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D85" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="E85" t="s">
-        <v>381</v>
+        <v>412</v>
       </c>
       <c r="F85" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3209,16 +3342,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D86" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="E86" t="s">
-        <v>382</v>
+        <v>413</v>
       </c>
       <c r="F86" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3226,16 +3359,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D87" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="E87" t="s">
-        <v>383</v>
+        <v>414</v>
       </c>
       <c r="F87" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3243,16 +3376,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="D88" t="s">
-        <v>289</v>
+        <v>311</v>
       </c>
       <c r="E88" t="s">
-        <v>384</v>
+        <v>415</v>
       </c>
       <c r="F88" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3260,16 +3393,16 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="D89" t="s">
-        <v>290</v>
+        <v>312</v>
       </c>
       <c r="E89" t="s">
-        <v>385</v>
+        <v>416</v>
       </c>
       <c r="F89" t="s">
-        <v>410</v>
+        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3277,16 +3410,16 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D90" t="s">
-        <v>291</v>
+        <v>313</v>
       </c>
       <c r="E90" t="s">
-        <v>386</v>
+        <v>417</v>
       </c>
       <c r="F90" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3294,19 +3427,19 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C91" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="D91" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="E91" t="s">
-        <v>387</v>
+        <v>418</v>
       </c>
       <c r="F91" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3314,19 +3447,19 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C92" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="D92" t="s">
-        <v>293</v>
+        <v>315</v>
       </c>
       <c r="E92" t="s">
-        <v>388</v>
+        <v>419</v>
       </c>
       <c r="F92" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3334,16 +3467,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D93" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="E93" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="F93" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3351,19 +3484,19 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C94" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="D94" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="E94" t="s">
-        <v>390</v>
+        <v>421</v>
       </c>
       <c r="F94" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3371,19 +3504,19 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C95" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="D95" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="E95" t="s">
-        <v>391</v>
+        <v>422</v>
       </c>
       <c r="F95" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3391,16 +3524,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D96" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="E96" t="s">
-        <v>392</v>
+        <v>423</v>
       </c>
       <c r="F96" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3408,7 +3541,7 @@
         <v>99</v>
       </c>
       <c r="F97" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3416,16 +3549,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D98" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="E98" t="s">
-        <v>393</v>
+        <v>424</v>
       </c>
       <c r="F98" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3433,19 +3566,199 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D99" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="E99" t="s">
-        <v>394</v>
+        <v>425</v>
       </c>
       <c r="F99" t="s">
-        <v>395</v>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>176</v>
+      </c>
+      <c r="D100" t="s">
+        <v>322</v>
+      </c>
+      <c r="E100" t="s">
+        <v>426</v>
+      </c>
+      <c r="F100" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" t="s">
+        <v>227</v>
+      </c>
+      <c r="D101" t="s">
+        <v>323</v>
+      </c>
+      <c r="E101" t="s">
+        <v>427</v>
+      </c>
+      <c r="F101" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>177</v>
+      </c>
+      <c r="C102" t="s">
+        <v>228</v>
+      </c>
+      <c r="D102" t="s">
+        <v>324</v>
+      </c>
+      <c r="E102" t="s">
+        <v>428</v>
+      </c>
+      <c r="F102" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>159</v>
+      </c>
+      <c r="C103" t="s">
+        <v>229</v>
+      </c>
+      <c r="D103" t="s">
+        <v>325</v>
+      </c>
+      <c r="E103" t="s">
+        <v>429</v>
+      </c>
+      <c r="F103" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="s">
+        <v>178</v>
+      </c>
+      <c r="C104" t="s">
+        <v>230</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E104" t="s">
+        <v>430</v>
+      </c>
+      <c r="F104" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="s">
+        <v>143</v>
+      </c>
+      <c r="C105" t="s">
+        <v>231</v>
+      </c>
+      <c r="D105" t="s">
+        <v>327</v>
+      </c>
+      <c r="E105" t="s">
+        <v>431</v>
+      </c>
+      <c r="F105" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="s">
+        <v>136</v>
+      </c>
+      <c r="C106" t="s">
+        <v>232</v>
+      </c>
+      <c r="D106" t="s">
+        <v>328</v>
+      </c>
+      <c r="E106" t="s">
+        <v>432</v>
+      </c>
+      <c r="F106" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="s">
+        <v>179</v>
+      </c>
+      <c r="C107" t="s">
+        <v>233</v>
+      </c>
+      <c r="D107" t="s">
+        <v>329</v>
+      </c>
+      <c r="E107" t="s">
+        <v>351</v>
+      </c>
+      <c r="F107" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="s">
+        <v>180</v>
+      </c>
+      <c r="C108" t="s">
+        <v>234</v>
+      </c>
+      <c r="D108" t="s">
+        <v>330</v>
+      </c>
+      <c r="E108" t="s">
+        <v>433</v>
+      </c>
+      <c r="F108" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D104" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed json errors and lisym upload
</commit_message>
<xml_diff>
--- a/results/publications.xlsx
+++ b/results/publications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="528">
   <si>
     <t>title</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Hepatic Smad7-overexpression causes severe iron overload in the mouse.</t>
   </si>
   <si>
-    <t>Systemic regulation of bilirubin homeostasis: Potential benefits of hyperbilirubinemia.</t>
-  </si>
-  <si>
     <t>Pharmacokinetics and pharmacodynamics of thiopurines in an in vitro model of human hepatocytes: Insights from an innovative mass spectrometry assay.</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t>Model Based Targeting of IL-6-Induced Inflammatory Responses in Cultured Primary Hepatocytes to Improve Application of the JAK Inhibitor Ruxolitinib.</t>
-  </si>
-  <si>
-    <t>Resolving the Combinatorial Complexity of Smad Protein Complex Formation and Its Link to Gene Expression.</t>
   </si>
   <si>
     <t>Bio-degradable highly fluorescent conjugated polymer nanoparticles for bio-medical imaging applications</t>
@@ -351,6 +345,63 @@
     <t>The fruit fly Drosophila melanogaster as an innovative preclinical ADME model for solute carrier membrane transporters, with consequences for pharmacology and drug therapy.</t>
   </si>
   <si>
+    <t>Liquid-crystal organization of liver tissue</t>
+  </si>
+  <si>
+    <t>Tomoelastography for the Evaluation of Pediatric Nonalcoholic Fatty Liver Disease</t>
+  </si>
+  <si>
+    <t>US Time-Harmonic Elastography: Detection of Liver Fibrosis in                     Adolescents with Extreme Obesity with Nonalcoholic Fatty Liver                     Disease</t>
+  </si>
+  <si>
+    <t>Genetic determinants of steatosis and fibrosis progression in pediatric non-alcoholic fatty liver disease.</t>
+  </si>
+  <si>
+    <t>Specifications of Standards in Systems and Synthetic Biology: Status and Developments in 2017.</t>
+  </si>
+  <si>
+    <t>Harmonizing semantic annotations for computational models in biology.</t>
+  </si>
+  <si>
+    <t>Data Formats for Systems Biology and Quantitative Modeling</t>
+  </si>
+  <si>
+    <t>A multiscale modelling approach to assess the impact of metabolic zonation and microperfusion on the hepatic carbohydrate metabolism.</t>
+  </si>
+  <si>
+    <t>HEPATOKIN1 is a biochemistry-based model of liver metabolism for applications in medicine and pharmacology.</t>
+  </si>
+  <si>
+    <t>Possible neurotoxicity of the anesthetic propofol: evidence for the inhibition of complex II of the respiratory chain in area CA3 of rat hippocampal slices.</t>
+  </si>
+  <si>
+    <t>Genetic variants in PNPLA3 and TM6SF2 predispose to the development of hepatocellular carcinoma in individuals with alcohol-related cirrhosis</t>
+  </si>
+  <si>
+    <t>Model-based identification of TNFalpha-induced IKKbeta-mediated and IkappaBalpha-mediated regulation of NFkappaB signal transduction as a tool to quantify the impact of drug-induced liver injury compounds.</t>
+  </si>
+  <si>
+    <t>Resolving the Combinatorial Complexity of Smad Protein Complex Formation and Its Link to Gene Expression.</t>
+  </si>
+  <si>
+    <t>Histologic improvement of NAFLD in patients with obesity after bariatric surgery based on standardized NAS (NAFLD activity score).</t>
+  </si>
+  <si>
+    <t>Whither systems medicine?</t>
+  </si>
+  <si>
+    <t>3D visualization of the biliary tree by X-ray phase-contrast computed tomography</t>
+  </si>
+  <si>
+    <t>Single cell polarity in liquid phase facilitates tumour metastasis.</t>
+  </si>
+  <si>
+    <t>The ascending pathophysiology of cholestatic liver disease.</t>
+  </si>
+  <si>
+    <t>Systemic regulation of bilirubin homeostasis: Potential benefits of hyperbilirubinemia</t>
+  </si>
+  <si>
     <t>J Integr Bioinform</t>
   </si>
   <si>
@@ -444,15 +495,15 @@
     <t>Anal Chem</t>
   </si>
   <si>
+    <t>Nat Commun</t>
+  </si>
+  <si>
+    <t>2017 Winter Simulation Conference (WSC)</t>
+  </si>
+  <si>
     <t>Cell Syst</t>
   </si>
   <si>
-    <t>Nat Commun</t>
-  </si>
-  <si>
-    <t>2017 Winter Simulation Conference (WSC)</t>
-  </si>
-  <si>
     <t>Cell Death Dis</t>
   </si>
   <si>
@@ -561,6 +612,30 @@
     <t>Drug Discov Today</t>
   </si>
   <si>
+    <t>Investigative Radiology</t>
+  </si>
+  <si>
+    <t>Radiology</t>
+  </si>
+  <si>
+    <t>Liver Int</t>
+  </si>
+  <si>
+    <t>Brief Bioinform</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Bioinformatics and Computational Biology</t>
+  </si>
+  <si>
+    <t>Am J Gastroenterol</t>
+  </si>
+  <si>
+    <t>Surg Obes Relat Dis</t>
+  </si>
+  <si>
+    <t>Exp Mol Med</t>
+  </si>
+  <si>
     <t>2017-02-12</t>
   </si>
   <si>
@@ -723,6 +798,54 @@
     <t>2018-06-12</t>
   </si>
   <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2018-07-01</t>
+  </si>
+  <si>
+    <t>2018-03-30</t>
+  </si>
+  <si>
+    <t>2018-01-22</t>
+  </si>
+  <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
+    <t>2018-02-16</t>
+  </si>
+  <si>
+    <t>2018-06-21</t>
+  </si>
+  <si>
+    <t>2018-08-26</t>
+  </si>
+  <si>
+    <t>2018-10-01</t>
+  </si>
+  <si>
+    <t>2018-06-15</t>
+  </si>
+  <si>
+    <t>2018-02-19</t>
+  </si>
+  <si>
+    <t>2018-08-28</t>
+  </si>
+  <si>
+    <t>2018-03-03</t>
+  </si>
+  <si>
+    <t>2018-03-02</t>
+  </si>
+  <si>
+    <t>2017-02-17</t>
+  </si>
+  <si>
+    <t>2018-04-01</t>
+  </si>
+  <si>
     <t>J Integr Bioinform. 2016 Dec 18;13(3):289. doi: 10.2390/biecoll-jib-2016-289.</t>
   </si>
   <si>
@@ -825,9 +948,6 @@
     <t>Blood. 2017 Dec 13. pii: blood-2017-07-796797. doi: 10.1182/blood-2017-07-796797.</t>
   </si>
   <si>
-    <t>Hepatology. 2017 Oct 23. doi: 10.1002/hep.29599.</t>
-  </si>
-  <si>
     <t>Chem Biol Interact. 2017 Sep 25;275:189-195. doi: 10.1016/j.cbi.2017.08.009. Epub 2017 Aug 12.</t>
   </si>
   <si>
@@ -855,9 +975,6 @@
     <t>Front Physiol. 2017 Oct 9;8:775. doi: 10.3389/fphys.2017.00775. eCollection 2017.</t>
   </si>
   <si>
-    <t>Cell Syst. 2017 Dec 13. pii: S2405-4712(17)30538-0. doi: 10.1016/j.cels.2017.11.010.</t>
-  </si>
-  <si>
     <t>Nat Commun 8(1) : 2</t>
   </si>
   <si>
@@ -1011,6 +1128,63 @@
     <t>Drug Discov Today. 2018 Oct;23(10):1746-1760. doi: 10.1016/j.drudis.2018.06.002.  Epub 2018 Jun 8.</t>
   </si>
   <si>
+    <t xml:space="preserve">Liquid-crystal organization of liver tissue </t>
+  </si>
+  <si>
+    <t>Investigative Radiology  : 1</t>
+  </si>
+  <si>
+    <t>Radiology 288(1) : 99</t>
+  </si>
+  <si>
+    <t>Liver Int. 2018 Nov 16. doi: 10.1111/liv.14006.</t>
+  </si>
+  <si>
+    <t>J Integr Bioinform. 2018 Mar 29;15(1). pii: /j/jib.ahead-of-print/jib-2018-0013/jib-2018-0013.xml. doi: 10.1515/jib-2018-0013.</t>
+  </si>
+  <si>
+    <t>Brief Bioinform. 2018 Nov 21. pii: 5164345. doi: 10.1093/bib/bby087.</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Bioinformatics and Computational Biology  : 884</t>
+  </si>
+  <si>
+    <t>PLoS Comput Biol. 2018 Feb 15;14(2):e1006005. doi: 10.1371/journal.pcbi.1006005.  eCollection 2018 Feb.</t>
+  </si>
+  <si>
+    <t>Nat Commun. 2018 Jun 19;9(1):2386. doi: 10.1038/s41467-018-04720-9.</t>
+  </si>
+  <si>
+    <t>Arch Toxicol. 2018 Oct;92(10):3191-3205. doi: 10.1007/s00204-018-2295-8. Epub 2018 Aug 24.</t>
+  </si>
+  <si>
+    <t>Am J Gastroenterol 113(10) : 1475</t>
+  </si>
+  <si>
+    <t>NPJ Syst Biol Appl. 2018 Jun 11;4:23. doi: 10.1038/s41540-018-0058-z. eCollection 2018.</t>
+  </si>
+  <si>
+    <t>Cell Syst. 2018 Jan 24;6(1):75-89.e11. doi: 10.1016/j.cels.2017.11.010. Epub 2017 Dec 13.</t>
+  </si>
+  <si>
+    <t>Surg Obes Relat Dis. 2018 Oct;14(10):1607-1616. doi: 10.1016/j.soard.2018.07.012. Epub 2018 Jul 24.</t>
+  </si>
+  <si>
+    <t>Exp Mol Med. 2018 Mar 2;50(3):e453. doi: 10.1038/emm.2017.290.</t>
+  </si>
+  <si>
+    <t>Arch Toxicol 92(12) : 3601</t>
+  </si>
+  <si>
+    <t>Nat Commun. 2018 Feb 28;9(1):887. doi: 10.1038/s41467-018-03139-6.</t>
+  </si>
+  <si>
+    <t>Hepatology. 2017 Feb;65(2):722-738. doi: 10.1002/hep.28965.</t>
+  </si>
+  <si>
+    <t>Hepatology 67(4) : 1609</t>
+  </si>
+  <si>
     <t>['F. Schreiber', 'G. D. Bader', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'N. Le Novere', 'C. Myers', 'D. Nickerson', 'B. Sommer', 'D. Walthemath']</t>
   </si>
   <si>
@@ -1119,9 +1293,6 @@
     <t>['D. Lai', 'F. Teng', 'Seddik Hammad', 'Julia Werle', 'T. Maas', 'A. Teufel', 'M. U. Muckenthaler', 'Steven Dooley', 'M. Vujic Spasic']</t>
   </si>
   <si>
-    <t>['R. Fujiwara', 'M. Haag', 'E. Schaeffeler', 'A. T. Nies', 'U. M. Zanger', 'Matthias Schwab']</t>
-  </si>
-  <si>
     <t>['M. Pelin', 'E. Genova', 'L. Fusco', 'M. Marisat', 'Ute Hofmann', 'D. Favretto', 'M. Lucafo', 'A. Taddio', 'S. Martelossi', 'A. Ventura', 'G. Stocco', 'Matthias Schwab', 'G. Decorti']</t>
   </si>
   <si>
@@ -1149,175 +1320,232 @@
     <t>['S. Sobotta', 'A. Raue', 'X. Huang', 'J. Vanlier', 'A. Junger', 'S. Bohl', 'U. Albrecht', 'M. J. Hahnel', 'S. Wolf', 'N. S. Mueller', "Lorenza D'Alessandro", 'S. Mueller-Bohl', 'M. E. Boehm', 'P. Lucarelli', 'S. Bonefas', 'G. Damm', 'D. Seehofer', 'W. D. Lehmann', 'S. Rose-John', 'F. van der Hoeven', 'N. Gretz', 'F. J. Theis', 'Christian Ehlting', 'Johannes Bode', 'J. Timmer', 'M. Schilling', 'U. Klingmuller']</t>
   </si>
   <si>
+    <t>['Tatjana Repenko', 'Anne Rix', 'Simon Ludwanowski', 'Dennis Go', 'Fabian Kiessling', 'Wiltrud Lederle', 'Alexander J. C. Kuehne']</t>
+  </si>
+  <si>
+    <t>['Chris J. Myers', 'Gary Bader', 'Padraig Gleeson', 'Martin Golebiewski', 'Michael Hucka', 'Nicolas Le Novere', 'David P. Nickerson', 'Falk Schreiber', 'Dagmar Waltemath']</t>
+  </si>
+  <si>
+    <t>['K. Meyer', 'O. Ostrenko', 'G. Bourantas', 'H. Morales-Navarrete', 'N. Porat-Shliom', 'F. Segovia-Miranda', 'H. Nonaka', 'A. Ghaemi', 'J. M. Verbavatz', 'Lutz Brusch', 'I. Sbalzarini', 'Y. Kalaidzidis', 'R. Weigert', 'M. Zerial']</t>
+  </si>
+  <si>
+    <t>['Haristi Gaitantzi', 'Christoph Meyer', 'Pia Rakoczy', 'Maria Thomas', 'Kristin Wahl', 'Franziska Wandrer', 'Heike Bantel', 'Hamed Alborzinia', 'Stefan Wölfl', 'Sabrina Ehnert', 'Andreas Nüssler', 'Ina Bergheim', 'Loredana Ciuclan', 'Matthias Ebert', 'Katja Breitkopf-Heinlein', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['Joaquim Moreno-Càceres', 'Daniel Caballero-Díaz', 'Zeribe Chike Nwosu', 'Christoph Meyer', 'Judit López-Luque', 'Andrea Malfettone', 'Raquel Lastra', 'Teresa Serrano', 'Emilio Ramos', 'Steven Dooley', 'Isabel Fabregat']</t>
+  </si>
+  <si>
+    <t>['Yaochen Zhang', 'Don-Kyu Kim', 'Yan Lu', 'Yoon Seok Jung', 'Ji-min Lee', 'Young-Hoon Kim', 'Yong Soo Lee', 'Jina Kim', 'Bedair Dewidar', 'Won-IL Jeong', 'In-Kyu Lee', 'Sung Jin Cho', 'Steven Dooley', 'Chul-Ho Lee', 'Xiaoying Li', 'Hueng-Sik Choi']</t>
+  </si>
+  <si>
+    <t>['Rodrigo Rojas-Moraleda', 'Wei Xiong', 'Niels Halama', 'Katja Breitkopf-Heinlein', 'Steven Dooley', 'Luis Salinas', 'Dieter W. Heermann', 'Nektarios A. Valous']</t>
+  </si>
+  <si>
+    <t>['T Feng', 'J Dzieran', 'X Yuan', 'A Dropmann', 'T Maass', 'A Teufel', 'S Marhenke', 'T Gaiser', 'F Rückert', 'I Kleiter', 'S Kanzler', 'M P Ebert', 'A Vogel', 'P ten Dijke', 'Steven Dooley', 'N M Meindl-Beinker']</t>
+  </si>
+  <si>
+    <t>['Zhe Shen', 'Yan Liu', 'Bedair Dewidar', 'Junhao Hu', 'Ogyi Park', 'Teng Feng', 'Chengfu Xu', 'Chaohui Yu', 'Qi Li', 'Christoph Meyer', 'Iryna Ilkavets', 'Alexandra Müller', 'Carolin Stump-Guthier', 'Stefan Munker', 'Roman Liebe', 'Vincent Zimmer', 'Frank Lammert', 'Peter R. Mertens', 'Hai Li', 'Peter ten Dijke', 'Hellmut G. Augustin', 'Jun Li', 'Bin Gao', 'Matthias P. Ebert', 'Steven Dooley', 'Youming Li', 'Hong-Lei Weng']</t>
+  </si>
+  <si>
+    <t>['Simeng Chen', 'Teng Feng', 'Maja Vujić Spasić', 'Sandro Altamura', 'Katja Breitkopf-Heinlein', 'Jutta Altenöder', 'Thomas S. Weiss', 'Steven Dooley', 'Martina U. Muckenthaler']</t>
+  </si>
+  <si>
+    <t>['Anne Dropmann', 'Tatjana Dediulia', 'Katja Breitkopf-Heinlein', 'Hanna Korhonen', 'Michel Janicot', 'Susanne Weber', 'Maria Thomas', 'Albrecht Piiper', 'Esther Bertran', 'Isabel Fabregat', 'Kerstin Abshagen', 'Jochen Hess', 'Peter Angel', 'Cédric Coulouarn', 'Steven Dooley', 'Nadja M. Meindl-Beinker']</t>
+  </si>
+  <si>
+    <t>['P. GONZÁLEZ-AVALOS', 'M. MÜRNSEER', 'J. DEEG', 'A. BACHMANN', 'J. SPATZ', 'Steven Dooley', 'R. EILS', 'E. GLADILIN']</t>
+  </si>
+  <si>
+    <t>['Wolfgang Schmidt-Heck', 'Eva C. Wönne', 'Thomas Hiller', 'Uwe Menzel', 'Dirk Koczan', 'Georg Damm', 'Daniel Seehofer', 'Fanny Knöspel', 'Nora Freyer', 'Reinhard Guthke', 'Steven Dooley', 'Katrin Zeilinger']</t>
+  </si>
+  <si>
+    <t>['Katharina Beuke', 'Frank A. Schildberg', 'Federico Pinna', 'Ute Albrecht', 'Roman Liebe', 'Michaela Bissinger', 'Peter Schirmacher', 'Steven Dooley', 'Johannes Bode', 'Percy A. Knolle', 'Ursula Kummer', 'Kai Breuhahn', 'Sven Sahle']</t>
+  </si>
+  <si>
+    <t>['F. Dittmann', 'H. Tzschatzsch', 'S. Hirsch', 'E. Barnhill', 'J. Braun', 'I. Sack', 'Jing Guo']</t>
+  </si>
+  <si>
+    <t>['F. Dittmann', 'R. Reiter', 'Jing Guo', 'M. Haas', 'P. Asbach', 'T. Fischer', 'J. Braun', 'I. Sack']</t>
+  </si>
+  <si>
+    <t>['S. R. Marticorena Garcia', 'M. Grossmann', 'S. T. Lang', 'H. Tzschatzsch', 'F. Dittmann', 'B. Hamm', 'J. Braun', 'Jing Guo', 'I. Sack']</t>
+  </si>
+  <si>
+    <t>['S. Ipek-Ugay', 'H. Tzschatzsch', 'J. Braun', 'T. Fischer', 'I. Sack']</t>
+  </si>
+  <si>
+    <t>['J. Braun', 'H. Tzschatzsch', 'C. Korting', 'A. Ariza de Schellenberger', 'M. Jenderka', 'T. Driessle', 'M. Ledwig', 'I. Sack']</t>
+  </si>
+  <si>
+    <t>['J. Johanning', 'P. Kroner', 'M. Thomas', 'U. M. Zanger', 'A. Norenberg', 'M. Eichelbaum', 'Matthias Schwab', 'H. Brauch', 'W. Schroth', 'T. E. Murdter']</t>
+  </si>
+  <si>
+    <t>['Tzschaetzsch H, Grossman M, Lang S, Trong M, Schultz M, Guo J, Hamm B, Braun J, Sack I.']</t>
+  </si>
+  <si>
+    <t>['V. Schutzhold', 'J. Hahn', 'K. Tummler', 'E. Klipp']</t>
+  </si>
+  <si>
+    <t>['Josch Pauling', 'E. Klipp']</t>
+  </si>
+  <si>
+    <t>['Marcin Krawczyk', 'Heike Bantel', 'Monika Rau', 'Jörn M Schattenberg', 'Frank Grünhage', 'Anita Pathil', 'Münnever Demir', 'Johannes Kluwe', 'Tobias Boettler', 'Susanne Weber', 'Andreas Geier', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['Malgorzata Jamka', 'Anita Arslanow', 'Annika Bohner', 'Marcin Krawczyk', 'Susanne Weber', 'Frank Grünhage', 'Frank Lammert', 'Caroline S Stokes']</t>
+  </si>
+  <si>
+    <t>['Johannes Eckstein', 'Hergo Holzhütter', 'Nikolaus Berndt']</t>
+  </si>
+  <si>
+    <t>['M. Leist', 'Ahmed Ghallab', 'R. Graepel', 'R. Marchan', 'Reham Hassan', 'S. H. Bennekou', 'A. Limonciel', 'M. Vinken', 'S. Schildknecht', 'T. Waldmann', 'E. Danen', 'B. van Ravenzwaay', 'H. Kamp', 'I. Gardner', 'P. Godoy', 'F. Y. Bois', 'A. Braeuning', 'R. Reif', 'F. Oesch', 'D. Drasdo', 'Stefan Hoehme', 'M. Schwarz', 'T. Hartung', 'T. Braunbeck', 'J. Beltman', 'H. Vrieling', 'F. Sanz', 'A. Forsby', 'D. Gadaleta', 'C. Fisher', 'J. Kelm', 'D. Fluri', 'G. Ecker', 'B. Zdrazil', 'A. Terron', 'P. Jennings', 'B. van der Burg', 'Steven Dooley', 'A. H. Meijer', 'E. Willighagen', 'M. Martens', 'C. Evelo', 'E. Mombelli', 'O. Taboureau', 'A. Mantovani', 'B. Hardy', 'B. Koch', 'S. Escher', 'C. van Thriel', 'C. Cadenas', 'D. Kroese', 'B. van de Water', 'J. G. Hengstler']</t>
+  </si>
+  <si>
+    <t>['Geert Peeters', 'Charlotte Debbaut', 'Wim Laleman', 'Adrian Friebel', 'Diethard Monbaliu', 'Ingrid Vander Elst', 'Jan R. Detrez', 'Tim Vandecasteele', 'Tim Johann', 'Thomas De Schryver', 'Luc Van Hoorebeke', 'Kasper Favere', 'Jonas Verbeke', 'Dirk Drasdo', 'Stefan Hoehme', 'Patrick Segers', 'Pieter Cornillie', 'Winnok H. De Vos']</t>
+  </si>
+  <si>
+    <t>['Stefan Hoehme', 'Francois Bertaux', 'William Weens', 'Bettina Grasl-Kraupp', 'Jan G. Hengstler', 'Dirk Drasdo']</t>
+  </si>
+  <si>
+    <t>['G. Peeters', 'C. Debbaut', 'A. Friebel', 'P. Cornillie', 'W. H. De Vos', 'K. Favere', 'I. Vander Elst', 'T. Vandecasteele', 'T. Johann', 'L. Van Hoorebeke', 'D. Monbaliu', 'D. Drasdo', 'Stefan Hoehme', 'W. Laleman', 'P. Segers']</t>
+  </si>
+  <si>
+    <t>['S. Stengel', 'A. Stallmach', 'K. Richter', 'A. Landrock', 'Jochen Hampe', 'T. Bruns']</t>
+  </si>
+  <si>
+    <t>['E. Patsenker', 'A. Chicca', 'V. Petrucci', 'S. Moghadamrad', 'A. de Gottardi', 'Jochen Hampe', 'J. Gertsch', 'N. Semmo', 'F. Stickel']</t>
+  </si>
+  <si>
+    <t>['F. Stickel', 'C. Datz', 'Jochen Hampe', 'R. Bataller']</t>
+  </si>
+  <si>
+    <t>['S. Wahl', 'A. Drong', 'B. Lehne', 'M. Loh', 'W. R. Scott', 'S. Kunze', 'P. C. Tsai', 'J. S. Ried', 'W. Zhang', 'Y. Yang', 'S. Tan', 'G. Fiorito', 'L. Franke', 'S. Guarrera', 'S. Kasela', 'J. Kriebel', 'R. C. Richmond', 'M. Adamo', 'U. Afzal', 'M. Ala-Korpela', 'B. Albetti', 'O. Ammerpohl', 'J. F. Apperley', 'M. Beekman', 'P. A. Bertazzi', 'S. L. Black', 'C. Blancher', 'M. J. Bonder', 'Mario Brosch', 'M. Carstensen-Kirberg', 'A. J. de Craen', 'S. de Lusignan', 'A. Dehghan', 'M. Elkalaawy', 'K. Fischer', 'O. H. Franco', 'T. R. Gaunt', 'Jochen Hampe', 'M. Hashemi', 'A. Isaacs', 'A. Jenkinson', 'S. Jha', 'N. Kato', 'V. Krogh', 'M. Laffan', 'C. Meisinger', 'T. Meitinger', 'Z. Y. Mok', 'V. Motta', 'H. K. Ng', 'Z. Nikolakopoulou', 'G. Nteliopoulos', 'S. Panico', 'N. Pervjakova', 'H. Prokisch', 'W. Rathmann', 'M. Roden', 'F. Rota', 'M. A. Rozario', 'J. K. Sandling', 'Clemens Schafmayer', 'K. Schramm', 'R. Siebert', 'P. E. Slagboom', 'P. Soininen', 'L. Stolk', 'K. Strauch', 'E. S. Tai', 'L. Tarantini', 'B. Thorand', 'E. F. Tigchelaar', 'R. Tumino', 'A. G. Uitterlinden', 'C. van Duijn', 'J. B. van Meurs', 'P. Vineis', 'A. R. Wickremasinghe', 'C. Wijmenga', 'T. P. Yang', 'W. Yuan', 'A. Zhernakova', 'R. L. Batterham', 'G. D. Smith', 'P. Deloukas', 'B. T. Heijmans', 'C. Herder', 'A. Hofman', 'C. M. Lindgren', 'L. Milani', 'P. van der Harst', 'A. Peters', 'T. Illig', 'C. L. Relton', 'M. Waldenberger', 'M. R. Jarvelin', 'V. Bollati', 'R. Soong', 'T. D. Spector', 'J. Scott', 'M. I. McCarthy', 'P. Elliott', 'J. T. Bell', 'G. Matullo', 'C. Gieger', 'J. S. Kooner', 'H. Grallert', 'J. C. Chambers']</t>
+  </si>
+  <si>
+    <t>['J. Mwinyi', 'A. E. Bostrom', 'C. Pisanu', 'S. K. Murphy', 'W. Erhart', 'Clemens Schafmayer', 'Jochen Hampe', 'C. Moylan', 'H. B. Schioth']</t>
+  </si>
+  <si>
+    <t>['F. Stickel', 'C. Moreno', 'Jochen Hampe', 'M. Y. Morgan']</t>
+  </si>
+  <si>
+    <t>['H. B. Schioth', 'A. Bostrom', 'S. K. Murphy', 'W. Erhart', 'Jochen Hampe', 'C. Moylan', 'J. Mwinyi']</t>
+  </si>
+  <si>
+    <t>['O. M. Will', 'T. Damm', 'G. M. Campbell', 'Witigo Von Schönfels', 'Y. Acil', 'M. Will', 'A. Chalaris-Rissmann', 'M. Ayna', 'C. Drucker', 'C. C. Gluer']</t>
+  </si>
+  <si>
+    <t>['D. Waltemath', 'J. R. Karr', 'F. T. Bergmann', 'V. Chelliah', 'M. Hucka', 'M. Krantz', 'W. Liebermeister', 'P. Mendes', 'C. J. Myers', 'P. Pir', 'B. Alaybeyoglu', 'N. K. Aranganathan', 'K. Baghalian', 'A. T. Bittig', 'P. E. Burke', 'M. Cantarelli', 'Y. H. Chew', 'R. S. Costa', 'J. Cursons', 'T. Czauderna', 'A. P. Goldberg', 'H. F. Gomez', 'J. Hahn', 'T. Hameri', 'D. F. Gardiol', 'D. Kazakiewicz', 'I. Kiselev', 'V. Knight-Schrijver', 'C. Knupfer', 'Matthias König', 'D. Lee', 'A. Lloret-Villas', 'N. Mandrik', 'J. K. Medley', 'B. Moreau', 'H. Naderi-Meshkin', 'S. K. Palaniappan', 'D. Priego-Espinosa', 'M. Scharm', 'M. Sharma', 'K. Smallbone', 'N. J. Stanford', 'J. H. Song', 'T. Theile', 'M. Tokic', 'N. Tomar', 'V. Toure', 'J. Uhlendorf', 'T. M. Varusai', 'L. H. Watanabe', 'F. Wendland', 'M. Wolfien', 'J. T. Yurkovich', 'Y. Zhu', 'A. Zardilis', 'A. Zhukova', 'F. Schreiber']</t>
+  </si>
+  <si>
+    <t>['A. Zeigerer', 'A. Wuttke', 'G. Marsico', 'S. Seifert', 'Y. Kalaidzidis', 'M. Zerial']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad', 'Elisabetta Cavalcanti', 'Julia Werle', 'Maria Lucia Caruso', 'Anne Dropmann', 'Antonia Ignazzi', 'Matthias Philip Ebert', 'Steven Dooley', 'Gianluigi Giannelli']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad', 'Amnah Othman', 'Christoph Meyer', 'Ahmad Telfah', 'Joerg Lambert', 'Bedair Dewidar', 'Julia Werle', 'Zeribe Chike Nwosu', 'Abdo Mahli', 'Christof Dormann', 'Yan Gao', 'Kerry Gould', 'Mei Han', 'Xiaodong Yuan', 'Mikheil Gogiashvili', 'Roland Hergenröder', 'Claus Hellerbrand', 'Maria Thomas', 'Matthias Philip Ebert', 'Salah Amasheh', 'Jan Hengstler', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['Oskar Knittelfelder', 'S. Traikov', 'Olga Vvedenskaya', 'A. Schuhmann', 'S. Segeletz', 'A. Shevchenko', 'A. Shevchenko']</t>
+  </si>
+  <si>
+    <t>['Selahaddin Sezgin', 'Reham Hassan', 'Sebastian Zühlke', 'Lars Kuepfer', 'Jan Hengstler', 'Michael Spiteller', 'Ahmed Ghallab']</t>
+  </si>
+  <si>
+    <t>['Ahmed Ghallab', 'Ute Hofmann', 'Selahaddin Sezgin', 'Nachiket Vartak', 'Reham Hassan', 'Ayham Zaza', 'Patricio Godoy', 'Kai Markus Schneider', 'Georgia Guenther', 'Yasser A Ahmed', 'Aya A Abbas', 'Verena Keitel', 'Lars Kuepfer', 'Steven Dooley', 'Frank Lammert', 'Christian Trautwein', 'Michael Spiteller', 'Dirk Drasdo', 'Alan F Hofmann', 'Peter Jansen', 'Jan Hengstler', 'Raymond Reif']</t>
+  </si>
+  <si>
+    <t>['A. Schmoldt', 'H. F. Benthe', 'G. Haberland']</t>
+  </si>
+  <si>
+    <t>['André Homeyer', 'Seddik Hammad', 'Lars Ole Schwen', 'U. Dahmen', 'H. Hofener', 'Y. Gao', 'Steven Dooley', 'Andrea Schenk']</t>
+  </si>
+  <si>
+    <t>['D. Waltemath', 'F. T. Bergmann', 'C. Chaouiya', 'T. Czauderna', 'P. Gleeson', 'C. Goble', 'Martin Golebiewski', 'M. Hucka', 'N. Juty', 'O. Krebs', 'N. Le Novere', 'H. Mi', 'I. I. Moraru', 'C. J. Myers', 'D. Nickerson', 'B. G. Olivier', 'N. Rodriguez', 'F. Schreiber', 'L. Smith', 'F. Zhang', 'E. Bonnet']</t>
+  </si>
+  <si>
+    <t>['Ersin Karatayli', 'R. A. Hall', 'Susanne Weber', 'Steven Dooley', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['K. Abshagen', 'B. Degenhardt', 'M. Liebig', 'A. Wendt', 'B. Genz', 'U. Schaeper', 'M. Stumvoll', 'Ute Hofmann', 'M. Frank', 'B. Vollmar', 'N. Kloting']</t>
+  </si>
+  <si>
+    <t>['Matthias Reichert', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['M. Jamka', 'A. Arslanow', 'A. Bohner', 'M. Krawczyk', 'Susanne Weber', 'F. Grunhage', 'Frank Lammert', 'C. S. Stokes']</t>
+  </si>
+  <si>
+    <t>['Olga Vvedenskaya', 'Yuting Wang', 'Jacobo Miranda Ackerman', 'Oskar Knittelfelder', 'Andrej Shevchenko']</t>
+  </si>
+  <si>
+    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Thomas Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
+  </si>
+  <si>
+    <t>['Christiane Rennert', 'Sebastian Vlaic', 'Eugenia Marbach-Breitrück', 'Carlo Thiel', 'Susanne Sales', 'Andrej Shevchenko', 'Rolf Gebhardt', 'Madlen Matz-Soja']</t>
+  </si>
+  <si>
+    <t>['Y. Wang', 'B. Moussian', 'E. Schaeffeler', 'Matthias Schwab', 'A. T. Nies']</t>
+  </si>
+  <si>
+    <t>['Hernan Morales-Navarrete', 'Hidenori Nonaka', 'Andre Scholich', 'Fabian Segovia Miranda', 'Walter de Back', 'Kirstin Meyer', 'Roman L Bogorad', 'Victor Koteliansky', 'Lutz Brusch', 'Yannis Kalaidzidis', 'Frank Julicher', 'Benjamin M. Friedrich', 'Marino Zerial']</t>
+  </si>
+  <si>
+    <t>['Christian Hudert', 'Heiko Tzschätzsch', 'Birgit Rudolph', 'Hendrik Bläker', 'Christoph Loddenkemper', 'Hans-Peter Müller', 'Stephan Henning', 'Philip Bufler', 'Bernd Hamm', 'Jürgen Braun', 'Hergo Holzhütter', 'Susanna Wiegand', 'Ingolf Sack', 'Jing Guo']</t>
+  </si>
+  <si>
+    <t>['Christian Hudert', 'Heiko Tzschätzsch', 'Jing Guo', 'Birgit Rudolph', 'Hendrik Bläker', 'Christoph Loddenkemper', 'Werner Luck', 'Hans-Peter Müller', 'Daniel C. Baumgart', 'Bernd Hamm', 'Jürgen Braun', 'Hergo Holzhütter', 'Susanna Wiegand', 'Ingolf Sack']</t>
+  </si>
+  <si>
+    <t>['Christian Hudert', 'S. Selinski', 'B. Rudolph', 'H. Blaker', 'C. Loddenkemper', 'R. Thielhorn', 'N. Berndt', 'K. Golka', 'C. Cadenas', 'J. Reinders', 'S. Henning', 'P. Bufler', 'P. L. M. Jansen', 'Hergo Holzhütter', 'David Meierhofer', 'J. G. Hengstler', 'S. Wiegand']</t>
+  </si>
+  <si>
+    <t>['F. Schreiber', 'G. D. Bader', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'S. M. Keating', 'N. L. Novere', 'C. Myers', 'D. Nickerson', 'B. Sommer', 'D. Waltemath']</t>
+  </si>
+  <si>
+    <t>['M. L. Neal', 'Matthias König', 'D. Nickerson', 'G. Misirli', 'R. Kalbasi', 'A. Drager', 'K. Atalag', 'V. Chelliah', 'M. T. Cooling', 'D. L. Cook', 'S. Crook', 'M. de Alba', 'S. H. Friedman', 'A. Garny', 'J. H. Gennari', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'N. Juty', 'C. Myers', 'B. G. Olivier', 'H. M. Sauro', 'M. Scharm', 'J. L. Snoep', 'V. Toure', 'A. Wipat', 'O. Wolkenhauer', 'D. Waltemath']</t>
+  </si>
+  <si>
+    <t>['Martin Golebiewski']</t>
+  </si>
+  <si>
+    <t>['N. Berndt', 'M. S. Horger', 'Sascha Bulik', 'Hergo Holzhütter']</t>
+  </si>
+  <si>
+    <t>['N. Berndt', 'Sascha Bulik', 'I. Wallach', 'T. Wunsch', 'Matthias König', 'Martin Stockmann', 'David Meierhofer', 'Hergo Holzhütter']</t>
+  </si>
+  <si>
+    <t>['N. Berndt', 'J. Rosner', 'R. U. Haq', 'O. Kann', 'R. Kovacs', 'Hergo Holzhütter', 'C. Spies', 'A. Liotta']</t>
+  </si>
+  <si>
+    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo Von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Ann-Kristin Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
+  </si>
+  <si>
+    <t>['Felix Stickel', 'Stephan Buch', 'Hans Dieter Nischalke', 'Karl Heinz Weiss', 'Daniel Gotthardt', 'Janett Fischer', 'Jonas Rosendahl', 'Astrid Marot', 'Mona Elamly', 'Markus Casper', 'Frank Lammert', 'Andrew McQuillin', 'Steffen Zopf', 'Ulrich Spengler', 'Silke Marhenke', 'Martha M. Kirstein', 'Arndt Vogel', 'Florian Eyer', 'Johann von Felden', 'Henning Wege', 'Thorsten Buch', 'Clemens Schafmayer', 'Felix Braun', 'Pierre Deltenre', 'Thomas Berg', 'Marsha Y. Morgan', 'Jochen Hampe']</t>
+  </si>
+  <si>
+    <t>['A. Oppelt', 'D. Kaschek', 'S. Huppelschoten', 'R. Sison-Young', 'F. Zhang', 'M. Buck-Wiese', 'F. Herrmann', 'S. Malkusch', 'C. L. Kruger', 'M. Meub', 'B. Merkt', 'L. Zimmermann', 'A. Schofield', 'R. P. Jones', 'H. Malik', 'M. Schilling', 'M. Heilemann', 'B. van de Water', 'C. E. Goldring', 'B. K. Park', 'J. Timmer', 'U. Klingmuller']</t>
+  </si>
+  <si>
     <t>['P. Lucarelli', 'M. Schilling', 'C. Kreutz', 'A. Vlasov', 'M. E. Boehm', 'N. Iwamoto', 'B. Steiert', 'S. Lattermann', 'M. Wasch', 'M. Stepath', 'M. S. Matter', 'M. Heikenwalder', 'Professor Dr.  Med. Katrin Hoffmann', 'D. Deharde', 'G. Damm', 'D. Seehofer', 'M. Muciek', 'N. Gretz', 'W. D. Lehmann', 'J. Timmer', 'U. Klingmuller']</t>
   </si>
   <si>
-    <t>['Tatjana Repenko', 'Anne Rix', 'Simon Ludwanowski', 'Dennis Go', 'Fabian Kiessling', 'Wiltrud Lederle', 'Alexander J. C. Kuehne']</t>
-  </si>
-  <si>
-    <t>['Chris J. Myers', 'Gary Bader', 'Padraig Gleeson', 'Martin Golebiewski', 'Michael Hucka', 'Nicolas Le Novere', 'David P. Nickerson', 'Falk Schreiber', 'Dagmar Waltemath']</t>
-  </si>
-  <si>
-    <t>['K. Meyer', 'O. Ostrenko', 'G. Bourantas', 'H. Morales-Navarrete', 'N. Porat-Shliom', 'F. Segovia-Miranda', 'H. Nonaka', 'A. Ghaemi', 'J. M. Verbavatz', 'Lutz Brusch', 'I. Sbalzarini', 'Y. Kalaidzidis', 'R. Weigert', 'M. Zerial']</t>
-  </si>
-  <si>
-    <t>['Haristi Gaitantzi', 'Christoph Meyer', 'Pia Rakoczy', 'Maria Thomas', 'Kristin Wahl', 'Franziska Wandrer', 'Heike Bantel', 'Hamed Alborzinia', 'Stefan Wölfl', 'Sabrina Ehnert', 'Andreas Nüssler', 'Ina Bergheim', 'Loredana Ciuclan', 'Matthias Ebert', 'Katja Breitkopf-Heinlein', 'Steven Dooley']</t>
-  </si>
-  <si>
-    <t>['Joaquim Moreno-Càceres', 'Daniel Caballero-Díaz', 'Zeribe Chike Nwosu', 'Christoph Meyer', 'Judit López-Luque', 'Andrea Malfettone', 'Raquel Lastra', 'Teresa Serrano', 'Emilio Ramos', 'Steven Dooley', 'Isabel Fabregat']</t>
-  </si>
-  <si>
-    <t>['Yaochen Zhang', 'Don-Kyu Kim', 'Yan Lu', 'Yoon Seok Jung', 'Ji-min Lee', 'Young-Hoon Kim', 'Yong Soo Lee', 'Jina Kim', 'Bedair Dewidar', 'Won-IL Jeong', 'In-Kyu Lee', 'Sung Jin Cho', 'Steven Dooley', 'Chul-Ho Lee', 'Xiaoying Li', 'Hueng-Sik Choi']</t>
-  </si>
-  <si>
-    <t>['Rodrigo Rojas-Moraleda', 'Wei Xiong', 'Niels Halama', 'Katja Breitkopf-Heinlein', 'Steven Dooley', 'Luis Salinas', 'Dieter W. Heermann', 'Nektarios A. Valous']</t>
-  </si>
-  <si>
-    <t>['T Feng', 'J Dzieran', 'X Yuan', 'A Dropmann', 'T Maass', 'A Teufel', 'S Marhenke', 'T Gaiser', 'F Rückert', 'I Kleiter', 'S Kanzler', 'M P Ebert', 'A Vogel', 'P ten Dijke', 'Steven Dooley', 'N M Meindl-Beinker']</t>
-  </si>
-  <si>
-    <t>['Zhe Shen', 'Yan Liu', 'Bedair Dewidar', 'Junhao Hu', 'Ogyi Park', 'Teng Feng', 'Chengfu Xu', 'Chaohui Yu', 'Qi Li', 'Christoph Meyer', 'Iryna Ilkavets', 'Alexandra Müller', 'Carolin Stump-Guthier', 'Stefan Munker', 'Roman Liebe', 'Vincent Zimmer', 'Frank Lammert', 'Peter R. Mertens', 'Hai Li', 'Peter ten Dijke', 'Hellmut G. Augustin', 'Jun Li', 'Bin Gao', 'Matthias P. Ebert', 'Steven Dooley', 'Youming Li', 'Hong-Lei Weng']</t>
-  </si>
-  <si>
-    <t>['Simeng Chen', 'Teng Feng', 'Maja Vujić Spasić', 'Sandro Altamura', 'Katja Breitkopf-Heinlein', 'Jutta Altenöder', 'Thomas S. Weiss', 'Steven Dooley', 'Martina U. Muckenthaler']</t>
-  </si>
-  <si>
-    <t>['Anne Dropmann', 'Tatjana Dediulia', 'Katja Breitkopf-Heinlein', 'Hanna Korhonen', 'Michel Janicot', 'Susanne Weber', 'Maria Thomas', 'Albrecht Piiper', 'Esther Bertran', 'Isabel Fabregat', 'Kerstin Abshagen', 'Jochen Hess', 'Peter Angel', 'Cédric Coulouarn', 'Steven Dooley', 'Nadja M. Meindl-Beinker']</t>
-  </si>
-  <si>
-    <t>['P. GONZÁLEZ-AVALOS', 'M. MÜRNSEER', 'J. DEEG', 'A. BACHMANN', 'J. SPATZ', 'Steven Dooley', 'R. EILS', 'E. GLADILIN']</t>
-  </si>
-  <si>
-    <t>['Wolfgang Schmidt-Heck', 'Eva C. Wönne', 'Thomas Hiller', 'Uwe Menzel', 'Dirk Koczan', 'Georg Damm', 'Daniel Seehofer', 'Fanny Knöspel', 'Nora Freyer', 'Reinhard Guthke', 'Steven Dooley', 'Katrin Zeilinger']</t>
-  </si>
-  <si>
-    <t>['Katharina Beuke', 'Frank A. Schildberg', 'Federico Pinna', 'Ute Albrecht', 'Roman Liebe', 'Michaela Bissinger', 'Peter Schirmacher', 'Steven Dooley', 'Johannes Bode', 'Percy A. Knolle', 'Ursula Kummer', 'Kai Breuhahn', 'Sven Sahle']</t>
-  </si>
-  <si>
-    <t>['F. Dittmann', 'H. Tzschatzsch', 'S. Hirsch', 'E. Barnhill', 'J. Braun', 'I. Sack', 'Jing Guo']</t>
-  </si>
-  <si>
-    <t>['F. Dittmann', 'R. Reiter', 'Jing Guo', 'M. Haas', 'P. Asbach', 'T. Fischer', 'J. Braun', 'I. Sack']</t>
-  </si>
-  <si>
-    <t>['S. R. Marticorena Garcia', 'M. Grossmann', 'S. T. Lang', 'H. Tzschatzsch', 'F. Dittmann', 'B. Hamm', 'J. Braun', 'Jing Guo', 'I. Sack']</t>
-  </si>
-  <si>
-    <t>['S. Ipek-Ugay', 'H. Tzschatzsch', 'J. Braun', 'T. Fischer', 'I. Sack']</t>
-  </si>
-  <si>
-    <t>['J. Braun', 'H. Tzschatzsch', 'C. Korting', 'A. Ariza de Schellenberger', 'M. Jenderka', 'T. Driessle', 'M. Ledwig', 'I. Sack']</t>
-  </si>
-  <si>
-    <t>['J. Johanning', 'P. Kroner', 'M. Thomas', 'U. M. Zanger', 'A. Norenberg', 'M. Eichelbaum', 'Matthias Schwab', 'H. Brauch', 'W. Schroth', 'T. E. Murdter']</t>
-  </si>
-  <si>
-    <t>['Tzschaetzsch H, Grossman M, Lang S, Trong M, Schultz M, Guo J, Hamm B, Braun J, Sack I.']</t>
-  </si>
-  <si>
-    <t>['V. Schutzhold', 'J. Hahn', 'K. Tummler', 'E. Klipp']</t>
-  </si>
-  <si>
-    <t>['Josch Pauling', 'E. Klipp']</t>
-  </si>
-  <si>
-    <t>['Marcin Krawczyk', 'Heike Bantel', 'Monika Rau', 'Jörn M Schattenberg', 'Frank Grünhage', 'Anita Pathil', 'Münnever Demir', 'Johannes Kluwe', 'Tobias Boettler', 'Susanne Weber', 'Andreas Geier', 'Frank Lammert']</t>
-  </si>
-  <si>
-    <t>['Malgorzata Jamka', 'Anita Arslanow', 'Annika Bohner', 'Marcin Krawczyk', 'Susanne Weber', 'Frank Grünhage', 'Frank Lammert', 'Caroline S Stokes']</t>
-  </si>
-  <si>
-    <t>['Johannes Eckstein', 'Hergo Holzhütter', 'Nikolaus Berndt']</t>
-  </si>
-  <si>
-    <t>['M. Leist', 'Ahmed Ghallab', 'R. Graepel', 'R. Marchan', 'Reham Hassan', 'S. H. Bennekou', 'A. Limonciel', 'M. Vinken', 'S. Schildknecht', 'T. Waldmann', 'E. Danen', 'B. van Ravenzwaay', 'H. Kamp', 'I. Gardner', 'P. Godoy', 'F. Y. Bois', 'A. Braeuning', 'R. Reif', 'F. Oesch', 'D. Drasdo', 'Stefan Hoehme', 'M. Schwarz', 'T. Hartung', 'T. Braunbeck', 'J. Beltman', 'H. Vrieling', 'F. Sanz', 'A. Forsby', 'D. Gadaleta', 'C. Fisher', 'J. Kelm', 'D. Fluri', 'G. Ecker', 'B. Zdrazil', 'A. Terron', 'P. Jennings', 'B. van der Burg', 'Steven Dooley', 'A. H. Meijer', 'E. Willighagen', 'M. Martens', 'C. Evelo', 'E. Mombelli', 'O. Taboureau', 'A. Mantovani', 'B. Hardy', 'B. Koch', 'S. Escher', 'C. van Thriel', 'C. Cadenas', 'D. Kroese', 'B. van de Water', 'J. G. Hengstler']</t>
-  </si>
-  <si>
-    <t>['Geert Peeters', 'Charlotte Debbaut', 'Wim Laleman', 'Adrian Friebel', 'Diethard Monbaliu', 'Ingrid Vander Elst', 'Jan R. Detrez', 'Tim Vandecasteele', 'Tim Johann', 'Thomas De Schryver', 'Luc Van Hoorebeke', 'Kasper Favere', 'Jonas Verbeke', 'Dirk Drasdo', 'Stefan Hoehme', 'Patrick Segers', 'Pieter Cornillie', 'Winnok H. De Vos']</t>
-  </si>
-  <si>
-    <t>['Stefan Hoehme', 'Francois Bertaux', 'William Weens', 'Bettina Grasl-Kraupp', 'Jan G. Hengstler', 'Dirk Drasdo']</t>
-  </si>
-  <si>
-    <t>['G. Peeters', 'C. Debbaut', 'A. Friebel', 'P. Cornillie', 'W. H. De Vos', 'K. Favere', 'I. Vander Elst', 'T. Vandecasteele', 'T. Johann', 'L. Van Hoorebeke', 'D. Monbaliu', 'D. Drasdo', 'Stefan Hoehme', 'W. Laleman', 'P. Segers']</t>
-  </si>
-  <si>
-    <t>['S. Stengel', 'A. Stallmach', 'K. Richter', 'A. Landrock', 'Jochen Hampe', 'T. Bruns']</t>
-  </si>
-  <si>
-    <t>['E. Patsenker', 'A. Chicca', 'V. Petrucci', 'S. Moghadamrad', 'A. de Gottardi', 'Jochen Hampe', 'J. Gertsch', 'N. Semmo', 'F. Stickel']</t>
-  </si>
-  <si>
-    <t>['F. Stickel', 'C. Datz', 'Jochen Hampe', 'R. Bataller']</t>
-  </si>
-  <si>
-    <t>['S. Wahl', 'A. Drong', 'B. Lehne', 'M. Loh', 'W. R. Scott', 'S. Kunze', 'P. C. Tsai', 'J. S. Ried', 'W. Zhang', 'Y. Yang', 'S. Tan', 'G. Fiorito', 'L. Franke', 'S. Guarrera', 'S. Kasela', 'J. Kriebel', 'R. C. Richmond', 'M. Adamo', 'U. Afzal', 'M. Ala-Korpela', 'B. Albetti', 'O. Ammerpohl', 'J. F. Apperley', 'M. Beekman', 'P. A. Bertazzi', 'S. L. Black', 'C. Blancher', 'M. J. Bonder', 'Mario Brosch', 'M. Carstensen-Kirberg', 'A. J. de Craen', 'S. de Lusignan', 'A. Dehghan', 'M. Elkalaawy', 'K. Fischer', 'O. H. Franco', 'T. R. Gaunt', 'Jochen Hampe', 'M. Hashemi', 'A. Isaacs', 'A. Jenkinson', 'S. Jha', 'N. Kato', 'V. Krogh', 'M. Laffan', 'C. Meisinger', 'T. Meitinger', 'Z. Y. Mok', 'V. Motta', 'H. K. Ng', 'Z. Nikolakopoulou', 'G. Nteliopoulos', 'S. Panico', 'N. Pervjakova', 'H. Prokisch', 'W. Rathmann', 'M. Roden', 'F. Rota', 'M. A. Rozario', 'J. K. Sandling', 'Clemens Schafmayer', 'K. Schramm', 'R. Siebert', 'P. E. Slagboom', 'P. Soininen', 'L. Stolk', 'K. Strauch', 'E. S. Tai', 'L. Tarantini', 'B. Thorand', 'E. F. Tigchelaar', 'R. Tumino', 'A. G. Uitterlinden', 'C. van Duijn', 'J. B. van Meurs', 'P. Vineis', 'A. R. Wickremasinghe', 'C. Wijmenga', 'T. P. Yang', 'W. Yuan', 'A. Zhernakova', 'R. L. Batterham', 'G. D. Smith', 'P. Deloukas', 'B. T. Heijmans', 'C. Herder', 'A. Hofman', 'C. M. Lindgren', 'L. Milani', 'P. van der Harst', 'A. Peters', 'T. Illig', 'C. L. Relton', 'M. Waldenberger', 'M. R. Jarvelin', 'V. Bollati', 'R. Soong', 'T. D. Spector', 'J. Scott', 'M. I. McCarthy', 'P. Elliott', 'J. T. Bell', 'G. Matullo', 'C. Gieger', 'J. S. Kooner', 'H. Grallert', 'J. C. Chambers']</t>
-  </si>
-  <si>
-    <t>['J. Mwinyi', 'A. E. Bostrom', 'C. Pisanu', 'S. K. Murphy', 'W. Erhart', 'Clemens Schafmayer', 'Jochen Hampe', 'C. Moylan', 'H. B. Schioth']</t>
-  </si>
-  <si>
-    <t>['F. Stickel', 'C. Moreno', 'Jochen Hampe', 'M. Y. Morgan']</t>
-  </si>
-  <si>
-    <t>['H. B. Schioth', 'A. Bostrom', 'S. K. Murphy', 'W. Erhart', 'Jochen Hampe', 'C. Moylan', 'J. Mwinyi']</t>
-  </si>
-  <si>
-    <t>['O. M. Will', 'T. Damm', 'G. M. Campbell', 'Witigo Von Schönfels', 'Y. Acil', 'M. Will', 'A. Chalaris-Rissmann', 'M. Ayna', 'C. Drucker', 'C. C. Gluer']</t>
-  </si>
-  <si>
-    <t>['D. Waltemath', 'J. R. Karr', 'F. T. Bergmann', 'V. Chelliah', 'M. Hucka', 'M. Krantz', 'W. Liebermeister', 'P. Mendes', 'C. J. Myers', 'P. Pir', 'B. Alaybeyoglu', 'N. K. Aranganathan', 'K. Baghalian', 'A. T. Bittig', 'P. E. Burke', 'M. Cantarelli', 'Y. H. Chew', 'R. S. Costa', 'J. Cursons', 'T. Czauderna', 'A. P. Goldberg', 'H. F. Gomez', 'J. Hahn', 'T. Hameri', 'D. F. Gardiol', 'D. Kazakiewicz', 'I. Kiselev', 'V. Knight-Schrijver', 'C. Knupfer', 'Matthias König', 'D. Lee', 'A. Lloret-Villas', 'N. Mandrik', 'J. K. Medley', 'B. Moreau', 'H. Naderi-Meshkin', 'S. K. Palaniappan', 'D. Priego-Espinosa', 'M. Scharm', 'M. Sharma', 'K. Smallbone', 'N. J. Stanford', 'J. H. Song', 'T. Theile', 'M. Tokic', 'N. Tomar', 'V. Toure', 'J. Uhlendorf', 'T. M. Varusai', 'L. H. Watanabe', 'F. Wendland', 'M. Wolfien', 'J. T. Yurkovich', 'Y. Zhu', 'A. Zardilis', 'A. Zhukova', 'F. Schreiber']</t>
-  </si>
-  <si>
-    <t>['A. Zeigerer', 'A. Wuttke', 'G. Marsico', 'S. Seifert', 'Y. Kalaidzidis', 'M. Zerial']</t>
-  </si>
-  <si>
-    <t>['Seddik Hammad', 'Elisabetta Cavalcanti', 'Julia Werle', 'Maria Lucia Caruso', 'Anne Dropmann', 'Antonia Ignazzi', 'Matthias Philip Ebert', 'Steven Dooley', 'Gianluigi Giannelli']</t>
-  </si>
-  <si>
-    <t>['Seddik Hammad', 'Amnah Othman', 'Christoph Meyer', 'Ahmad Telfah', 'Joerg Lambert', 'Bedair Dewidar', 'Julia Werle', 'Zeribe Chike Nwosu', 'Abdo Mahli', 'Christof Dormann', 'Yan Gao', 'Kerry Gould', 'Mei Han', 'Xiaodong Yuan', 'Mikheil Gogiashvili', 'Roland Hergenröder', 'Claus Hellerbrand', 'Maria Thomas', 'Matthias Philip Ebert', 'Salah Amasheh', 'Jan Hengstler', 'Steven Dooley']</t>
-  </si>
-  <si>
-    <t>['Oskar Knittelfelder', 'S. Traikov', 'Olga Vvedenskaya', 'A. Schuhmann', 'S. Segeletz', 'A. Shevchenko', 'A. Shevchenko']</t>
-  </si>
-  <si>
-    <t>['Selahaddin Sezgin', 'Reham Hassan', 'Sebastian Zühlke', 'Lars Kuepfer', 'Jan Hengstler', 'Michael Spiteller', 'Ahmed Ghallab']</t>
-  </si>
-  <si>
-    <t>['Ahmed Ghallab', 'Ute Hofmann', 'Selahaddin Sezgin', 'Nachiket Vartak', 'Reham Hassan', 'Ayham Zaza', 'Patricio Godoy', 'Kai Markus Schneider', 'Georgia Guenther', 'Yasser A Ahmed', 'Aya A Abbas', 'Verena Keitel', 'Lars Kuepfer', 'Steven Dooley', 'Frank Lammert', 'Christian Trautwein', 'Michael Spiteller', 'Dirk Drasdo', 'Alan F Hofmann', 'Peter Jansen', 'Jan Hengstler', 'Raymond Reif']</t>
-  </si>
-  <si>
-    <t>['A. Schmoldt', 'H. F. Benthe', 'G. Haberland']</t>
-  </si>
-  <si>
-    <t>['André Homeyer', 'Seddik Hammad', 'Lars Ole Schwen', 'U. Dahmen', 'H. Hofener', 'Y. Gao', 'Steven Dooley', 'Andrea Schenk']</t>
-  </si>
-  <si>
-    <t>['D. Waltemath', 'F. T. Bergmann', 'C. Chaouiya', 'T. Czauderna', 'P. Gleeson', 'C. Goble', 'Martin Golebiewski', 'M. Hucka', 'N. Juty', 'O. Krebs', 'N. Le Novere', 'H. Mi', 'I. I. Moraru', 'C. J. Myers', 'D. Nickerson', 'B. G. Olivier', 'N. Rodriguez', 'F. Schreiber', 'L. Smith', 'F. Zhang', 'E. Bonnet']</t>
-  </si>
-  <si>
-    <t>['Ersin Karatayli', 'R. A. Hall', 'Susanne Weber', 'Steven Dooley', 'Frank Lammert']</t>
-  </si>
-  <si>
-    <t>['K. Abshagen', 'B. Degenhardt', 'M. Liebig', 'A. Wendt', 'B. Genz', 'U. Schaeper', 'M. Stumvoll', 'Ute Hofmann', 'M. Frank', 'B. Vollmar', 'N. Kloting']</t>
-  </si>
-  <si>
-    <t>['Matthias Reichert', 'Frank Lammert']</t>
-  </si>
-  <si>
-    <t>['M. Jamka', 'A. Arslanow', 'A. Bohner', 'M. Krawczyk', 'Susanne Weber', 'F. Grunhage', 'Frank Lammert', 'C. S. Stokes']</t>
-  </si>
-  <si>
-    <t>['Olga Vvedenskaya', 'Yuting Wang', 'Jacobo Miranda Ackerman', 'Oskar Knittelfelder', 'Andrej Shevchenko']</t>
-  </si>
-  <si>
-    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Thomas Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
-  </si>
-  <si>
-    <t>['Christiane Rennert', 'Sebastian Vlaic', 'Eugenia Marbach-Breitrück', 'Carlo Thiel', 'Susanne Sales', 'Andrej Shevchenko', 'Rolf Gebhardt', 'Madlen Matz-Soja']</t>
-  </si>
-  <si>
-    <t>['Y. Wang', 'B. Moussian', 'E. Schaeffeler', 'Matthias Schwab', 'A. T. Nies']</t>
+    <t>['Witigo Von Schönfels', 'J. H. Beckmann', 'M. Ahrens', 'A. Hendricks', 'C. Rocken', 'S. Szymczak', 'Jochen Hampe', 'Clemens Schafmayer']</t>
+  </si>
+  <si>
+    <t>['R. Apweiler', 'T. Beissbarth', 'M. R. Berthold', 'N. Bluthgen', 'Y. Burmeister', 'O. Dammann', 'A. Deutsch', 'F. Feuerhake', 'A. Franke', 'J. Hasenauer', 'S. Hoffmann', 'T. Hofer', 'P. L. Jansen', 'Lars Kaderali', 'U. Klingmuller', 'Ulrike Koch', 'O. Kohlbacher', 'Lars Kuepfer', 'F. Lammert', 'D. Maier', 'N. Pfeifer', 'N. Radde', 'M. Rehm', 'I. Roeder', 'J. Saez-Rodriguez', 'U. Sax', 'B. Schmeck', 'A. Schuppert', 'B. Seilheimer', 'F. J. Theis', 'J. Vera', 'O. Wolkenhauer']</t>
+  </si>
+  <si>
+    <t>['Amruta Damle Vartak']</t>
+  </si>
+  <si>
+    <t>['A. Lorentzen', 'P. F. Becker', 'J. Kosla', 'M. Saini', 'K. Weidele', 'P. Ronchi', 'C. Klein', 'M. J. Wolf', 'F. Geist', 'B. Seubert', 'M. Ringelhan', 'D. Mihic-Probst', 'K. Esser', 'M. Roblek', 'F. Kuehne', 'G. Bianco', "T. O'Connor", 'Q. Muller', 'K. Schuck', 'S. Lange', 'D. Hartmann', 'S. Spaich', 'O. Gross', 'J. Utikal', 'S. Haferkamp', 'M. R. Sprick', 'Amruta Damle Vartak', 'A. Hapfelmeier', 'N. Huser', 'U. Protzer', 'A. Trumpp', 'D. Saur', 'Nachiket Vartak', 'C. A. Klein', 'B. Polzer', 'L. Borsig', 'M. Heikenwalder']</t>
+  </si>
+  <si>
+    <t>['Peter Jansen', 'Ahmed Ghallab', 'Nachiket Vartak', 'R. Reif', 'Frank Lammert', 'Jochen Hampe', 'Jan Hengstler']</t>
+  </si>
+  <si>
+    <t>['Ryoichi Fujiwara', 'Mathias Haag', 'Elke Schaeffeler', 'Anne T. Nies', 'Ulrich M. Zanger', 'Matthias Schwab']</t>
   </si>
   <si>
     <t>{'data': [{'id': '2', 'type': 'projects'}]}</t>
@@ -1369,6 +1597,9 @@
   </si>
   <si>
     <t>{'data': [{'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '2', 'type': 'projects'}, {'id': '10', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
   </si>
 </sst>
 </file>
@@ -1739,7 +1970,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1770,19 +2001,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="E2" t="s">
-        <v>331</v>
+        <v>389</v>
       </c>
       <c r="F2" t="s">
-        <v>434</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1790,19 +2021,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
-        <v>332</v>
+        <v>390</v>
       </c>
       <c r="F3" t="s">
-        <v>434</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1810,19 +2041,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="E4" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="F4" t="s">
-        <v>434</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1830,19 +2061,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>238</v>
+        <v>279</v>
       </c>
       <c r="E5" t="s">
-        <v>334</v>
+        <v>392</v>
       </c>
       <c r="F5" t="s">
-        <v>434</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1850,19 +2081,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="E6" t="s">
-        <v>335</v>
+        <v>393</v>
       </c>
       <c r="F6" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1870,19 +2101,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
       <c r="E7" t="s">
-        <v>336</v>
+        <v>394</v>
       </c>
       <c r="F7" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1890,19 +2121,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="D8" t="s">
-        <v>241</v>
+        <v>282</v>
       </c>
       <c r="E8" t="s">
-        <v>337</v>
+        <v>395</v>
       </c>
       <c r="F8" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1910,19 +2141,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
       <c r="E9" t="s">
-        <v>338</v>
+        <v>396</v>
       </c>
       <c r="F9" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1930,19 +2161,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
-        <v>243</v>
+        <v>284</v>
       </c>
       <c r="E10" t="s">
-        <v>339</v>
+        <v>397</v>
       </c>
       <c r="F10" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1950,19 +2181,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>244</v>
+        <v>285</v>
       </c>
       <c r="E11" t="s">
-        <v>340</v>
+        <v>398</v>
       </c>
       <c r="F11" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1970,19 +2201,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="E12" t="s">
-        <v>341</v>
+        <v>399</v>
       </c>
       <c r="F12" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1990,19 +2221,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
       <c r="E13" t="s">
-        <v>342</v>
+        <v>400</v>
       </c>
       <c r="F13" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2010,19 +2241,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="D14" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="E14" t="s">
-        <v>343</v>
+        <v>401</v>
       </c>
       <c r="F14" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2030,19 +2261,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="E15" t="s">
-        <v>344</v>
+        <v>402</v>
       </c>
       <c r="F15" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2050,19 +2281,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
       <c r="E16" t="s">
-        <v>345</v>
+        <v>403</v>
       </c>
       <c r="F16" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2070,19 +2301,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>291</v>
       </c>
       <c r="E17" t="s">
-        <v>346</v>
+        <v>404</v>
       </c>
       <c r="F17" t="s">
-        <v>439</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2090,19 +2321,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="D18" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="E18" t="s">
-        <v>347</v>
+        <v>405</v>
       </c>
       <c r="F18" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2110,19 +2341,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
       <c r="E19" t="s">
-        <v>348</v>
+        <v>406</v>
       </c>
       <c r="F19" t="s">
-        <v>440</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2130,19 +2361,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="D20" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="E20" t="s">
-        <v>349</v>
+        <v>407</v>
       </c>
       <c r="F20" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2150,19 +2381,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="D21" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="E21" t="s">
-        <v>350</v>
+        <v>408</v>
       </c>
       <c r="F21" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2170,19 +2401,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
       <c r="E22" t="s">
-        <v>351</v>
+        <v>409</v>
       </c>
       <c r="F22" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2190,19 +2421,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="E23" t="s">
-        <v>352</v>
+        <v>410</v>
       </c>
       <c r="F23" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2210,19 +2441,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="D24" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="E24" t="s">
-        <v>353</v>
+        <v>411</v>
       </c>
       <c r="F24" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2230,19 +2461,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="E25" t="s">
-        <v>354</v>
+        <v>412</v>
       </c>
       <c r="F25" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2250,19 +2481,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="D26" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="E26" t="s">
-        <v>355</v>
+        <v>413</v>
       </c>
       <c r="F26" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2270,19 +2501,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="D27" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="E27" t="s">
-        <v>356</v>
+        <v>414</v>
       </c>
       <c r="F27" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2290,19 +2521,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="E28" t="s">
-        <v>357</v>
+        <v>415</v>
       </c>
       <c r="F28" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2310,19 +2541,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="D29" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="E29" t="s">
-        <v>357</v>
+        <v>415</v>
       </c>
       <c r="F29" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2330,19 +2561,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
+        <v>303</v>
       </c>
       <c r="E30" t="s">
-        <v>358</v>
+        <v>416</v>
       </c>
       <c r="F30" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2350,19 +2581,19 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="C31" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="D31" t="s">
-        <v>263</v>
+        <v>304</v>
       </c>
       <c r="E31" t="s">
-        <v>359</v>
+        <v>417</v>
       </c>
       <c r="F31" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2370,19 +2601,19 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="D32" t="s">
-        <v>262</v>
+        <v>303</v>
       </c>
       <c r="E32" t="s">
-        <v>360</v>
+        <v>418</v>
       </c>
       <c r="F32" t="s">
-        <v>440</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2390,19 +2621,19 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="E33" t="s">
-        <v>361</v>
+        <v>419</v>
       </c>
       <c r="F33" t="s">
-        <v>441</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2410,19 +2641,19 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="D34" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
       <c r="E34" t="s">
-        <v>362</v>
+        <v>420</v>
       </c>
       <c r="F34" t="s">
-        <v>441</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2430,19 +2661,19 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="C35" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="D35" t="s">
-        <v>266</v>
+        <v>307</v>
       </c>
       <c r="E35" t="s">
-        <v>363</v>
+        <v>421</v>
       </c>
       <c r="F35" t="s">
-        <v>442</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2450,19 +2681,19 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="D36" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="E36" t="s">
-        <v>364</v>
+        <v>422</v>
       </c>
       <c r="F36" t="s">
-        <v>443</v>
+        <v>519</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2470,16 +2701,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="E37" t="s">
-        <v>365</v>
+        <v>423</v>
       </c>
       <c r="F37" t="s">
-        <v>444</v>
+        <v>520</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2487,16 +2718,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>268</v>
+        <v>309</v>
       </c>
       <c r="E38" t="s">
-        <v>366</v>
+        <v>424</v>
       </c>
       <c r="F38" t="s">
-        <v>445</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2504,16 +2735,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="E39" t="s">
-        <v>367</v>
+        <v>425</v>
       </c>
       <c r="F39" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2521,16 +2752,19 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>156</v>
+      </c>
+      <c r="C40" t="s">
+        <v>209</v>
       </c>
       <c r="D40" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
       <c r="E40" t="s">
-        <v>368</v>
+        <v>426</v>
       </c>
       <c r="F40" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2538,19 +2772,19 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="D41" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="E41" t="s">
-        <v>369</v>
+        <v>427</v>
       </c>
       <c r="F41" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2558,19 +2792,16 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="E42" t="s">
-        <v>370</v>
+        <v>428</v>
       </c>
       <c r="F42" t="s">
-        <v>437</v>
+        <v>522</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2578,16 +2809,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="E43" t="s">
-        <v>371</v>
+        <v>429</v>
       </c>
       <c r="F43" t="s">
-        <v>446</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2595,16 +2826,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D44" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="E44" t="s">
-        <v>372</v>
+        <v>430</v>
       </c>
       <c r="F44" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2612,16 +2843,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>275</v>
+        <v>316</v>
       </c>
       <c r="E45" t="s">
-        <v>373</v>
+        <v>431</v>
       </c>
       <c r="F45" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2629,50 +2860,50 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="D46" t="s">
-        <v>276</v>
+        <v>317</v>
       </c>
       <c r="E46" t="s">
-        <v>374</v>
+        <v>432</v>
       </c>
       <c r="F46" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="E47" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="F47" t="s">
-        <v>437</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
-        <v>247</v>
+        <v>318</v>
       </c>
       <c r="E48" t="s">
-        <v>343</v>
+        <v>433</v>
       </c>
       <c r="F48" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2680,16 +2911,19 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>159</v>
+      </c>
+      <c r="C49" t="s">
+        <v>223</v>
       </c>
       <c r="D49" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="E49" t="s">
-        <v>376</v>
+        <v>434</v>
       </c>
       <c r="F49" t="s">
-        <v>435</v>
+        <v>514</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2697,16 +2931,19 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
+        <v>223</v>
       </c>
       <c r="D50" t="s">
-        <v>279</v>
+        <v>320</v>
       </c>
       <c r="E50" t="s">
-        <v>377</v>
+        <v>435</v>
       </c>
       <c r="F50" t="s">
-        <v>435</v>
+        <v>523</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2714,19 +2951,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" t="s">
-        <v>198</v>
+        <v>161</v>
       </c>
       <c r="D51" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="E51" t="s">
-        <v>378</v>
+        <v>436</v>
       </c>
       <c r="F51" t="s">
-        <v>438</v>
+        <v>513</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2734,19 +2968,19 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D52" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="E52" t="s">
-        <v>379</v>
+        <v>437</v>
       </c>
       <c r="F52" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2754,16 +2988,19 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>162</v>
+      </c>
+      <c r="C53" t="s">
+        <v>239</v>
       </c>
       <c r="D53" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="E53" t="s">
-        <v>380</v>
+        <v>438</v>
       </c>
       <c r="F53" t="s">
-        <v>437</v>
+        <v>521</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2771,19 +3008,19 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="C54" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="D54" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="E54" t="s">
-        <v>381</v>
+        <v>439</v>
       </c>
       <c r="F54" t="s">
-        <v>438</v>
+        <v>521</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2791,19 +3028,19 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="D55" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="E55" t="s">
-        <v>382</v>
+        <v>440</v>
       </c>
       <c r="F55" t="s">
-        <v>445</v>
+        <v>521</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2811,19 +3048,19 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C56" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="D56" t="s">
-        <v>285</v>
+        <v>326</v>
       </c>
       <c r="E56" t="s">
-        <v>383</v>
+        <v>441</v>
       </c>
       <c r="F56" t="s">
-        <v>445</v>
+        <v>520</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2831,19 +3068,19 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="D57" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="E57" t="s">
-        <v>384</v>
+        <v>442</v>
       </c>
       <c r="F57" t="s">
-        <v>445</v>
+        <v>514</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2851,19 +3088,19 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="D58" t="s">
-        <v>287</v>
+        <v>328</v>
       </c>
       <c r="E58" t="s">
-        <v>385</v>
+        <v>443</v>
       </c>
       <c r="F58" t="s">
-        <v>444</v>
+        <v>521</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2871,19 +3108,19 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="C59" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D59" t="s">
-        <v>288</v>
+        <v>329</v>
       </c>
       <c r="E59" t="s">
-        <v>386</v>
+        <v>444</v>
       </c>
       <c r="F59" t="s">
-        <v>438</v>
+        <v>521</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2891,19 +3128,19 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="D60" t="s">
-        <v>289</v>
+        <v>330</v>
       </c>
       <c r="E60" t="s">
-        <v>387</v>
+        <v>445</v>
       </c>
       <c r="F60" t="s">
-        <v>445</v>
+        <v>521</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2911,19 +3148,19 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="D61" t="s">
-        <v>290</v>
+        <v>331</v>
       </c>
       <c r="E61" t="s">
-        <v>388</v>
+        <v>446</v>
       </c>
       <c r="F61" t="s">
-        <v>445</v>
+        <v>521</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2931,19 +3168,19 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C62" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D62" t="s">
-        <v>291</v>
+        <v>332</v>
       </c>
       <c r="E62" t="s">
-        <v>389</v>
+        <v>447</v>
       </c>
       <c r="F62" t="s">
-        <v>445</v>
+        <v>521</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2951,19 +3188,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="E63" t="s">
-        <v>390</v>
+        <v>448</v>
       </c>
       <c r="F63" t="s">
-        <v>445</v>
+        <v>524</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2971,19 +3205,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
-      </c>
-      <c r="C64" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>293</v>
+        <v>334</v>
       </c>
       <c r="E64" t="s">
-        <v>391</v>
+        <v>449</v>
       </c>
       <c r="F64" t="s">
-        <v>445</v>
+        <v>524</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2991,16 +3222,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="E65" t="s">
-        <v>392</v>
+        <v>450</v>
       </c>
       <c r="F65" t="s">
-        <v>448</v>
+        <v>524</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3008,16 +3239,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D66" t="s">
-        <v>295</v>
+        <v>336</v>
       </c>
       <c r="E66" t="s">
-        <v>393</v>
+        <v>451</v>
       </c>
       <c r="F66" t="s">
-        <v>448</v>
+        <v>524</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3025,16 +3256,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>296</v>
+        <v>337</v>
       </c>
       <c r="E67" t="s">
-        <v>394</v>
+        <v>452</v>
       </c>
       <c r="F67" t="s">
-        <v>448</v>
+        <v>524</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3042,16 +3273,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>297</v>
+        <v>338</v>
       </c>
       <c r="E68" t="s">
-        <v>395</v>
+        <v>453</v>
       </c>
       <c r="F68" t="s">
-        <v>448</v>
+        <v>513</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3059,16 +3290,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>154</v>
-      </c>
-      <c r="D69" t="s">
-        <v>298</v>
+        <v>173</v>
       </c>
       <c r="E69" t="s">
-        <v>396</v>
+        <v>454</v>
       </c>
       <c r="F69" t="s">
-        <v>448</v>
+        <v>524</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3076,16 +3304,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="D70" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
       <c r="E70" t="s">
-        <v>397</v>
+        <v>455</v>
       </c>
       <c r="F70" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3093,13 +3321,16 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>156</v>
+        <v>128</v>
+      </c>
+      <c r="D71" t="s">
+        <v>340</v>
       </c>
       <c r="E71" t="s">
-        <v>398</v>
+        <v>456</v>
       </c>
       <c r="F71" t="s">
-        <v>448</v>
+        <v>513</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3107,16 +3338,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>157</v>
-      </c>
-      <c r="D72" t="s">
-        <v>300</v>
+        <v>175</v>
+      </c>
+      <c r="C72" t="s">
+        <v>245</v>
       </c>
       <c r="E72" t="s">
-        <v>399</v>
+        <v>457</v>
       </c>
       <c r="F72" t="s">
-        <v>437</v>
+        <v>511</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3124,16 +3355,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
-      </c>
-      <c r="D73" t="s">
-        <v>301</v>
+        <v>176</v>
+      </c>
+      <c r="C73" t="s">
+        <v>245</v>
       </c>
       <c r="E73" t="s">
-        <v>400</v>
+        <v>458</v>
       </c>
       <c r="F73" t="s">
-        <v>437</v>
+        <v>511</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3141,16 +3372,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>158</v>
-      </c>
-      <c r="C74" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E74" t="s">
-        <v>401</v>
+        <v>459</v>
       </c>
       <c r="F74" t="s">
-        <v>435</v>
+        <v>524</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3158,16 +3386,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
-      </c>
-      <c r="C75" t="s">
-        <v>220</v>
+        <v>136</v>
+      </c>
+      <c r="D75" t="s">
+        <v>341</v>
       </c>
       <c r="E75" t="s">
-        <v>402</v>
+        <v>460</v>
       </c>
       <c r="F75" t="s">
-        <v>435</v>
+        <v>512</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3175,13 +3403,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>160</v>
+        <v>178</v>
+      </c>
+      <c r="C76" t="s">
+        <v>246</v>
       </c>
       <c r="E76" t="s">
-        <v>403</v>
+        <v>461</v>
       </c>
       <c r="F76" t="s">
-        <v>448</v>
+        <v>513</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3189,16 +3420,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
-      </c>
-      <c r="D77" t="s">
-        <v>302</v>
+        <v>179</v>
+      </c>
+      <c r="C77" t="s">
+        <v>247</v>
       </c>
       <c r="E77" t="s">
-        <v>404</v>
+        <v>462</v>
       </c>
       <c r="F77" t="s">
-        <v>436</v>
+        <v>513</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3206,16 +3437,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
-      </c>
-      <c r="C78" t="s">
-        <v>221</v>
+        <v>180</v>
+      </c>
+      <c r="D78" t="s">
+        <v>342</v>
       </c>
       <c r="E78" t="s">
-        <v>405</v>
+        <v>463</v>
       </c>
       <c r="F78" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3223,16 +3454,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
-      </c>
-      <c r="C79" t="s">
-        <v>222</v>
+        <v>181</v>
+      </c>
+      <c r="D79" t="s">
+        <v>343</v>
       </c>
       <c r="E79" t="s">
-        <v>406</v>
+        <v>464</v>
       </c>
       <c r="F79" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3240,16 +3471,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="D80" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="E80" t="s">
-        <v>407</v>
+        <v>465</v>
       </c>
       <c r="F80" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3257,16 +3488,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="D81" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="E81" t="s">
-        <v>408</v>
+        <v>466</v>
       </c>
       <c r="F81" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3274,16 +3505,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="D82" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="E82" t="s">
-        <v>409</v>
+        <v>467</v>
       </c>
       <c r="F82" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3291,16 +3522,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="D83" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="E83" t="s">
-        <v>410</v>
+        <v>468</v>
       </c>
       <c r="F83" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3308,16 +3539,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D84" t="s">
-        <v>307</v>
+        <v>348</v>
       </c>
       <c r="E84" t="s">
-        <v>411</v>
+        <v>469</v>
       </c>
       <c r="F84" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3325,16 +3556,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="D85" t="s">
-        <v>308</v>
+        <v>349</v>
       </c>
       <c r="E85" t="s">
-        <v>412</v>
+        <v>470</v>
       </c>
       <c r="F85" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3342,16 +3573,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="D86" t="s">
-        <v>309</v>
+        <v>350</v>
       </c>
       <c r="E86" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
       <c r="F86" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3359,16 +3590,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="D87" t="s">
-        <v>310</v>
+        <v>351</v>
       </c>
       <c r="E87" t="s">
-        <v>414</v>
+        <v>472</v>
       </c>
       <c r="F87" t="s">
-        <v>437</v>
+        <v>525</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3376,16 +3607,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="D88" t="s">
-        <v>311</v>
+        <v>352</v>
       </c>
       <c r="E88" t="s">
-        <v>415</v>
+        <v>473</v>
       </c>
       <c r="F88" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3393,16 +3624,19 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>136</v>
+      </c>
+      <c r="C89" t="s">
+        <v>248</v>
       </c>
       <c r="D89" t="s">
-        <v>312</v>
+        <v>353</v>
       </c>
       <c r="E89" t="s">
-        <v>416</v>
+        <v>474</v>
       </c>
       <c r="F89" t="s">
-        <v>449</v>
+        <v>520</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3410,16 +3644,19 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>136</v>
+      </c>
+      <c r="C90" t="s">
+        <v>249</v>
       </c>
       <c r="D90" t="s">
-        <v>313</v>
+        <v>354</v>
       </c>
       <c r="E90" t="s">
-        <v>417</v>
+        <v>475</v>
       </c>
       <c r="F90" t="s">
-        <v>437</v>
+        <v>521</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3427,19 +3664,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
-      </c>
-      <c r="C91" t="s">
-        <v>223</v>
+        <v>158</v>
       </c>
       <c r="D91" t="s">
-        <v>314</v>
+        <v>355</v>
       </c>
       <c r="E91" t="s">
-        <v>418</v>
+        <v>476</v>
       </c>
       <c r="F91" t="s">
-        <v>444</v>
+        <v>513</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3447,19 +3681,19 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C92" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="D92" t="s">
-        <v>315</v>
+        <v>356</v>
       </c>
       <c r="E92" t="s">
-        <v>419</v>
+        <v>477</v>
       </c>
       <c r="F92" t="s">
-        <v>445</v>
+        <v>512</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3467,16 +3701,19 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>141</v>
+        <v>190</v>
+      </c>
+      <c r="C93" t="s">
+        <v>251</v>
       </c>
       <c r="D93" t="s">
-        <v>316</v>
+        <v>357</v>
       </c>
       <c r="E93" t="s">
-        <v>420</v>
+        <v>478</v>
       </c>
       <c r="F93" t="s">
-        <v>437</v>
+        <v>512</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3484,39 +3721,24 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
-      </c>
-      <c r="C94" t="s">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="D94" t="s">
-        <v>317</v>
+        <v>358</v>
       </c>
       <c r="E94" t="s">
-        <v>421</v>
+        <v>479</v>
       </c>
       <c r="F94" t="s">
-        <v>436</v>
+        <v>517</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>97</v>
       </c>
-      <c r="B95" t="s">
-        <v>173</v>
-      </c>
-      <c r="C95" t="s">
-        <v>226</v>
-      </c>
-      <c r="D95" t="s">
-        <v>318</v>
-      </c>
-      <c r="E95" t="s">
-        <v>422</v>
-      </c>
       <c r="F95" t="s">
-        <v>436</v>
+        <v>517</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3524,24 +3746,33 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>133</v>
+        <v>191</v>
       </c>
       <c r="D96" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="E96" t="s">
-        <v>423</v>
+        <v>480</v>
       </c>
       <c r="F96" t="s">
-        <v>441</v>
+        <v>514</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>99</v>
       </c>
+      <c r="B97" t="s">
+        <v>192</v>
+      </c>
+      <c r="D97" t="s">
+        <v>360</v>
+      </c>
+      <c r="E97" t="s">
+        <v>481</v>
+      </c>
       <c r="F97" t="s">
-        <v>441</v>
+        <v>510</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3549,16 +3780,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="D98" t="s">
-        <v>320</v>
+        <v>361</v>
       </c>
       <c r="E98" t="s">
-        <v>424</v>
+        <v>482</v>
       </c>
       <c r="F98" t="s">
-        <v>438</v>
+        <v>526</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3566,16 +3797,19 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>175</v>
+        <v>141</v>
+      </c>
+      <c r="C99" t="s">
+        <v>252</v>
       </c>
       <c r="D99" t="s">
-        <v>321</v>
+        <v>362</v>
       </c>
       <c r="E99" t="s">
-        <v>425</v>
+        <v>483</v>
       </c>
       <c r="F99" t="s">
-        <v>434</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3583,16 +3817,19 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>176</v>
+        <v>194</v>
+      </c>
+      <c r="C100" t="s">
+        <v>253</v>
       </c>
       <c r="D100" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="E100" t="s">
-        <v>426</v>
+        <v>484</v>
       </c>
       <c r="F100" t="s">
-        <v>450</v>
+        <v>526</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3600,19 +3837,19 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="C101" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="D101" t="s">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="E101" t="s">
-        <v>427</v>
+        <v>485</v>
       </c>
       <c r="F101" t="s">
-        <v>437</v>
+        <v>526</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3620,19 +3857,19 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C102" t="s">
-        <v>228</v>
-      </c>
-      <c r="D102" t="s">
-        <v>324</v>
+        <v>255</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="E102" t="s">
-        <v>428</v>
+        <v>486</v>
       </c>
       <c r="F102" t="s">
-        <v>450</v>
+        <v>513</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3643,16 +3880,16 @@
         <v>159</v>
       </c>
       <c r="C103" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="D103" t="s">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c r="E103" t="s">
-        <v>429</v>
+        <v>487</v>
       </c>
       <c r="F103" t="s">
-        <v>450</v>
+        <v>522</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3660,19 +3897,19 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C104" t="s">
-        <v>230</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>326</v>
+        <v>257</v>
+      </c>
+      <c r="D104" t="s">
+        <v>367</v>
       </c>
       <c r="E104" t="s">
-        <v>430</v>
+        <v>488</v>
       </c>
       <c r="F104" t="s">
-        <v>437</v>
+        <v>522</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3680,19 +3917,19 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
       <c r="C105" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="D105" t="s">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="E105" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="F105" t="s">
-        <v>446</v>
+        <v>513</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3700,39 +3937,33 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="C106" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="D106" t="s">
-        <v>328</v>
+        <v>369</v>
       </c>
       <c r="E106" t="s">
-        <v>432</v>
+        <v>489</v>
       </c>
       <c r="F106" t="s">
-        <v>446</v>
+        <v>513</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>109</v>
       </c>
-      <c r="B107" t="s">
-        <v>179</v>
-      </c>
-      <c r="C107" t="s">
-        <v>233</v>
-      </c>
       <c r="D107" t="s">
-        <v>329</v>
+        <v>370</v>
       </c>
       <c r="E107" t="s">
-        <v>351</v>
+        <v>490</v>
       </c>
       <c r="F107" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3740,24 +3971,384 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="C108" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="D108" t="s">
-        <v>330</v>
+        <v>371</v>
       </c>
       <c r="E108" t="s">
-        <v>433</v>
+        <v>491</v>
       </c>
       <c r="F108" t="s">
-        <v>437</v>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="s">
+        <v>199</v>
+      </c>
+      <c r="C109" t="s">
+        <v>261</v>
+      </c>
+      <c r="D109" t="s">
+        <v>372</v>
+      </c>
+      <c r="E109" t="s">
+        <v>492</v>
+      </c>
+      <c r="F109" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="s">
+        <v>200</v>
+      </c>
+      <c r="C110" t="s">
+        <v>252</v>
+      </c>
+      <c r="D110" t="s">
+        <v>373</v>
+      </c>
+      <c r="E110" t="s">
+        <v>493</v>
+      </c>
+      <c r="F110" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="s">
+        <v>128</v>
+      </c>
+      <c r="C111" t="s">
+        <v>262</v>
+      </c>
+      <c r="D111" t="s">
+        <v>374</v>
+      </c>
+      <c r="E111" t="s">
+        <v>494</v>
+      </c>
+      <c r="F111" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>201</v>
+      </c>
+      <c r="C112" t="s">
+        <v>263</v>
+      </c>
+      <c r="D112" t="s">
+        <v>375</v>
+      </c>
+      <c r="E112" t="s">
+        <v>495</v>
+      </c>
+      <c r="F112" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" t="s">
+        <v>202</v>
+      </c>
+      <c r="C113" t="s">
+        <v>264</v>
+      </c>
+      <c r="D113" t="s">
+        <v>376</v>
+      </c>
+      <c r="E113" t="s">
+        <v>496</v>
+      </c>
+      <c r="F113" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" t="s">
+        <v>133</v>
+      </c>
+      <c r="C114" t="s">
+        <v>265</v>
+      </c>
+      <c r="D114" t="s">
+        <v>377</v>
+      </c>
+      <c r="E114" t="s">
+        <v>497</v>
+      </c>
+      <c r="F114" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115" t="s">
+        <v>159</v>
+      </c>
+      <c r="C115" t="s">
+        <v>266</v>
+      </c>
+      <c r="D115" t="s">
+        <v>378</v>
+      </c>
+      <c r="E115" t="s">
+        <v>498</v>
+      </c>
+      <c r="F115" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" t="s">
+        <v>136</v>
+      </c>
+      <c r="C116" t="s">
+        <v>267</v>
+      </c>
+      <c r="D116" t="s">
+        <v>379</v>
+      </c>
+      <c r="E116" t="s">
+        <v>499</v>
+      </c>
+      <c r="F116" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" t="s">
+        <v>159</v>
+      </c>
+      <c r="C117" t="s">
+        <v>256</v>
+      </c>
+      <c r="D117" t="s">
+        <v>366</v>
+      </c>
+      <c r="E117" t="s">
+        <v>500</v>
+      </c>
+      <c r="F117" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" t="s">
+        <v>119</v>
+      </c>
+      <c r="B118" t="s">
+        <v>203</v>
+      </c>
+      <c r="C118" t="s">
+        <v>268</v>
+      </c>
+      <c r="D118" t="s">
+        <v>380</v>
+      </c>
+      <c r="E118" t="s">
+        <v>501</v>
+      </c>
+      <c r="F118" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" t="s">
+        <v>149</v>
+      </c>
+      <c r="C119" t="s">
+        <v>269</v>
+      </c>
+      <c r="D119" t="s">
+        <v>381</v>
+      </c>
+      <c r="E119" t="s">
+        <v>502</v>
+      </c>
+      <c r="F119" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" t="s">
+        <v>270</v>
+      </c>
+      <c r="D120" t="s">
+        <v>382</v>
+      </c>
+      <c r="E120" t="s">
+        <v>503</v>
+      </c>
+      <c r="F120" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" t="s">
+        <v>204</v>
+      </c>
+      <c r="C121" t="s">
+        <v>271</v>
+      </c>
+      <c r="D121" t="s">
+        <v>383</v>
+      </c>
+      <c r="E121" t="s">
+        <v>504</v>
+      </c>
+      <c r="F121" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" t="s">
+        <v>205</v>
+      </c>
+      <c r="C122" t="s">
+        <v>272</v>
+      </c>
+      <c r="D122" t="s">
+        <v>384</v>
+      </c>
+      <c r="E122" t="s">
+        <v>505</v>
+      </c>
+      <c r="F122" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" t="s">
+        <v>136</v>
+      </c>
+      <c r="C123" t="s">
+        <v>256</v>
+      </c>
+      <c r="D123" t="s">
+        <v>385</v>
+      </c>
+      <c r="E123" t="s">
+        <v>506</v>
+      </c>
+      <c r="F123" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" t="s">
+        <v>159</v>
+      </c>
+      <c r="C124" t="s">
+        <v>273</v>
+      </c>
+      <c r="D124" t="s">
+        <v>386</v>
+      </c>
+      <c r="E124" t="s">
+        <v>507</v>
+      </c>
+      <c r="F124" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" t="s">
+        <v>137</v>
+      </c>
+      <c r="C125" t="s">
+        <v>274</v>
+      </c>
+      <c r="D125" t="s">
+        <v>387</v>
+      </c>
+      <c r="E125" t="s">
+        <v>508</v>
+      </c>
+      <c r="F125" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" t="s">
+        <v>127</v>
+      </c>
+      <c r="B126" t="s">
+        <v>137</v>
+      </c>
+      <c r="C126" t="s">
+        <v>275</v>
+      </c>
+      <c r="D126" t="s">
+        <v>388</v>
+      </c>
+      <c r="E126" t="s">
+        <v>509</v>
+      </c>
+      <c r="F126" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D104" r:id="rId1"/>
+    <hyperlink ref="D102" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated code for SEEK 1.8.1
</commit_message>
<xml_diff>
--- a/results/publications.xlsx
+++ b/results/publications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="574">
   <si>
     <t>title</t>
   </si>
@@ -309,97 +309,129 @@
     <t>Digitoxin metabolism by rat liver microsomes.</t>
   </si>
   <si>
+    <t>Focused scores enable reliable discrimination of small differences in steatosis.</t>
+  </si>
+  <si>
+    <t>Correction to: Meeting report from the fourth meeting of the Computational Modeling in Biology Network (COMBINE).</t>
+  </si>
+  <si>
+    <t>Effect of alcohol on the interleukin 6-mediated inflammatory response in a new mouse model of acute-on-chronic liver injury.</t>
+  </si>
+  <si>
+    <t>Liver-specific Repin1 deficiency impairs transient hepatic steatosis in liver regeneration.</t>
+  </si>
+  <si>
+    <t>ABCB4 Gene Aberrations in Human Liver Disease: An Evolving Spectrum</t>
+  </si>
+  <si>
+    <t>Effects of Gene Variants Controlling Vitamin D Metabolism and Serum Levels on Hepatic Steatosis.</t>
+  </si>
+  <si>
+    <t>Analytical challenges in human plasma lipidomics: A winding path towards the truth</t>
+  </si>
+  <si>
+    <t>Epigenomic map of human liver reveals principles of zonated morphogenic and metabolic control</t>
+  </si>
+  <si>
+    <t>The Diurnal Timing of Starvation Differently Impacts Murine Hepatic Gene Expression and Lipid Metabolism – A Systems Biology Analysis Using Self-Organizing Maps</t>
+  </si>
+  <si>
+    <t>Clinical and Functional Relevance of the Monocarboxylate Transporter Family in Disease Pathophysiology and Drug Therapy.</t>
+  </si>
+  <si>
+    <t>The fruit fly Drosophila melanogaster as an innovative preclinical ADME model for solute carrier membrane transporters, with consequences for pharmacology and drug therapy.</t>
+  </si>
+  <si>
+    <t>Liquid-crystal organization of liver tissue</t>
+  </si>
+  <si>
+    <t>Tomoelastography for the Evaluation of Pediatric Nonalcoholic Fatty Liver Disease</t>
+  </si>
+  <si>
+    <t>US Time-Harmonic Elastography: Detection of Liver Fibrosis in                     Adolescents with Extreme Obesity with Nonalcoholic Fatty Liver                     Disease</t>
+  </si>
+  <si>
+    <t>Genetic determinants of steatosis and fibrosis progression in pediatric non-alcoholic fatty liver disease.</t>
+  </si>
+  <si>
+    <t>Specifications of Standards in Systems and Synthetic Biology: Status and Developments in 2017.</t>
+  </si>
+  <si>
+    <t>Harmonizing semantic annotations for computational models in biology.</t>
+  </si>
+  <si>
+    <t>Data Formats for Systems Biology and Quantitative Modeling</t>
+  </si>
+  <si>
+    <t>A multiscale modelling approach to assess the impact of metabolic zonation and microperfusion on the hepatic carbohydrate metabolism.</t>
+  </si>
+  <si>
+    <t>HEPATOKIN1 is a biochemistry-based model of liver metabolism for applications in medicine and pharmacology.</t>
+  </si>
+  <si>
+    <t>Possible neurotoxicity of the anesthetic propofol: evidence for the inhibition of complex II of the respiratory chain in area CA3 of rat hippocampal slices.</t>
+  </si>
+  <si>
+    <t>Genetic variants in PNPLA3 and TM6SF2 predispose to the development of hepatocellular carcinoma in individuals with alcohol-related cirrhosis</t>
+  </si>
+  <si>
+    <t>Model-based identification of TNFalpha-induced IKKbeta-mediated and IkappaBalpha-mediated regulation of NFkappaB signal transduction as a tool to quantify the impact of drug-induced liver injury compounds.</t>
+  </si>
+  <si>
+    <t>Resolving the Combinatorial Complexity of Smad Protein Complex Formation and Its Link to Gene Expression.</t>
+  </si>
+  <si>
+    <t>Histologic improvement of NAFLD in patients with obesity after bariatric surgery based on standardized NAS (NAFLD activity score).</t>
+  </si>
+  <si>
+    <t>Whither systems medicine?</t>
+  </si>
+  <si>
+    <t>3D visualization of the biliary tree by X-ray phase-contrast computed tomography</t>
+  </si>
+  <si>
+    <t>Single cell polarity in liquid phase facilitates tumour metastasis.</t>
+  </si>
+  <si>
+    <t>The ascending pathophysiology of cholestatic liver disease.</t>
+  </si>
+  <si>
+    <t>Systemic regulation of bilirubin homeostasis: Potential benefits of hyperbilirubinemia</t>
+  </si>
+  <si>
     <t>Liver cancer cell lines distinctly mimic the metabolic gene expression pattern of the corresponding human tumours.</t>
   </si>
   <si>
-    <t>Focused scores enable reliable discrimination of small differences in steatosis.</t>
-  </si>
-  <si>
-    <t>Correction to: Meeting report from the fourth meeting of the Computational Modeling in Biology Network (COMBINE).</t>
-  </si>
-  <si>
-    <t>Effect of alcohol on the interleukin 6-mediated inflammatory response in a new mouse model of acute-on-chronic liver injury.</t>
-  </si>
-  <si>
-    <t>Liver-specific Repin1 deficiency impairs transient hepatic steatosis in liver regeneration.</t>
-  </si>
-  <si>
-    <t>ABCB4 Gene Aberrations in Human Liver Disease: An Evolving Spectrum</t>
-  </si>
-  <si>
-    <t>Effects of Gene Variants Controlling Vitamin D Metabolism and Serum Levels on Hepatic Steatosis.</t>
-  </si>
-  <si>
-    <t>Analytical challenges in human plasma lipidomics: A winding path towards the truth</t>
-  </si>
-  <si>
-    <t>Epigenomic map of human liver reveals principles of zonated morphogenic and metabolic control</t>
-  </si>
-  <si>
-    <t>The Diurnal Timing of Starvation Differently Impacts Murine Hepatic Gene Expression and Lipid Metabolism – A Systems Biology Analysis Using Self-Organizing Maps</t>
-  </si>
-  <si>
-    <t>Clinical and Functional Relevance of the Monocarboxylate Transporter Family in Disease Pathophysiology and Drug Therapy.</t>
-  </si>
-  <si>
-    <t>The fruit fly Drosophila melanogaster as an innovative preclinical ADME model for solute carrier membrane transporters, with consequences for pharmacology and drug therapy.</t>
-  </si>
-  <si>
-    <t>Liquid-crystal organization of liver tissue</t>
-  </si>
-  <si>
-    <t>Tomoelastography for the Evaluation of Pediatric Nonalcoholic Fatty Liver Disease</t>
-  </si>
-  <si>
-    <t>US Time-Harmonic Elastography: Detection of Liver Fibrosis in                     Adolescents with Extreme Obesity with Nonalcoholic Fatty Liver                     Disease</t>
-  </si>
-  <si>
-    <t>Genetic determinants of steatosis and fibrosis progression in pediatric non-alcoholic fatty liver disease.</t>
-  </si>
-  <si>
-    <t>Specifications of Standards in Systems and Synthetic Biology: Status and Developments in 2017.</t>
-  </si>
-  <si>
-    <t>Harmonizing semantic annotations for computational models in biology.</t>
-  </si>
-  <si>
-    <t>Data Formats for Systems Biology and Quantitative Modeling</t>
-  </si>
-  <si>
-    <t>A multiscale modelling approach to assess the impact of metabolic zonation and microperfusion on the hepatic carbohydrate metabolism.</t>
-  </si>
-  <si>
-    <t>HEPATOKIN1 is a biochemistry-based model of liver metabolism for applications in medicine and pharmacology.</t>
-  </si>
-  <si>
-    <t>Possible neurotoxicity of the anesthetic propofol: evidence for the inhibition of complex II of the respiratory chain in area CA3 of rat hippocampal slices.</t>
-  </si>
-  <si>
-    <t>Genetic variants in PNPLA3 and TM6SF2 predispose to the development of hepatocellular carcinoma in individuals with alcohol-related cirrhosis</t>
-  </si>
-  <si>
-    <t>Model-based identification of TNFalpha-induced IKKbeta-mediated and IkappaBalpha-mediated regulation of NFkappaB signal transduction as a tool to quantify the impact of drug-induced liver injury compounds.</t>
-  </si>
-  <si>
-    <t>Resolving the Combinatorial Complexity of Smad Protein Complex Formation and Its Link to Gene Expression.</t>
-  </si>
-  <si>
-    <t>Histologic improvement of NAFLD in patients with obesity after bariatric surgery based on standardized NAS (NAFLD activity score).</t>
-  </si>
-  <si>
-    <t>Whither systems medicine?</t>
-  </si>
-  <si>
-    <t>3D visualization of the biliary tree by X-ray phase-contrast computed tomography</t>
-  </si>
-  <si>
-    <t>Single cell polarity in liquid phase facilitates tumour metastasis.</t>
-  </si>
-  <si>
-    <t>The ascending pathophysiology of cholestatic liver disease.</t>
-  </si>
-  <si>
-    <t>Systemic regulation of bilirubin homeostasis: Potential benefits of hyperbilirubinemia</t>
+    <t>Simulation Experiment Description Markup Language (SED-ML) Level 1 Version 3 (L1V3).</t>
+  </si>
+  <si>
+    <t>Tellurium: An extensible python-based modeling environment for systems and synthetic biology.</t>
+  </si>
+  <si>
+    <t>Tellurium notebooks-An environment for reproducible dynamical modeling in systems biology.</t>
+  </si>
+  <si>
+    <t>Effect of alcohol on the interleukin 6-mediated inflammatory response in a new mouse model of acute-on-chronic liver injury</t>
+  </si>
+  <si>
+    <t>MicroRNA-942 mediates hepatic stellate cell activation by regulating BAMBI expression in human liver fibrosis.</t>
+  </si>
+  <si>
+    <t>Inverse agonist of ERRgamma reduces cannabinoid receptor type 1-mediated induction of fibrinogen synthesis in mice with a high-fat diet-intoxicated liver.</t>
+  </si>
+  <si>
+    <t>Ethanol sensitizes hepatocytes for TGF-beta-triggered apoptosis.</t>
+  </si>
+  <si>
+    <t>Hepatic
+              Smad7
+              overexpression causes severe iron overload in mice</t>
+  </si>
+  <si>
+    <t>Evolutionary Distance Predicts Recurrence After Liver Transplantation in Multifocal Hepatocellular Carcinoma.</t>
+  </si>
+  <si>
+    <t>SECOND EXPOSURE TO ACETAMINOPHEN OVERDOSE IS  ASSOCIATED WITH LIVER FIBROSIS IN MICE</t>
   </si>
   <si>
     <t>J Integr Bioinform</t>
@@ -636,6 +668,21 @@
     <t>Exp Mol Med</t>
   </si>
   <si>
+    <t>J Exp Clin Cancer Res</t>
+  </si>
+  <si>
+    <t>Biosystems</t>
+  </si>
+  <si>
+    <t>Biochimica et Biophysica Acta (BBA) - Molecular Basis of Disease</t>
+  </si>
+  <si>
+    <t>Transplantation</t>
+  </si>
+  <si>
+    <t>EXCLI</t>
+  </si>
+  <si>
     <t>2017-02-12</t>
   </si>
   <si>
@@ -846,6 +893,36 @@
     <t>2018-04-01</t>
   </si>
   <si>
+    <t>2018-09-05</t>
+  </si>
+  <si>
+    <t>2018-03-20</t>
+  </si>
+  <si>
+    <t>2018-07-28</t>
+  </si>
+  <si>
+    <t>2018-06-16</t>
+  </si>
+  <si>
+    <t>2019-02-01</t>
+  </si>
+  <si>
+    <t>2018-08-12</t>
+  </si>
+  <si>
+    <t>2018-07-19</t>
+  </si>
+  <si>
+    <t>2018-01-21</t>
+  </si>
+  <si>
+    <t>2018-07-12</t>
+  </si>
+  <si>
+    <t>2019-02-06</t>
+  </si>
+  <si>
     <t>J Integr Bioinform. 2016 Dec 18;13(3):289. doi: 10.2390/biecoll-jib-2016-289.</t>
   </si>
   <si>
@@ -1185,6 +1262,36 @@
     <t>Hepatology 67(4) : 1609</t>
   </si>
   <si>
+    <t>J Exp Clin Cancer Res. 2018 Sep 3;37(1):211. doi: 10.1186/s13046-018-0872-6.</t>
+  </si>
+  <si>
+    <t>J Integr Bioinform. 2018 Mar 19;15(1). pii: /j/jib.ahead-of-print/jib-2017-0086/jib-2017-0086.xml. doi: 10.1515/jib-2017-0086.</t>
+  </si>
+  <si>
+    <t>Biosystems. 2018 Sep;171:74-79. doi: 10.1016/j.biosystems.2018.07.006. Epub 2018  Jul 25.</t>
+  </si>
+  <si>
+    <t>PLoS Comput Biol. 2018 Jun 15;14(6):e1006220. doi: 10.1371/journal.pcbi.1006220.  eCollection 2018 Jun.</t>
+  </si>
+  <si>
+    <t>Biochimica et Biophysica Acta (BBA) - Molecular Basis of Disease 1865(2) : 298</t>
+  </si>
+  <si>
+    <t>Arch Toxicol. 2018 Sep;92(9):2935-2946. doi: 10.1007/s00204-018-2278-9. Epub 2018 Aug 10.</t>
+  </si>
+  <si>
+    <t>Arch Toxicol. 2018 Sep;92(9):2885-2896. doi: 10.1007/s00204-018-2270-4. Epub 2018 Jul 17.</t>
+  </si>
+  <si>
+    <t>Cell Death Dis. 2018 Jan 19;9(2):51. doi: 10.1038/s41419-017-0071-y.</t>
+  </si>
+  <si>
+    <t>Blood 131(5) : 581</t>
+  </si>
+  <si>
+    <t>Transplantation. 2018 Oct;102(10):e424-e430. doi: 10.1097/TP.0000000000002356.</t>
+  </si>
+  <si>
     <t>['F. Schreiber', 'G. D. Bader', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'N. Le Novere', 'C. Myers', 'D. Nickerson', 'B. Sommer', 'D. Walthemath']</t>
   </si>
   <si>
@@ -1197,16 +1304,16 @@
     <t>['Wolfgang Müller', 'Meik Bittkowski', 'Martin Golebiewski', 'Renate Kania', 'Maja Rey', 'Andreas Weidemann', 'Ulrike Wittig']</t>
   </si>
   <si>
-    <t>['B. Steiert', 'J. Timmer', 'C. Kreutz']</t>
-  </si>
-  <si>
-    <t>['R. Merkle', 'B. Steiert', 'F. Salopiata', 'S. Depner', 'A. Raue', 'N. Iwamoto', 'M. Schelker', 'H. Hass', 'M. Wasch', 'M. E. Bohm', 'O. Mucke', 'D. B. Lipka', 'C. Plass', 'W. D. Lehmann', 'C. Kreutz', 'J. Timmer', 'M. Schilling', 'U. Klingmuller']</t>
-  </si>
-  <si>
-    <t>['T. Maiwald', 'H. Hass', 'B. Steiert', 'J. Vanlier', 'R. Engesser', 'A. Raue', 'F. Kipkeew', 'H. H. Bock', 'D. Kaschek', 'C. Kreutz', 'J. Timmer']</t>
-  </si>
-  <si>
-    <t>['Ahmed Ghallab', 'Géraldine Cellière', 'Sebastian G. Henkel', 'Dominik Driesch', 'Stefan Hoehme', 'Ute Hofmann', 'Sebastian Zellmer', 'Patricio Godoy', 'Agapios Sachinidis', 'Meinolf Blaszkewicz', 'Raymond Reif', 'Rosemarie Marchan', 'Lars Kuepfer', 'Dieter Häussinger', 'Dirk Drasdo', 'Rolf Gebhardt', 'Jan G. Hengstler']</t>
+    <t>['B. Steiert', 'Jens Timmer', 'C. Kreutz']</t>
+  </si>
+  <si>
+    <t>['R. Merkle', 'B. Steiert', 'F. Salopiata', 'S. Depner', 'A. Raue', 'N. Iwamoto', 'M. Schelker', 'H. Hass', 'M. Wasch', 'M. E. Bohm', 'O. Mucke', 'D. B. Lipka', 'C. Plass', 'W. D. Lehmann', 'C. Kreutz', 'Jens Timmer', 'M. Schilling', 'U. Klingmuller']</t>
+  </si>
+  <si>
+    <t>['T. Maiwald', 'H. Hass', 'B. Steiert', 'J. Vanlier', 'R. Engesser', 'A. Raue', 'F. Kipkeew', 'H. H. Bock', 'D. Kaschek', 'C. Kreutz', 'Jens Timmer']</t>
+  </si>
+  <si>
+    <t>['Ahmed Ghallab', 'Géraldine Cellière', 'Sebastian G. Henkel', 'Dominik Driesch', 'Stefan Hoehme', 'Ute Hofmann', 'Sebastian Zellmer', 'Patricio Godoy', 'Agapios Sachinidis', 'Meinolf Blaszkewicz', 'Raymond Reif', 'Rosemarie Marchan', 'Lars Kuepfer', 'Dieter Häussinger', 'Dirk Drasdo', 'Rolf Gebhardt', 'Jan Hengstler']</t>
   </si>
   <si>
     <t>['Raymond Reif', 'Ahmed Ghallab', 'Lynette Beattie', 'Georgia Günther', 'Lars Kuepfer', 'Paul M. Kaye', 'Jan G. Hengstler']</t>
@@ -1218,7 +1325,7 @@
     <t>['A. Teufel', 'T. Itzel', 'W. Erhart', 'Mario Brosch', 'X. Y. Wang', 'Y. O. Kim', 'Witigo Von Schönfels', 'A. Herrmann', 'S. Bruckner', 'F. Stickel', 'J. F. Dufour', 'T. Chavakis', 'C. Hellerbrand', 'R. Spang', 'T. Maass', 'T. Becker', 'S. Schreiber', 'Clemens Schafmayer', 'D. Schuppan', 'Jochen Hampe']</t>
   </si>
   <si>
-    <t>['Stefan Hoehme', 'A. Friebel', 'Seddik Hammad', 'D. Drasdo', 'J. G. Hengstler']</t>
+    <t>['Stefan Hoehme', 'A. Friebel', 'Seddik Hammad', 'Dirk Drasdo', 'Jan Hengstler']</t>
   </si>
   <si>
     <t>['K. Breitkopf-Heinlein', 'C. Meyer', 'C. Konig', 'H. Gaitantzi', 'A. Addante', 'M. Thomas', 'E. Wiercinska', 'C. Cai', 'Q. Li', 'F. Wan', 'C. Hellerbrand', 'N. A. Valous', 'M. Hahnel', 'Christian Ehlting', 'Johannes Bode', 'S. Muller-Bohl', 'U. Klingmuller', 'J. Altenoder', 'I. Ilkavets', 'M. J. Goumans', 'L. J. Hawinkels', 'S. J. Lee', 'M. Wieland', 'C. Mogler', 'M. P. Ebert', 'B. Herrera', 'H. Augustin', 'A. Sanchez', 'Steven Dooley', 'P. Ten Dijke']</t>
@@ -1239,7 +1346,7 @@
     <t>['Christiane Rennert', 'Franziska Eplinius', 'Ute Hofmann', 'Janina Johänning', 'Franziska Rolfs', 'Wolfgang Schmidt-Heck', 'Reinhardt Guthke', 'Rolf Gebhardt', 'Albert M. Ricken', 'Madlen Matz-Soja']</t>
   </si>
   <si>
-    <t>['M. Krawczyk', 'S. Zimmermann', 'G. Hess', 'R. Holz', 'M. Dauer', 'J. Raedle', 'F. Lammert', 'F. Grunhage']</t>
+    <t>['M. Krawczyk', 'S. Zimmermann', 'G. Hess', 'R. Holz', 'M. Dauer', 'J. Raedle', 'Frank Lammert', 'F. Grunhage']</t>
   </si>
   <si>
     <t>['Markus Krauss', 'Ute Hofmann', 'Clemens Schafmayer', 'Svitlana Igel', 'Jan Schlender', 'Christian Mueller', 'Mario Brosch', 'Witigo von Schoenfels', 'Wiebke Erhart', 'Andreas Schuppert', 'Michael Block', 'Elke Schaeffeler', 'Gabriele Boehmer', 'Linus Goerlitz', 'Jan Hoecker', 'Joerg Lippert', 'Reinhold Kerb', 'Jochen Hampe', 'Lars Kuepfer', 'Matthias Schwab']</t>
@@ -1269,13 +1376,13 @@
     <t>['Christoph Thiel', 'Ute Hofmann', 'Ahmed Ghallab', 'Rolf Gebhardt', 'Jan G. Hengstler', 'Lars Kuepfer']</t>
   </si>
   <si>
-    <t>['T. Cvitanovic', 'Matthias Reichert', 'M. Moskon', 'M. Mraz', 'F. Lammert', 'D. Rozman']</t>
+    <t>['T. Cvitanovic', 'Matthias Reichert', 'M. Moskon', 'M. Mraz', 'Frank Lammert', 'D. Rozman']</t>
   </si>
   <si>
     <t>['Madlen Matz-Soja']</t>
   </si>
   <si>
-    <t>['Seddik Hammad', 'A. Braeuning', 'C. Meyer', 'F. E. Z. A. Mohamed', 'J. G. Hengstler', 'Steven Dooley']</t>
+    <t>['Seddik Hammad', 'A. Braeuning', 'C. Meyer', 'F. E. Z. A. Mohamed', 'Jan Hengstler', 'Steven Dooley']</t>
   </si>
   <si>
     <t>['Zeribe Chike Nwosu', 'Dominik Andre Megger', 'Seddik Hammad', 'Barbara Sitek', 'Stephanie Roessler', 'Matthias Philip Ebert', 'Christoph Meyer', 'Steven Dooley']</t>
@@ -1326,7 +1433,7 @@
     <t>['Chris J. Myers', 'Gary Bader', 'Padraig Gleeson', 'Martin Golebiewski', 'Michael Hucka', 'Nicolas Le Novere', 'David P. Nickerson', 'Falk Schreiber', 'Dagmar Waltemath']</t>
   </si>
   <si>
-    <t>['K. Meyer', 'O. Ostrenko', 'G. Bourantas', 'H. Morales-Navarrete', 'N. Porat-Shliom', 'F. Segovia-Miranda', 'H. Nonaka', 'A. Ghaemi', 'J. M. Verbavatz', 'Lutz Brusch', 'I. Sbalzarini', 'Y. Kalaidzidis', 'R. Weigert', 'M. Zerial']</t>
+    <t>['K. Meyer', 'O. Ostrenko', 'G. Bourantas', 'H. Morales-Navarrete', 'N. Porat-Shliom', 'Fabian Segovia Miranda', 'H. Nonaka', 'A. Ghaemi', 'J. M. Verbavatz', 'Lutz Brusch', 'I. Sbalzarini', 'Y. Kalaidzidis', 'R. Weigert', 'Marino Zerial']</t>
   </si>
   <si>
     <t>['Haristi Gaitantzi', 'Christoph Meyer', 'Pia Rakoczy', 'Maria Thomas', 'Kristin Wahl', 'Franziska Wandrer', 'Heike Bantel', 'Hamed Alborzinia', 'Stefan Wölfl', 'Sabrina Ehnert', 'Andreas Nüssler', 'Ina Bergheim', 'Loredana Ciuclan', 'Matthias Ebert', 'Katja Breitkopf-Heinlein', 'Steven Dooley']</t>
@@ -1398,16 +1505,16 @@
     <t>['Johannes Eckstein', 'Hergo Holzhütter', 'Nikolaus Berndt']</t>
   </si>
   <si>
-    <t>['M. Leist', 'Ahmed Ghallab', 'R. Graepel', 'R. Marchan', 'Reham Hassan', 'S. H. Bennekou', 'A. Limonciel', 'M. Vinken', 'S. Schildknecht', 'T. Waldmann', 'E. Danen', 'B. van Ravenzwaay', 'H. Kamp', 'I. Gardner', 'P. Godoy', 'F. Y. Bois', 'A. Braeuning', 'R. Reif', 'F. Oesch', 'D. Drasdo', 'Stefan Hoehme', 'M. Schwarz', 'T. Hartung', 'T. Braunbeck', 'J. Beltman', 'H. Vrieling', 'F. Sanz', 'A. Forsby', 'D. Gadaleta', 'C. Fisher', 'J. Kelm', 'D. Fluri', 'G. Ecker', 'B. Zdrazil', 'A. Terron', 'P. Jennings', 'B. van der Burg', 'Steven Dooley', 'A. H. Meijer', 'E. Willighagen', 'M. Martens', 'C. Evelo', 'E. Mombelli', 'O. Taboureau', 'A. Mantovani', 'B. Hardy', 'B. Koch', 'S. Escher', 'C. van Thriel', 'C. Cadenas', 'D. Kroese', 'B. van de Water', 'J. G. Hengstler']</t>
+    <t>['M. Leist', 'Ahmed Ghallab', 'R. Graepel', 'R. Marchan', 'Reham Hassan', 'S. H. Bennekou', 'A. Limonciel', 'M. Vinken', 'S. Schildknecht', 'T. Waldmann', 'E. Danen', 'B. van Ravenzwaay', 'H. Kamp', 'I. Gardner', 'P. Godoy', 'F. Y. Bois', 'A. Braeuning', 'R. Reif', 'F. Oesch', 'Dirk Drasdo', 'Stefan Hoehme', 'M. Schwarz', 'T. Hartung', 'T. Braunbeck', 'J. Beltman', 'H. Vrieling', 'F. Sanz', 'A. Forsby', 'D. Gadaleta', 'C. Fisher', 'J. Kelm', 'D. Fluri', 'G. Ecker', 'B. Zdrazil', 'A. Terron', 'P. Jennings', 'B. van der Burg', 'Steven Dooley', 'A. H. Meijer', 'E. Willighagen', 'M. Martens', 'C. Evelo', 'E. Mombelli', 'O. Taboureau', 'A. Mantovani', 'B. Hardy', 'B. Koch', 'S. Escher', 'C. van Thriel', 'C. Cadenas', 'D. Kroese', 'B. van de Water', 'Jan Hengstler']</t>
   </si>
   <si>
     <t>['Geert Peeters', 'Charlotte Debbaut', 'Wim Laleman', 'Adrian Friebel', 'Diethard Monbaliu', 'Ingrid Vander Elst', 'Jan R. Detrez', 'Tim Vandecasteele', 'Tim Johann', 'Thomas De Schryver', 'Luc Van Hoorebeke', 'Kasper Favere', 'Jonas Verbeke', 'Dirk Drasdo', 'Stefan Hoehme', 'Patrick Segers', 'Pieter Cornillie', 'Winnok H. De Vos']</t>
   </si>
   <si>
-    <t>['Stefan Hoehme', 'Francois Bertaux', 'William Weens', 'Bettina Grasl-Kraupp', 'Jan G. Hengstler', 'Dirk Drasdo']</t>
-  </si>
-  <si>
-    <t>['G. Peeters', 'C. Debbaut', 'A. Friebel', 'P. Cornillie', 'W. H. De Vos', 'K. Favere', 'I. Vander Elst', 'T. Vandecasteele', 'T. Johann', 'L. Van Hoorebeke', 'D. Monbaliu', 'D. Drasdo', 'Stefan Hoehme', 'W. Laleman', 'P. Segers']</t>
+    <t>['Stefan Hoehme', 'Francois Bertaux', 'William Weens', 'Bettina Grasl-Kraupp', 'Jan Hengstler', 'Dirk Drasdo']</t>
+  </si>
+  <si>
+    <t>['G. Peeters', 'C. Debbaut', 'A. Friebel', 'P. Cornillie', 'W. H. De Vos', 'K. Favere', 'I. Vander Elst', 'T. Vandecasteele', 'Tim Johann', 'L. Van Hoorebeke', 'D. Monbaliu', 'Dirk Drasdo', 'Stefan Hoehme', 'W. Laleman', 'P. Segers']</t>
   </si>
   <si>
     <t>['S. Stengel', 'A. Stallmach', 'K. Richter', 'A. Landrock', 'Jochen Hampe', 'T. Bruns']</t>
@@ -1437,7 +1544,7 @@
     <t>['D. Waltemath', 'J. R. Karr', 'F. T. Bergmann', 'V. Chelliah', 'M. Hucka', 'M. Krantz', 'W. Liebermeister', 'P. Mendes', 'C. J. Myers', 'P. Pir', 'B. Alaybeyoglu', 'N. K. Aranganathan', 'K. Baghalian', 'A. T. Bittig', 'P. E. Burke', 'M. Cantarelli', 'Y. H. Chew', 'R. S. Costa', 'J. Cursons', 'T. Czauderna', 'A. P. Goldberg', 'H. F. Gomez', 'J. Hahn', 'T. Hameri', 'D. F. Gardiol', 'D. Kazakiewicz', 'I. Kiselev', 'V. Knight-Schrijver', 'C. Knupfer', 'Matthias König', 'D. Lee', 'A. Lloret-Villas', 'N. Mandrik', 'J. K. Medley', 'B. Moreau', 'H. Naderi-Meshkin', 'S. K. Palaniappan', 'D. Priego-Espinosa', 'M. Scharm', 'M. Sharma', 'K. Smallbone', 'N. J. Stanford', 'J. H. Song', 'T. Theile', 'M. Tokic', 'N. Tomar', 'V. Toure', 'J. Uhlendorf', 'T. M. Varusai', 'L. H. Watanabe', 'F. Wendland', 'M. Wolfien', 'J. T. Yurkovich', 'Y. Zhu', 'A. Zardilis', 'A. Zhukova', 'F. Schreiber']</t>
   </si>
   <si>
-    <t>['A. Zeigerer', 'A. Wuttke', 'G. Marsico', 'S. Seifert', 'Y. Kalaidzidis', 'M. Zerial']</t>
+    <t>['A. Zeigerer', 'A. Wuttke', 'G. Marsico', 'S. Seifert', 'Y. Kalaidzidis', 'Marino Zerial']</t>
   </si>
   <si>
     <t>['Seddik Hammad', 'Elisabetta Cavalcanti', 'Julia Werle', 'Maria Lucia Caruso', 'Anne Dropmann', 'Antonia Ignazzi', 'Matthias Philip Ebert', 'Steven Dooley', 'Gianluigi Giannelli']</t>
@@ -1479,7 +1586,7 @@
     <t>['Olga Vvedenskaya', 'Yuting Wang', 'Jacobo Miranda Ackerman', 'Oskar Knittelfelder', 'Andrej Shevchenko']</t>
   </si>
   <si>
-    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Thomas Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
+    <t>['Mario Brosch', 'Kathrin Kattler', 'Alexander Herrmann', 'Witigo Von Schönfels', 'Karl Nordström', 'Daniel Seehofer', 'Georg Damm', 'Thomas Becker', 'Sebastian Zeissig', 'Sophie Nehring', 'Fabian Reichel', 'Vincent Moser', 'Raghavan Veera Thangapandi', 'Felix Stickel', 'Gustavo Baretton', 'Christoph Röcken', 'Michael Muders', 'Madlen Matz-Soja', 'Michael Krawczak', 'Gilles Gasparoni', 'Hella Hartmann', 'Andreas Dahl', 'Clemens Schafmayer', 'Jörn Walter', 'Jochen Hampe']</t>
   </si>
   <si>
     <t>['Christiane Rennert', 'Sebastian Vlaic', 'Eugenia Marbach-Breitrück', 'Carlo Thiel', 'Susanne Sales', 'Andrej Shevchenko', 'Rolf Gebhardt', 'Madlen Matz-Soja']</t>
@@ -1524,7 +1631,7 @@
     <t>['Felix Stickel', 'Stephan Buch', 'Hans Dieter Nischalke', 'Karl Heinz Weiss', 'Daniel Gotthardt', 'Janett Fischer', 'Jonas Rosendahl', 'Astrid Marot', 'Mona Elamly', 'Markus Casper', 'Frank Lammert', 'Andrew McQuillin', 'Steffen Zopf', 'Ulrich Spengler', 'Silke Marhenke', 'Martha M. Kirstein', 'Arndt Vogel', 'Florian Eyer', 'Johann von Felden', 'Henning Wege', 'Thorsten Buch', 'Clemens Schafmayer', 'Felix Braun', 'Pierre Deltenre', 'Thomas Berg', 'Marsha Y. Morgan', 'Jochen Hampe']</t>
   </si>
   <si>
-    <t>['A. Oppelt', 'D. Kaschek', 'S. Huppelschoten', 'R. Sison-Young', 'F. Zhang', 'M. Buck-Wiese', 'F. Herrmann', 'S. Malkusch', 'C. L. Kruger', 'M. Meub', 'B. Merkt', 'L. Zimmermann', 'A. Schofield', 'R. P. Jones', 'H. Malik', 'M. Schilling', 'M. Heilemann', 'B. van de Water', 'C. E. Goldring', 'B. K. Park', 'J. Timmer', 'U. Klingmuller']</t>
+    <t>['A. Oppelt', 'D. Kaschek', 'S. Huppelschoten', 'R. Sison-Young', 'F. Zhang', 'M. Buck-Wiese', 'F. Herrmann', 'S. Malkusch', 'C. L. Kruger', 'M. Meub', 'B. Merkt', 'L. Zimmermann', 'A. Schofield', 'R. P. Jones', 'H. Malik', 'M. Schilling', 'M. Heilemann', 'B. van de Water', 'C. E. Goldring', 'B. K. Park', 'Jens Timmer', 'U. Klingmuller']</t>
   </si>
   <si>
     <t>['P. Lucarelli', 'M. Schilling', 'C. Kreutz', 'A. Vlasov', 'M. E. Boehm', 'N. Iwamoto', 'B. Steiert', 'S. Lattermann', 'M. Wasch', 'M. Stepath', 'M. S. Matter', 'M. Heikenwalder', 'Professor Dr.  Med. Katrin Hoffmann', 'D. Deharde', 'G. Damm', 'D. Seehofer', 'M. Muciek', 'N. Gretz', 'W. D. Lehmann', 'J. Timmer', 'U. Klingmuller']</t>
@@ -1548,58 +1655,91 @@
     <t>['Ryoichi Fujiwara', 'Mathias Haag', 'Elke Schaeffeler', 'Anne T. Nies', 'Ulrich M. Zanger', 'Matthias Schwab']</t>
   </si>
   <si>
-    <t>{'data': [{'id': '2', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '5', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '7', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '3', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '4', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '5', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '9', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '10', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '8', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '9', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '2', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '6', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '10', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'id': '2', 'type': 'projects'}, {'id': '10', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+    <t>['Z. C. Nwosu', 'N. Battello', 'M. Rothley', 'W. Pioronska', 'B. Sitek', 'M. P. Ebert', 'Ute Hofmann', 'J. Sleeman', 'S. Wolfl', 'C. Meyer', 'D. A. Megger', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['F. T. Bergmann', 'J. Cooper', 'Matthias König', 'I. Moraru', 'D. Nickerson', 'N. Le Novere', 'B. G. Olivier', 'S. Sahle', 'L. Smith', 'D. Waltemath']</t>
+  </si>
+  <si>
+    <t>['K. Choi', 'J. K. Medley', 'Matthias König', 'K. Stocking', 'L. Smith', 'S. Gu', 'H. M. Sauro']</t>
+  </si>
+  <si>
+    <t>['J. K. Medley', 'K. Choi', 'Matthias König', 'L. Smith', 'S. Gu', 'J. Hellerstein', 'S. C. Sealfon', 'H. M. Sauro']</t>
+  </si>
+  <si>
+    <t>['Ersin Karatayli', 'Rabea A. Hall', 'Susanne Weber', 'Steven Dooley', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['L. Tao', 'D. Xue', 'D. Shen', 'W. Ma', 'J. Zhang', 'X. Wang', 'W. Zhang', 'L. Wu', 'K. Pan', 'Y. Yang', 'Z. C. Nwosu', 'Steven Dooley', 'E. Seki', 'C. Liu']</t>
+  </si>
+  <si>
+    <t>['Y. Zhang', 'D. K. Kim', 'Y. S. Jung', 'Y. H. Kim', 'Y. S. Lee', 'J. Kim', 'W. I. Jeong', 'I. K. Lee', 'S. J. Cho', 'Steven Dooley', 'C. H. Lee', 'H. S. Choi']</t>
+  </si>
+  <si>
+    <t>['H. Gaitantzi', 'C. Meyer', 'P. Rakoczy', 'M. Thomas', 'K. Wahl', 'F. Wandrer', 'H. Bantel', 'H. Alborzinia', 'S. Wolfl', 'S. Ehnert', 'A. Nussler', 'I. Bergheim', 'L. Ciuclan', 'M. Ebert', 'K. Breitkopf-Heinlein', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['Dilay Lai', 'Feng Teng', 'Seddik Hammad', 'Julia Werle', 'Thorsten Maas', 'Andreas Teufel', 'Martina U. Muckenthaler', 'Steven Dooley', 'Maja Vujić Spasić']</t>
+  </si>
+  <si>
+    <t>['N. Heits', 'Mario Brosch', 'A. Herrmann', 'R. Behrens', 'C. Rocken', 'H. Schrem', 'A. Kaltenborn', 'J. Klempnauer', 'H. H. Kreipe', 'B. Reichert', 'C. Lenschow', 'C. Wilms', 'T. Vogel', 'H. Wolters', 'E. Wardelmann', 'D. Seehofer', 'S. Buch', 'S. Zeissig', 'S. Pannach', 'N. Raschzok', 'M. Dietel', 'W. von Schoenfels', 'S. Hinz', 'A. Teufel', 'M. Evert', 'A. Franke', 'Ann-Kristin Becker', 'F. Braun', 'Jochen Hampe', 'Clemens Schafmayer']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad']</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '2'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '5'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '7'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '3'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '4'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '5'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '9'}, {'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '5'}, {'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '10'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '8'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '9'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '2'}, {'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '6'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '10'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '5'}, {'type': 'projects', 'id': '13'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'type': 'projects', 'id': '2'}, {'type': 'projects', 'id': '10'}, {'type': 'projects', 'id': '13'}]}</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +2110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2001,19 +2141,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="F2" t="s">
-        <v>510</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2021,19 +2161,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D3" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="E3" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="F3" t="s">
-        <v>510</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2041,19 +2181,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="E4" t="s">
-        <v>391</v>
+        <v>426</v>
       </c>
       <c r="F4" t="s">
-        <v>510</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2061,19 +2201,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="E5" t="s">
-        <v>392</v>
+        <v>427</v>
       </c>
       <c r="F5" t="s">
-        <v>510</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2081,19 +2221,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="E6" t="s">
-        <v>393</v>
+        <v>428</v>
       </c>
       <c r="F6" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2101,19 +2241,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D7" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="E7" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="F7" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2121,19 +2261,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D8" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="E8" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="F8" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2141,19 +2281,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="E9" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
       <c r="F9" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2161,19 +2301,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="E10" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2181,19 +2321,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="E11" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
       <c r="F11" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2201,19 +2341,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="E12" t="s">
-        <v>399</v>
+        <v>434</v>
       </c>
       <c r="F12" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2221,19 +2361,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="D13" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="E13" t="s">
-        <v>400</v>
+        <v>435</v>
       </c>
       <c r="F13" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2241,19 +2381,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="D14" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="E14" t="s">
-        <v>401</v>
+        <v>436</v>
       </c>
       <c r="F14" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2261,19 +2401,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="E15" t="s">
-        <v>402</v>
+        <v>437</v>
       </c>
       <c r="F15" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2281,19 +2421,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="E16" t="s">
-        <v>403</v>
+        <v>438</v>
       </c>
       <c r="F16" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2301,19 +2441,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D17" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="E17" t="s">
-        <v>404</v>
+        <v>439</v>
       </c>
       <c r="F17" t="s">
-        <v>515</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2321,19 +2461,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="D18" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
       <c r="E18" t="s">
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="F18" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2341,19 +2481,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="D19" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="E19" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="F19" t="s">
-        <v>516</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2361,19 +2501,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="D20" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="E20" t="s">
-        <v>407</v>
+        <v>442</v>
       </c>
       <c r="F20" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2381,19 +2521,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D21" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="E21" t="s">
-        <v>408</v>
+        <v>443</v>
       </c>
       <c r="F21" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2401,19 +2541,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="D22" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="E22" t="s">
-        <v>409</v>
+        <v>444</v>
       </c>
       <c r="F22" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2421,19 +2561,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D23" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
       <c r="E23" t="s">
-        <v>410</v>
+        <v>445</v>
       </c>
       <c r="F23" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2441,19 +2581,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="D24" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="E24" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="F24" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2461,19 +2601,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="D25" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="E25" t="s">
-        <v>412</v>
+        <v>447</v>
       </c>
       <c r="F25" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2481,19 +2621,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="D26" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="E26" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
       <c r="F26" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2501,19 +2641,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="D27" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="E27" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
       <c r="F27" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2521,19 +2661,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D28" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="E28" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
       <c r="F28" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2541,19 +2681,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D29" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="E29" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
       <c r="F29" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2561,19 +2701,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="D30" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="E30" t="s">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="F30" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2581,19 +2721,19 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="E31" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
       <c r="F31" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2601,19 +2741,19 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="D32" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="E32" t="s">
-        <v>418</v>
+        <v>453</v>
       </c>
       <c r="F32" t="s">
-        <v>516</v>
+        <v>562</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2621,19 +2761,19 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="D33" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="E33" t="s">
-        <v>419</v>
+        <v>454</v>
       </c>
       <c r="F33" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2641,19 +2781,19 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="D34" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="E34" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="F34" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2661,19 +2801,19 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="D35" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="E35" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
       <c r="F35" t="s">
-        <v>518</v>
+        <v>564</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2681,19 +2821,19 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="D36" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="E36" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="F36" t="s">
-        <v>519</v>
+        <v>565</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2701,16 +2841,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="E37" t="s">
-        <v>423</v>
+        <v>458</v>
       </c>
       <c r="F37" t="s">
-        <v>520</v>
+        <v>566</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2718,16 +2858,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="E38" t="s">
-        <v>424</v>
+        <v>459</v>
       </c>
       <c r="F38" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2735,16 +2875,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D39" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="E39" t="s">
-        <v>425</v>
+        <v>460</v>
       </c>
       <c r="F39" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2752,19 +2892,19 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D40" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="E40" t="s">
-        <v>426</v>
+        <v>461</v>
       </c>
       <c r="F40" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2772,19 +2912,19 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C41" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="D41" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="E41" t="s">
-        <v>427</v>
+        <v>462</v>
       </c>
       <c r="F41" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2792,16 +2932,16 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="E42" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="F42" t="s">
-        <v>522</v>
+        <v>568</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2809,16 +2949,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="E43" t="s">
-        <v>429</v>
+        <v>464</v>
       </c>
       <c r="F43" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2826,16 +2966,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="E44" t="s">
-        <v>430</v>
+        <v>465</v>
       </c>
       <c r="F44" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2843,16 +2983,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="E45" t="s">
-        <v>431</v>
+        <v>466</v>
       </c>
       <c r="F45" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2860,16 +3000,16 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D46" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="E46" t="s">
-        <v>432</v>
+        <v>467</v>
       </c>
       <c r="F46" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2877,16 +3017,16 @@
         <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="E47" t="s">
-        <v>401</v>
+        <v>436</v>
       </c>
       <c r="F47" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2894,16 +3034,16 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="E48" t="s">
-        <v>433</v>
+        <v>468</v>
       </c>
       <c r="F48" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2911,19 +3051,19 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C49" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D49" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="E49" t="s">
-        <v>434</v>
+        <v>469</v>
       </c>
       <c r="F49" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2931,19 +3071,19 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D50" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="E50" t="s">
-        <v>435</v>
+        <v>470</v>
       </c>
       <c r="F50" t="s">
-        <v>523</v>
+        <v>569</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2951,16 +3091,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="E51" t="s">
-        <v>436</v>
+        <v>471</v>
       </c>
       <c r="F51" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2968,19 +3108,19 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D52" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="E52" t="s">
-        <v>437</v>
+        <v>472</v>
       </c>
       <c r="F52" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2988,19 +3128,19 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="D53" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
       <c r="E53" t="s">
-        <v>438</v>
+        <v>473</v>
       </c>
       <c r="F53" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3008,19 +3148,19 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="D54" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="E54" t="s">
-        <v>439</v>
+        <v>474</v>
       </c>
       <c r="F54" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3028,19 +3168,19 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D55" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="E55" t="s">
-        <v>440</v>
+        <v>475</v>
       </c>
       <c r="F55" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3048,19 +3188,19 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="D56" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="E56" t="s">
-        <v>441</v>
+        <v>476</v>
       </c>
       <c r="F56" t="s">
-        <v>520</v>
+        <v>566</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3068,19 +3208,19 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="D57" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="E57" t="s">
-        <v>442</v>
+        <v>477</v>
       </c>
       <c r="F57" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3088,19 +3228,19 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C58" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="D58" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="E58" t="s">
-        <v>443</v>
+        <v>478</v>
       </c>
       <c r="F58" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3108,19 +3248,19 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="D59" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="E59" t="s">
-        <v>444</v>
+        <v>479</v>
       </c>
       <c r="F59" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3128,19 +3268,19 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D60" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="E60" t="s">
-        <v>445</v>
+        <v>480</v>
       </c>
       <c r="F60" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3148,19 +3288,19 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D61" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="E61" t="s">
-        <v>446</v>
+        <v>481</v>
       </c>
       <c r="F61" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3168,19 +3308,19 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D62" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="E62" t="s">
-        <v>447</v>
+        <v>482</v>
       </c>
       <c r="F62" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3188,16 +3328,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D63" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="E63" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="F63" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3205,16 +3345,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D64" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="E64" t="s">
-        <v>449</v>
+        <v>484</v>
       </c>
       <c r="F64" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3222,16 +3362,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D65" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="E65" t="s">
-        <v>450</v>
+        <v>485</v>
       </c>
       <c r="F65" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3239,16 +3379,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D66" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="E66" t="s">
-        <v>451</v>
+        <v>486</v>
       </c>
       <c r="F66" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3256,16 +3396,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D67" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="E67" t="s">
-        <v>452</v>
+        <v>487</v>
       </c>
       <c r="F67" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3273,16 +3413,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="E68" t="s">
-        <v>453</v>
+        <v>488</v>
       </c>
       <c r="F68" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3290,13 +3430,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E69" t="s">
-        <v>454</v>
+        <v>489</v>
       </c>
       <c r="F69" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3304,16 +3444,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D70" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="E70" t="s">
-        <v>455</v>
+        <v>490</v>
       </c>
       <c r="F70" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3321,16 +3461,16 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="E71" t="s">
-        <v>456</v>
+        <v>491</v>
       </c>
       <c r="F71" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3338,16 +3478,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="C72" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="E72" t="s">
-        <v>457</v>
+        <v>492</v>
       </c>
       <c r="F72" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3355,16 +3495,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C73" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="E73" t="s">
-        <v>458</v>
+        <v>493</v>
       </c>
       <c r="F73" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3372,13 +3512,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>459</v>
+        <v>494</v>
       </c>
       <c r="F74" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3386,16 +3526,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D75" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="E75" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
       <c r="F75" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3403,16 +3543,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C76" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="E76" t="s">
-        <v>461</v>
+        <v>496</v>
       </c>
       <c r="F76" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3420,16 +3560,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="C77" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E77" t="s">
-        <v>462</v>
+        <v>497</v>
       </c>
       <c r="F77" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3437,16 +3577,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D78" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="E78" t="s">
-        <v>463</v>
+        <v>498</v>
       </c>
       <c r="F78" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3454,16 +3594,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="D79" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="E79" t="s">
-        <v>464</v>
+        <v>499</v>
       </c>
       <c r="F79" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3471,16 +3611,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D80" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="E80" t="s">
-        <v>465</v>
+        <v>500</v>
       </c>
       <c r="F80" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3488,16 +3628,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D81" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="E81" t="s">
-        <v>466</v>
+        <v>501</v>
       </c>
       <c r="F81" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3505,16 +3645,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="D82" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="E82" t="s">
-        <v>467</v>
+        <v>502</v>
       </c>
       <c r="F82" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3522,16 +3662,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="E83" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="F83" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3539,16 +3679,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="D84" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="E84" t="s">
-        <v>469</v>
+        <v>504</v>
       </c>
       <c r="F84" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3556,16 +3696,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D85" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="E85" t="s">
-        <v>470</v>
+        <v>505</v>
       </c>
       <c r="F85" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3573,16 +3713,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="D86" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="E86" t="s">
-        <v>471</v>
+        <v>506</v>
       </c>
       <c r="F86" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3590,16 +3730,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D87" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="E87" t="s">
-        <v>472</v>
+        <v>507</v>
       </c>
       <c r="F87" t="s">
-        <v>525</v>
+        <v>571</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3607,16 +3747,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D88" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="E88" t="s">
-        <v>473</v>
+        <v>508</v>
       </c>
       <c r="F88" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3624,19 +3764,19 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C89" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="D89" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="E89" t="s">
-        <v>474</v>
+        <v>509</v>
       </c>
       <c r="F89" t="s">
-        <v>520</v>
+        <v>566</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3644,19 +3784,19 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C90" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="E90" t="s">
-        <v>475</v>
+        <v>510</v>
       </c>
       <c r="F90" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3664,16 +3804,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D91" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="E91" t="s">
-        <v>476</v>
+        <v>511</v>
       </c>
       <c r="F91" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3681,19 +3821,19 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C92" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="D92" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="E92" t="s">
-        <v>477</v>
+        <v>512</v>
       </c>
       <c r="F92" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3701,19 +3841,19 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="D93" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="E93" t="s">
-        <v>478</v>
+        <v>513</v>
       </c>
       <c r="F93" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3721,24 +3861,33 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D94" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="E94" t="s">
-        <v>479</v>
+        <v>514</v>
       </c>
       <c r="F94" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>97</v>
       </c>
+      <c r="B95" t="s">
+        <v>201</v>
+      </c>
+      <c r="D95" t="s">
+        <v>384</v>
+      </c>
+      <c r="E95" t="s">
+        <v>515</v>
+      </c>
       <c r="F95" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3746,16 +3895,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D96" t="s">
-        <v>359</v>
+        <v>385</v>
       </c>
       <c r="E96" t="s">
-        <v>480</v>
+        <v>516</v>
       </c>
       <c r="F96" t="s">
-        <v>514</v>
+        <v>556</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3763,16 +3912,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="D97" t="s">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="E97" t="s">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="F97" t="s">
-        <v>510</v>
+        <v>572</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3780,16 +3929,19 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>193</v>
+        <v>151</v>
+      </c>
+      <c r="C98" t="s">
+        <v>267</v>
       </c>
       <c r="D98" t="s">
-        <v>361</v>
+        <v>387</v>
       </c>
       <c r="E98" t="s">
-        <v>482</v>
+        <v>518</v>
       </c>
       <c r="F98" t="s">
-        <v>526</v>
+        <v>559</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3797,19 +3949,19 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="C99" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="D99" t="s">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="E99" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
       <c r="F99" t="s">
-        <v>513</v>
+        <v>572</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3817,19 +3969,19 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C100" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D100" t="s">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="E100" t="s">
-        <v>484</v>
+        <v>520</v>
       </c>
       <c r="F100" t="s">
-        <v>526</v>
+        <v>572</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3837,19 +3989,19 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="C101" t="s">
-        <v>254</v>
-      </c>
-      <c r="D101" t="s">
-        <v>364</v>
+        <v>270</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>390</v>
       </c>
       <c r="E101" t="s">
-        <v>485</v>
+        <v>521</v>
       </c>
       <c r="F101" t="s">
-        <v>526</v>
+        <v>559</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3857,19 +4009,19 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C102" t="s">
-        <v>255</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>365</v>
+        <v>271</v>
+      </c>
+      <c r="D102" t="s">
+        <v>391</v>
       </c>
       <c r="E102" t="s">
-        <v>486</v>
+        <v>522</v>
       </c>
       <c r="F102" t="s">
-        <v>513</v>
+        <v>568</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3877,19 +4029,19 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C103" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D103" t="s">
-        <v>366</v>
+        <v>392</v>
       </c>
       <c r="E103" t="s">
-        <v>487</v>
+        <v>523</v>
       </c>
       <c r="F103" t="s">
-        <v>522</v>
+        <v>568</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3897,19 +4049,19 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="C104" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="D104" t="s">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="E104" t="s">
-        <v>488</v>
+        <v>444</v>
       </c>
       <c r="F104" t="s">
-        <v>522</v>
+        <v>559</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3917,53 +4069,53 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="D105" t="s">
-        <v>368</v>
+        <v>394</v>
       </c>
       <c r="E105" t="s">
-        <v>409</v>
+        <v>524</v>
       </c>
       <c r="F105" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>108</v>
       </c>
-      <c r="B106" t="s">
-        <v>197</v>
-      </c>
-      <c r="C106" t="s">
-        <v>259</v>
-      </c>
       <c r="D106" t="s">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="E106" t="s">
-        <v>489</v>
+        <v>525</v>
       </c>
       <c r="F106" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>109</v>
       </c>
+      <c r="B107" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" t="s">
+        <v>275</v>
+      </c>
       <c r="D107" t="s">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="E107" t="s">
-        <v>490</v>
+        <v>526</v>
       </c>
       <c r="F107" t="s">
-        <v>513</v>
+        <v>570</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3971,19 +4123,19 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C108" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="D108" t="s">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="E108" t="s">
-        <v>491</v>
+        <v>527</v>
       </c>
       <c r="F108" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3991,19 +4143,19 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="C109" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D109" t="s">
-        <v>372</v>
+        <v>398</v>
       </c>
       <c r="E109" t="s">
-        <v>492</v>
+        <v>528</v>
       </c>
       <c r="F109" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4011,19 +4163,19 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
       <c r="C110" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="D110" t="s">
-        <v>373</v>
+        <v>399</v>
       </c>
       <c r="E110" t="s">
-        <v>493</v>
+        <v>529</v>
       </c>
       <c r="F110" t="s">
-        <v>524</v>
+        <v>569</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4031,19 +4183,19 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="C111" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="D111" t="s">
-        <v>374</v>
+        <v>400</v>
       </c>
       <c r="E111" t="s">
-        <v>494</v>
+        <v>530</v>
       </c>
       <c r="F111" t="s">
-        <v>523</v>
+        <v>573</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4051,19 +4203,19 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="C112" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="D112" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="E112" t="s">
-        <v>495</v>
+        <v>531</v>
       </c>
       <c r="F112" t="s">
-        <v>527</v>
+        <v>569</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4071,19 +4223,19 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>202</v>
+        <v>143</v>
       </c>
       <c r="C113" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="D113" t="s">
-        <v>376</v>
+        <v>402</v>
       </c>
       <c r="E113" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="F113" t="s">
-        <v>523</v>
+        <v>570</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4091,19 +4243,19 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="C114" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="D114" t="s">
-        <v>377</v>
+        <v>403</v>
       </c>
       <c r="E114" t="s">
-        <v>497</v>
+        <v>533</v>
       </c>
       <c r="F114" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4111,59 +4263,59 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="D115" t="s">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="E115" t="s">
-        <v>498</v>
+        <v>534</v>
       </c>
       <c r="F115" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B116" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="C116" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D116" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="E116" t="s">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="F116" t="s">
-        <v>524</v>
+        <v>559</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="C117" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="D117" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="E117" t="s">
-        <v>500</v>
+        <v>536</v>
       </c>
       <c r="F117" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -4171,19 +4323,19 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="C118" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="D118" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="E118" t="s">
-        <v>501</v>
+        <v>537</v>
       </c>
       <c r="F118" t="s">
-        <v>513</v>
+        <v>557</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -4191,19 +4343,19 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C119" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="D119" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="E119" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="F119" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4211,19 +4363,19 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="C120" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="D120" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="E120" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="F120" t="s">
-        <v>511</v>
+        <v>559</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4231,19 +4383,19 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C121" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="D121" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="E121" t="s">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="F121" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4251,19 +4403,19 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="C122" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D122" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="E122" t="s">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="F122" t="s">
-        <v>513</v>
+        <v>565</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4271,19 +4423,19 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="C123" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="D123" t="s">
-        <v>385</v>
+        <v>411</v>
       </c>
       <c r="E123" t="s">
-        <v>506</v>
+        <v>542</v>
       </c>
       <c r="F123" t="s">
-        <v>519</v>
+        <v>565</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -4291,19 +4443,19 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C124" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="D124" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="E124" t="s">
-        <v>507</v>
+        <v>543</v>
       </c>
       <c r="F124" t="s">
-        <v>519</v>
+        <v>565</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4311,19 +4463,19 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C125" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="D125" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="E125" t="s">
-        <v>508</v>
+        <v>544</v>
       </c>
       <c r="F125" t="s">
-        <v>519</v>
+        <v>559</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -4331,24 +4483,221 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
+        <v>216</v>
+      </c>
+      <c r="C126" t="s">
+        <v>291</v>
+      </c>
+      <c r="D126" t="s">
+        <v>414</v>
+      </c>
+      <c r="E126" t="s">
+        <v>545</v>
+      </c>
+      <c r="F126" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>128</v>
+      </c>
+      <c r="B127" t="s">
+        <v>138</v>
+      </c>
+      <c r="C127" t="s">
+        <v>292</v>
+      </c>
+      <c r="D127" t="s">
+        <v>415</v>
+      </c>
+      <c r="E127" t="s">
+        <v>546</v>
+      </c>
+      <c r="F127" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>129</v>
+      </c>
+      <c r="B128" t="s">
+        <v>217</v>
+      </c>
+      <c r="C128" t="s">
+        <v>293</v>
+      </c>
+      <c r="D128" t="s">
+        <v>416</v>
+      </c>
+      <c r="E128" t="s">
+        <v>547</v>
+      </c>
+      <c r="F128" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>130</v>
+      </c>
+      <c r="B129" t="s">
+        <v>143</v>
+      </c>
+      <c r="C129" t="s">
+        <v>294</v>
+      </c>
+      <c r="D129" t="s">
+        <v>417</v>
+      </c>
+      <c r="E129" t="s">
+        <v>548</v>
+      </c>
+      <c r="F129" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>131</v>
+      </c>
+      <c r="B130" t="s">
+        <v>218</v>
+      </c>
+      <c r="C130" t="s">
+        <v>295</v>
+      </c>
+      <c r="D130" t="s">
+        <v>418</v>
+      </c>
+      <c r="E130" t="s">
+        <v>549</v>
+      </c>
+      <c r="F130" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" t="s">
+        <v>146</v>
+      </c>
+      <c r="C131" t="s">
+        <v>296</v>
+      </c>
+      <c r="D131" t="s">
+        <v>419</v>
+      </c>
+      <c r="E131" t="s">
+        <v>550</v>
+      </c>
+      <c r="F131" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>133</v>
+      </c>
+      <c r="B132" t="s">
+        <v>146</v>
+      </c>
+      <c r="C132" t="s">
+        <v>297</v>
+      </c>
+      <c r="D132" t="s">
+        <v>420</v>
+      </c>
+      <c r="E132" t="s">
+        <v>551</v>
+      </c>
+      <c r="F132" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>134</v>
+      </c>
+      <c r="B133" t="s">
+        <v>172</v>
+      </c>
+      <c r="C133" t="s">
+        <v>298</v>
+      </c>
+      <c r="D133" t="s">
+        <v>421</v>
+      </c>
+      <c r="E133" t="s">
+        <v>552</v>
+      </c>
+      <c r="F133" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>135</v>
+      </c>
+      <c r="B134" t="s">
+        <v>164</v>
+      </c>
+      <c r="C134" t="s">
+        <v>253</v>
+      </c>
+      <c r="D134" t="s">
+        <v>422</v>
+      </c>
+      <c r="E134" t="s">
+        <v>553</v>
+      </c>
+      <c r="F134" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>136</v>
+      </c>
+      <c r="B135" t="s">
+        <v>219</v>
+      </c>
+      <c r="C135" t="s">
+        <v>299</v>
+      </c>
+      <c r="D135" t="s">
+        <v>423</v>
+      </c>
+      <c r="E135" t="s">
+        <v>554</v>
+      </c>
+      <c r="F135" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" t="s">
         <v>137</v>
       </c>
-      <c r="C126" t="s">
-        <v>275</v>
-      </c>
-      <c r="D126" t="s">
-        <v>388</v>
-      </c>
-      <c r="E126" t="s">
-        <v>509</v>
-      </c>
-      <c r="F126" t="s">
-        <v>513</v>
+      <c r="B136" t="s">
+        <v>220</v>
+      </c>
+      <c r="C136" t="s">
+        <v>300</v>
+      </c>
+      <c r="E136" t="s">
+        <v>555</v>
+      </c>
+      <c r="F136" t="s">
+        <v>563</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D102" r:id="rId1"/>
+    <hyperlink ref="D101" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adapting for fairdom hub
</commit_message>
<xml_diff>
--- a/results/publications.xlsx
+++ b/results/publications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="623">
   <si>
     <t>title</t>
   </si>
@@ -434,6 +434,54 @@
     <t>SECOND EXPOSURE TO ACETAMINOPHEN OVERDOSE IS  ASSOCIATED WITH LIVER FIBROSIS IN MICE</t>
   </si>
   <si>
+    <t>Non-invasive structure-function assessment of the liver by 2D time-harmonic elastography and the dynamic Liver MAximum capacity (LiMAx) test.</t>
+  </si>
+  <si>
+    <t>Hepatic CYP1A2 activity in liver tumors and the implications for preoperative volume-function analysis.</t>
+  </si>
+  <si>
+    <t>Wet-tip versus dry-tip regimes of osmotically driven fluid flow</t>
+  </si>
+  <si>
+    <t>Common NOD2 Risk Variants as Major Susceptibility Factors for Bacterial Infections in Compensated Cirrhosis.</t>
+  </si>
+  <si>
+    <t>Glial cell line-derived neurotrophic factor (GDNF) mediates hepatic stellate cell activation via ALK5/Smad signalling.</t>
+  </si>
+  <si>
+    <t>Aged Abcb4-/- mice upon acute sublethal chemical insult recapitulate features of acute-on-chronic liver failure in patients</t>
+  </si>
+  <si>
+    <t>ECM1 is a gatekeeper that restrains TGF-β activation to maintain liver homeostasis and prevent fibrogenesis</t>
+  </si>
+  <si>
+    <t>Simultaneous isolation of parenchymal and non-parenchymal cells from healthy and diseased mice liver</t>
+  </si>
+  <si>
+    <t>Jagged-1 upregulation in stressed hepatocytes is crucial for liver regeneration</t>
+  </si>
+  <si>
+    <t>Cellular and nuclear hepatocyte ploidy represent a repository in regenerating livers</t>
+  </si>
+  <si>
+    <t>Liver cell type specific discrimination of TGF-beta signaling and outcome in vitro and in vivo</t>
+  </si>
+  <si>
+    <t>CYP2E1 recovery is associated with a pericentral fibrosis pattern after repeated CCl4 insults</t>
+  </si>
+  <si>
+    <t>Transcription factor TRIM33 controls liver progenitor cell towards hepatocyte differentiation through synergizing with phosphorylated Smad2/3 in liver cirrhosis</t>
+  </si>
+  <si>
+    <t>Maintenance of functional hepatocellular polarity determines recovery in acute-on-chronic liver failure</t>
+  </si>
+  <si>
+    <t>Liquid-crystal organization of liver tissue.</t>
+  </si>
+  <si>
+    <t>Correlative SMLM and electron tomography reveals endosome nanoscale domains.</t>
+  </si>
+  <si>
     <t>J Integr Bioinform</t>
   </si>
   <si>
@@ -683,6 +731,18 @@
     <t>EXCLI</t>
   </si>
   <si>
+    <t>J Gastroenterol Hepatol</t>
+  </si>
+  <si>
+    <t>Am J Physiol Gastrointest Liver Physiol</t>
+  </si>
+  <si>
+    <t>Clin Transl Gastroenterol</t>
+  </si>
+  <si>
+    <t>Traffic</t>
+  </si>
+  <si>
     <t>2017-02-12</t>
   </si>
   <si>
@@ -923,6 +983,21 @@
     <t>2019-02-06</t>
   </si>
   <si>
+    <t>2019-02-13</t>
+  </si>
+  <si>
+    <t>2019-03-14</t>
+  </si>
+  <si>
+    <t>2019-12-01</t>
+  </si>
+  <si>
+    <t>2019-06-06</t>
+  </si>
+  <si>
+    <t>2019-06-17</t>
+  </si>
+  <si>
     <t>J Integr Bioinform. 2016 Dec 18;13(3):289. doi: 10.2390/biecoll-jib-2016-289.</t>
   </si>
   <si>
@@ -1292,6 +1367,30 @@
     <t>Transplantation. 2018 Oct;102(10):e424-e430. doi: 10.1097/TP.0000000000002356.</t>
   </si>
   <si>
+    <t>J Gastroenterol Hepatol. 2019 Feb 13. doi: 10.1111/jgh.14629.</t>
+  </si>
+  <si>
+    <t>Am J Physiol Gastrointest Liver Physiol. 2019 Mar 14. doi: 10.1152/ajpgi.00335.2018.</t>
+  </si>
+  <si>
+    <t>Sci Rep 9(1) : 823</t>
+  </si>
+  <si>
+    <t>Clin Transl Gastroenterol. 2019 Jan;10(1):e00002. doi: 10.14309/ctg.0000000000000002.</t>
+  </si>
+  <si>
+    <t>Gut. 2019 Jun 6. pii: gutjnl-2018-317872. doi: 10.1136/gutjnl-2018-317872.</t>
+  </si>
+  <si>
+    <t>Zeitschrift für Gastroenterologie 57</t>
+  </si>
+  <si>
+    <t>Elife. 2019 Jun 17;8. pii: 44860. doi: 10.7554/eLife.44860.</t>
+  </si>
+  <si>
+    <t>Traffic. 2019 Jun 17. doi: 10.1111/tra.12671.</t>
+  </si>
+  <si>
     <t>['F. Schreiber', 'G. D. Bader', 'P. Gleeson', 'Martin Golebiewski', 'M. Hucka', 'N. Le Novere', 'C. Myers', 'D. Nickerson', 'B. Sommer', 'D. Walthemath']</t>
   </si>
   <si>
@@ -1688,58 +1787,106 @@
     <t>['Seddik Hammad']</t>
   </si>
   <si>
-    <t>{'data': [{'type': 'projects', 'id': '2'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '5'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '7'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '3'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '4'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '5'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '9'}, {'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '5'}, {'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '10'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '8'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '4'}, {'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '9'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '2'}, {'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '6'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '10'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '5'}, {'type': 'projects', 'id': '13'}]}</t>
-  </si>
-  <si>
-    <t>{'data': [{'type': 'projects', 'id': '2'}, {'type': 'projects', 'id': '10'}, {'type': 'projects', 'id': '13'}]}</t>
+    <t>['Niklas Heucke', 'Tilo Wuensch', 'J. Mohr', 'M. Kaffarnik', 'R. Arsenic', 'B. Sinn', 'T. Muller', 'J. Pratschke', 'Martin Stockmann', 'I. Sack', 'H. Tzschatzsch']</t>
+  </si>
+  <si>
+    <t>['Tilo Wuensch', 'Niklas Heucke', 'J. Wizenty', 'J. Quint', 'B. Sinn', 'R. Arsenic', 'M. Jara', 'M. Kaffarnik', 'J. Pratschke', 'Martin Stockmann']</t>
+  </si>
+  <si>
+    <t>['Oleksandr Ostrenko', 'Jochen Hampe', 'Lutz Brusch']</t>
+  </si>
+  <si>
+    <t>['Matthias Reichert', 'C. Ripoll', 'M. Casper', 'R. Greinert', 'E. Vandieken', 'F. Grunhage', 'B. Appenrodt', 'A. Zipprich', 'Frank Lammert']</t>
+  </si>
+  <si>
+    <t>['L. Tao', 'W. Ma', 'L. Wu', 'M. Xu', 'Y. Yang', 'W. Zhang', 'W. Sha', 'H. Li', 'J. Xu', 'R. Feng', 'D. Xue', 'J. Zhang', 'Steven Dooley', 'E. Seki', 'P. Liu', 'C. Liu']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad', 'Jan Hengstler', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['Steven Dooley', 'W Fan', 'Seddik Hammad', 'K Gould', 'T Longerich', 'T Liu', 'W Chen', 'C Liu', 'J Hou', 'J Jia', 'B Sun']</t>
+  </si>
+  <si>
+    <t>['B Dewidar', 'A Dropmann', 'K Gould', 'V Hartwig', 'C Dormann', 'Steven Dooley', 'Seddik Hammad']</t>
+  </si>
+  <si>
+    <t>['B Dewidar', 'Seddik Hammad', 'MP Ebert', 'Jan Hengstler', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad', 'U Dahmen', 'A Othman', 'I Recklinghausen', 'Jan Hengstler', 'U Klingmüller', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['M Han', 'ZC Nwosu', 'MP Ebert', 'Seddik Hammad', 'Steven Dooley', 'C Meyer']</t>
+  </si>
+  <si>
+    <t>['Seddik Hammad', 'Jieling Zhao', 'Yi Yin', 'Ayham Zaza', 'Dirk Drasdo', 'Jan Hengstler', 'Steven Dooley']</t>
+  </si>
+  <si>
+    <t>['T Lin', 'S Wang', 'C Shao', 'X Yuan', 'F Wandrer', 'H Bantel', 'MP Ebert', 'H Ding', 'Steven Dooley', 'HL Weng']</t>
+  </si>
+  <si>
+    <t>['S Wang', 'R Feng', 'X Yuan', 'F Wandrer', 'MP Ebert', 'H Bantel', 'H Li', 'Steven Dooley', 'HL Weng']</t>
+  </si>
+  <si>
+    <t>['H. Morales-Navarrete', 'H. Nonaka', 'A. Scholich', 'F. Segovia-Miranda', 'W. de Back', 'K. Meyer', 'R. L. Bogorad', 'V. Koteliansky', 'Lutz Brusch', 'Y. Kalaidzidis', 'F. Julicher', 'B. M. Friedrich', 'Marino Zerial']</t>
+  </si>
+  <si>
+    <t>['C. Franke', 'U. Repnik', 'S. Segeletz', 'N. Brouilly', 'Y. Kalaidzidis', 'J. M. Verbavatz', 'Marino Zerial']</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '2', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '5', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '7', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '3', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '4', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '5', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '9', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '10', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '8', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '4', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '9', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '2', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '6', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '10', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '5', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
+  </si>
+  <si>
+    <t>{'data': [{'id': '2', 'type': 'projects'}, {'id': '10', 'type': 'projects'}, {'id': '13', 'type': 'projects'}]}</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2141,19 +2288,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="E2" t="s">
-        <v>424</v>
+        <v>457</v>
       </c>
       <c r="F2" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2161,19 +2308,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="D3" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="E3" t="s">
-        <v>425</v>
+        <v>458</v>
       </c>
       <c r="F3" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2181,19 +2328,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="E4" t="s">
-        <v>426</v>
+        <v>459</v>
       </c>
       <c r="F4" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2201,19 +2348,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D5" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="E5" t="s">
-        <v>427</v>
+        <v>460</v>
       </c>
       <c r="F5" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2221,19 +2368,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="E6" t="s">
-        <v>428</v>
+        <v>461</v>
       </c>
       <c r="F6" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2241,19 +2388,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="D7" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="E7" t="s">
-        <v>429</v>
+        <v>462</v>
       </c>
       <c r="F7" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2261,19 +2408,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D8" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="E8" t="s">
-        <v>430</v>
+        <v>463</v>
       </c>
       <c r="F8" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2281,19 +2428,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="E9" t="s">
-        <v>431</v>
+        <v>464</v>
       </c>
       <c r="F9" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2301,19 +2448,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="E10" t="s">
-        <v>432</v>
+        <v>465</v>
       </c>
       <c r="F10" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2321,19 +2468,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>433</v>
+        <v>466</v>
       </c>
       <c r="F11" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2341,19 +2488,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="E12" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="F12" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2361,19 +2508,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="E13" t="s">
-        <v>435</v>
+        <v>468</v>
       </c>
       <c r="F13" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2381,19 +2528,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="E14" t="s">
-        <v>436</v>
+        <v>469</v>
       </c>
       <c r="F14" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2401,19 +2548,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="E15" t="s">
-        <v>437</v>
+        <v>470</v>
       </c>
       <c r="F15" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2421,19 +2568,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="C16" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="E16" t="s">
-        <v>438</v>
+        <v>471</v>
       </c>
       <c r="F16" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2441,19 +2588,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="D17" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="E17" t="s">
-        <v>439</v>
+        <v>472</v>
       </c>
       <c r="F17" t="s">
-        <v>561</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2461,19 +2608,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="D18" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="E18" t="s">
-        <v>440</v>
+        <v>473</v>
       </c>
       <c r="F18" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2481,19 +2628,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="D19" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="E19" t="s">
-        <v>441</v>
+        <v>474</v>
       </c>
       <c r="F19" t="s">
-        <v>562</v>
+        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2501,19 +2648,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="E20" t="s">
-        <v>442</v>
+        <v>475</v>
       </c>
       <c r="F20" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2521,19 +2668,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="E21" t="s">
-        <v>443</v>
+        <v>476</v>
       </c>
       <c r="F21" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2541,19 +2688,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D22" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="E22" t="s">
-        <v>444</v>
+        <v>477</v>
       </c>
       <c r="F22" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2561,19 +2708,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="D23" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="E23" t="s">
-        <v>445</v>
+        <v>478</v>
       </c>
       <c r="F23" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2581,19 +2728,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D24" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
       <c r="E24" t="s">
-        <v>446</v>
+        <v>479</v>
       </c>
       <c r="F24" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2601,19 +2748,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C25" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="D25" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="E25" t="s">
-        <v>447</v>
+        <v>480</v>
       </c>
       <c r="F25" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2621,19 +2768,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="D26" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="E26" t="s">
-        <v>448</v>
+        <v>481</v>
       </c>
       <c r="F26" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2641,19 +2788,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D27" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="E27" t="s">
-        <v>449</v>
+        <v>482</v>
       </c>
       <c r="F27" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2661,19 +2808,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C28" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D28" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="E28" t="s">
-        <v>450</v>
+        <v>483</v>
       </c>
       <c r="F28" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2681,19 +2828,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D29" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="E29" t="s">
-        <v>450</v>
+        <v>483</v>
       </c>
       <c r="F29" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2701,19 +2848,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C30" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="D30" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="E30" t="s">
-        <v>451</v>
+        <v>484</v>
       </c>
       <c r="F30" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2721,19 +2868,19 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="D31" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="E31" t="s">
-        <v>452</v>
+        <v>485</v>
       </c>
       <c r="F31" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2741,19 +2888,19 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C32" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D32" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="E32" t="s">
-        <v>453</v>
+        <v>486</v>
       </c>
       <c r="F32" t="s">
-        <v>562</v>
+        <v>611</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2761,19 +2908,19 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D33" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="E33" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="F33" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2781,19 +2928,19 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="D34" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="E34" t="s">
-        <v>455</v>
+        <v>488</v>
       </c>
       <c r="F34" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2801,19 +2948,19 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C35" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="D35" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="E35" t="s">
-        <v>456</v>
+        <v>489</v>
       </c>
       <c r="F35" t="s">
-        <v>564</v>
+        <v>613</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2821,19 +2968,19 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D36" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="E36" t="s">
-        <v>457</v>
+        <v>490</v>
       </c>
       <c r="F36" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2841,16 +2988,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="E37" t="s">
-        <v>458</v>
+        <v>491</v>
       </c>
       <c r="F37" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2858,16 +3005,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="D38" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="E38" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="F38" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2875,16 +3022,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="D39" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="E39" t="s">
-        <v>460</v>
+        <v>493</v>
       </c>
       <c r="F39" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2892,19 +3039,19 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D40" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="E40" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
       <c r="F40" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2912,19 +3059,19 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D41" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="E41" t="s">
-        <v>462</v>
+        <v>495</v>
       </c>
       <c r="F41" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2932,16 +3079,16 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="D42" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="E42" t="s">
-        <v>463</v>
+        <v>496</v>
       </c>
       <c r="F42" t="s">
-        <v>568</v>
+        <v>617</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2949,16 +3096,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="D43" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="E43" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="F43" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2966,16 +3113,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="D44" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="E44" t="s">
-        <v>465</v>
+        <v>498</v>
       </c>
       <c r="F44" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2983,16 +3130,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="E45" t="s">
-        <v>466</v>
+        <v>499</v>
       </c>
       <c r="F45" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3000,16 +3147,16 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="E46" t="s">
-        <v>467</v>
+        <v>500</v>
       </c>
       <c r="F46" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3017,16 +3164,16 @@
         <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="D47" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
       <c r="E47" t="s">
-        <v>436</v>
+        <v>469</v>
       </c>
       <c r="F47" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3034,16 +3181,16 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D48" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="E48" t="s">
-        <v>468</v>
+        <v>501</v>
       </c>
       <c r="F48" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3051,19 +3198,19 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C49" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D49" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="E49" t="s">
-        <v>469</v>
+        <v>502</v>
       </c>
       <c r="F49" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3071,19 +3218,19 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="C50" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D50" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="E50" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="F50" t="s">
-        <v>569</v>
+        <v>618</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3091,16 +3238,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="D51" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="E51" t="s">
-        <v>471</v>
+        <v>504</v>
       </c>
       <c r="F51" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3108,19 +3255,19 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C52" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D52" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="E52" t="s">
-        <v>472</v>
+        <v>505</v>
       </c>
       <c r="F52" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3128,19 +3275,19 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C53" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="D53" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="E53" t="s">
-        <v>473</v>
+        <v>506</v>
       </c>
       <c r="F53" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3148,19 +3295,19 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C54" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D54" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="E54" t="s">
-        <v>474</v>
+        <v>507</v>
       </c>
       <c r="F54" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3168,19 +3315,19 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C55" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="D55" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="E55" t="s">
-        <v>475</v>
+        <v>508</v>
       </c>
       <c r="F55" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3188,19 +3335,19 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="D56" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="E56" t="s">
-        <v>476</v>
+        <v>509</v>
       </c>
       <c r="F56" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3208,19 +3355,19 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C57" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="D57" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="E57" t="s">
-        <v>477</v>
+        <v>510</v>
       </c>
       <c r="F57" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3228,19 +3375,19 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="D58" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="E58" t="s">
-        <v>478</v>
+        <v>511</v>
       </c>
       <c r="F58" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3248,19 +3395,19 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="C59" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="D59" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="E59" t="s">
-        <v>479</v>
+        <v>512</v>
       </c>
       <c r="F59" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3268,19 +3415,19 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="D60" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="E60" t="s">
-        <v>480</v>
+        <v>513</v>
       </c>
       <c r="F60" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3288,19 +3435,19 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C61" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="D61" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="E61" t="s">
-        <v>481</v>
+        <v>514</v>
       </c>
       <c r="F61" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3308,19 +3455,19 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="D62" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="E62" t="s">
-        <v>482</v>
+        <v>515</v>
       </c>
       <c r="F62" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3328,16 +3475,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D63" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="E63" t="s">
-        <v>483</v>
+        <v>516</v>
       </c>
       <c r="F63" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3345,16 +3492,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D64" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="E64" t="s">
-        <v>484</v>
+        <v>517</v>
       </c>
       <c r="F64" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3362,16 +3509,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D65" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="E65" t="s">
-        <v>485</v>
+        <v>518</v>
       </c>
       <c r="F65" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3379,16 +3526,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="E66" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="F66" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3396,16 +3543,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D67" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="E67" t="s">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="F67" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3413,16 +3560,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
       <c r="E68" t="s">
-        <v>488</v>
+        <v>521</v>
       </c>
       <c r="F68" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3430,13 +3577,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E69" t="s">
-        <v>489</v>
+        <v>522</v>
       </c>
       <c r="F69" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3444,16 +3591,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D70" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="E70" t="s">
-        <v>490</v>
+        <v>523</v>
       </c>
       <c r="F70" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3461,16 +3608,16 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="E71" t="s">
-        <v>491</v>
+        <v>524</v>
       </c>
       <c r="F71" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3478,16 +3625,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C72" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E72" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
       <c r="F72" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3495,16 +3642,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="C73" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E73" t="s">
-        <v>493</v>
+        <v>526</v>
       </c>
       <c r="F73" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3512,13 +3659,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="E74" t="s">
-        <v>494</v>
+        <v>527</v>
       </c>
       <c r="F74" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3526,16 +3673,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="D75" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="E75" t="s">
-        <v>495</v>
+        <v>528</v>
       </c>
       <c r="F75" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3543,16 +3690,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C76" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="E76" t="s">
-        <v>496</v>
+        <v>529</v>
       </c>
       <c r="F76" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3560,16 +3707,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="C77" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="E77" t="s">
-        <v>497</v>
+        <v>530</v>
       </c>
       <c r="F77" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3577,16 +3724,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="D78" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="E78" t="s">
-        <v>498</v>
+        <v>531</v>
       </c>
       <c r="F78" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3594,16 +3741,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D79" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="E79" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
       <c r="F79" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3611,16 +3758,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D80" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
       <c r="E80" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="F80" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3628,16 +3775,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D81" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="E81" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="F81" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3645,16 +3792,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="E82" t="s">
-        <v>502</v>
+        <v>535</v>
       </c>
       <c r="F82" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3662,16 +3809,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D83" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="E83" t="s">
-        <v>503</v>
+        <v>536</v>
       </c>
       <c r="F83" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3679,16 +3826,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D84" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="E84" t="s">
-        <v>504</v>
+        <v>537</v>
       </c>
       <c r="F84" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3696,16 +3843,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D85" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="E85" t="s">
-        <v>505</v>
+        <v>538</v>
       </c>
       <c r="F85" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3713,16 +3860,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D86" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="E86" t="s">
-        <v>506</v>
+        <v>539</v>
       </c>
       <c r="F86" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3730,16 +3877,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="D87" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="E87" t="s">
-        <v>507</v>
+        <v>540</v>
       </c>
       <c r="F87" t="s">
-        <v>571</v>
+        <v>620</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3747,16 +3894,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="D88" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="E88" t="s">
-        <v>508</v>
+        <v>541</v>
       </c>
       <c r="F88" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3764,19 +3911,19 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C89" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="D89" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
       <c r="E89" t="s">
-        <v>509</v>
+        <v>542</v>
       </c>
       <c r="F89" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3784,19 +3931,19 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C90" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D90" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="E90" t="s">
-        <v>510</v>
+        <v>543</v>
       </c>
       <c r="F90" t="s">
-        <v>567</v>
+        <v>616</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3804,16 +3951,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="D91" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="E91" t="s">
-        <v>511</v>
+        <v>544</v>
       </c>
       <c r="F91" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3821,19 +3968,19 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C92" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="D92" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="E92" t="s">
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="F92" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3841,19 +3988,19 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="C93" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="D93" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="E93" t="s">
-        <v>513</v>
+        <v>546</v>
       </c>
       <c r="F93" t="s">
-        <v>558</v>
+        <v>607</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3861,16 +4008,16 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="D94" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
       <c r="E94" t="s">
-        <v>514</v>
+        <v>547</v>
       </c>
       <c r="F94" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3878,16 +4025,16 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D95" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="E95" t="s">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="F95" t="s">
-        <v>560</v>
+        <v>609</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3895,16 +4042,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="D96" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
       <c r="E96" t="s">
-        <v>516</v>
+        <v>549</v>
       </c>
       <c r="F96" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3912,16 +4059,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D97" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
       <c r="E97" t="s">
-        <v>517</v>
+        <v>550</v>
       </c>
       <c r="F97" t="s">
-        <v>572</v>
+        <v>621</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3929,19 +4076,19 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="C98" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D98" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
       <c r="E98" t="s">
-        <v>518</v>
+        <v>551</v>
       </c>
       <c r="F98" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3949,19 +4096,19 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="C99" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="D99" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="E99" t="s">
-        <v>519</v>
+        <v>552</v>
       </c>
       <c r="F99" t="s">
-        <v>572</v>
+        <v>621</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3969,19 +4116,19 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="C100" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="D100" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="E100" t="s">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="F100" t="s">
-        <v>572</v>
+        <v>621</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3989,19 +4136,19 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="C101" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="E101" t="s">
-        <v>521</v>
+        <v>554</v>
       </c>
       <c r="F101" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4009,19 +4156,19 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C102" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D102" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="E102" t="s">
-        <v>522</v>
+        <v>555</v>
       </c>
       <c r="F102" t="s">
-        <v>568</v>
+        <v>617</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4029,19 +4176,19 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C103" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="D103" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
       <c r="E103" t="s">
-        <v>523</v>
+        <v>556</v>
       </c>
       <c r="F103" t="s">
-        <v>568</v>
+        <v>617</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4049,19 +4196,19 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="C104" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="D104" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="E104" t="s">
-        <v>444</v>
+        <v>477</v>
       </c>
       <c r="F104" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4069,19 +4216,19 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="C105" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="D105" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="E105" t="s">
-        <v>524</v>
+        <v>557</v>
       </c>
       <c r="F105" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4089,13 +4236,13 @@
         <v>108</v>
       </c>
       <c r="D106" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="E106" t="s">
-        <v>525</v>
+        <v>558</v>
       </c>
       <c r="F106" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4103,19 +4250,19 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="C107" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="D107" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="E107" t="s">
-        <v>526</v>
+        <v>559</v>
       </c>
       <c r="F107" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4123,19 +4270,19 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="C108" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D108" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="E108" t="s">
-        <v>527</v>
+        <v>560</v>
       </c>
       <c r="F108" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4143,19 +4290,19 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="C109" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D109" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
       <c r="E109" t="s">
-        <v>528</v>
+        <v>561</v>
       </c>
       <c r="F109" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4163,19 +4310,19 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="D110" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="E110" t="s">
-        <v>529</v>
+        <v>562</v>
       </c>
       <c r="F110" t="s">
-        <v>569</v>
+        <v>618</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4183,19 +4330,19 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C111" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D111" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="E111" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="F111" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4203,19 +4350,19 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C112" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D112" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="E112" t="s">
-        <v>531</v>
+        <v>564</v>
       </c>
       <c r="F112" t="s">
-        <v>569</v>
+        <v>618</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4223,19 +4370,19 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C113" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="D113" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="E113" t="s">
-        <v>532</v>
+        <v>565</v>
       </c>
       <c r="F113" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4243,19 +4390,19 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C114" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="D114" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="E114" t="s">
-        <v>533</v>
+        <v>566</v>
       </c>
       <c r="F114" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4263,19 +4410,19 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="D115" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="E115" t="s">
-        <v>534</v>
+        <v>567</v>
       </c>
       <c r="F115" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -4283,19 +4430,19 @@
         <v>104</v>
       </c>
       <c r="B116" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C116" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D116" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="E116" t="s">
-        <v>535</v>
+        <v>568</v>
       </c>
       <c r="F116" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -4303,19 +4450,19 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="C117" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D117" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="E117" t="s">
-        <v>536</v>
+        <v>569</v>
       </c>
       <c r="F117" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -4323,19 +4470,19 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C118" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="D118" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
       <c r="E118" t="s">
-        <v>537</v>
+        <v>570</v>
       </c>
       <c r="F118" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -4343,19 +4490,19 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C119" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="D119" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="E119" t="s">
-        <v>538</v>
+        <v>571</v>
       </c>
       <c r="F119" t="s">
-        <v>557</v>
+        <v>606</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4363,19 +4510,19 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C120" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="D120" t="s">
-        <v>408</v>
+        <v>433</v>
       </c>
       <c r="E120" t="s">
-        <v>539</v>
+        <v>572</v>
       </c>
       <c r="F120" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4383,19 +4530,19 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="C121" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="D121" t="s">
-        <v>409</v>
+        <v>434</v>
       </c>
       <c r="E121" t="s">
-        <v>540</v>
+        <v>573</v>
       </c>
       <c r="F121" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4403,19 +4550,19 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C122" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D122" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
       <c r="E122" t="s">
-        <v>541</v>
+        <v>574</v>
       </c>
       <c r="F122" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4423,19 +4570,19 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C123" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="D123" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="E123" t="s">
-        <v>542</v>
+        <v>575</v>
       </c>
       <c r="F123" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -4443,19 +4590,19 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C124" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="D124" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="E124" t="s">
-        <v>543</v>
+        <v>576</v>
       </c>
       <c r="F124" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4463,19 +4610,19 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C125" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="D125" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="E125" t="s">
-        <v>544</v>
+        <v>577</v>
       </c>
       <c r="F125" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -4483,19 +4630,19 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C126" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="D126" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="E126" t="s">
-        <v>545</v>
+        <v>578</v>
       </c>
       <c r="F126" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -4503,19 +4650,19 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="C127" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="D127" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="E127" t="s">
-        <v>546</v>
+        <v>579</v>
       </c>
       <c r="F127" t="s">
-        <v>571</v>
+        <v>620</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -4523,19 +4670,19 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C128" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="D128" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="E128" t="s">
-        <v>547</v>
+        <v>580</v>
       </c>
       <c r="F128" t="s">
-        <v>571</v>
+        <v>620</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -4543,19 +4690,19 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C129" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="D129" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="E129" t="s">
-        <v>548</v>
+        <v>581</v>
       </c>
       <c r="F129" t="s">
-        <v>571</v>
+        <v>620</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4563,19 +4710,19 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="C130" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="D130" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="E130" t="s">
-        <v>549</v>
+        <v>582</v>
       </c>
       <c r="F130" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -4583,19 +4730,19 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C131" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="D131" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="E131" t="s">
-        <v>550</v>
+        <v>583</v>
       </c>
       <c r="F131" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -4603,19 +4750,19 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C132" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="D132" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="E132" t="s">
-        <v>551</v>
+        <v>584</v>
       </c>
       <c r="F132" t="s">
-        <v>563</v>
+        <v>612</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -4623,19 +4770,19 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C133" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="D133" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="E133" t="s">
-        <v>552</v>
+        <v>585</v>
       </c>
       <c r="F133" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -4643,19 +4790,19 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="C134" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D134" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="E134" t="s">
-        <v>553</v>
+        <v>586</v>
       </c>
       <c r="F134" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -4663,19 +4810,19 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C135" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D135" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="E135" t="s">
-        <v>554</v>
+        <v>587</v>
       </c>
       <c r="F135" t="s">
-        <v>559</v>
+        <v>608</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -4683,16 +4830,309 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="C136" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="E136" t="s">
-        <v>555</v>
+        <v>588</v>
       </c>
       <c r="F136" t="s">
-        <v>563</v>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" t="s">
+        <v>237</v>
+      </c>
+      <c r="C137" t="s">
+        <v>321</v>
+      </c>
+      <c r="D137" t="s">
+        <v>449</v>
+      </c>
+      <c r="E137" t="s">
+        <v>589</v>
+      </c>
+      <c r="F137" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" t="s">
+        <v>238</v>
+      </c>
+      <c r="C138" t="s">
+        <v>322</v>
+      </c>
+      <c r="D138" t="s">
+        <v>450</v>
+      </c>
+      <c r="E138" t="s">
+        <v>590</v>
+      </c>
+      <c r="F138" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" t="s">
+        <v>323</v>
+      </c>
+      <c r="D139" t="s">
+        <v>451</v>
+      </c>
+      <c r="E139" t="s">
+        <v>591</v>
+      </c>
+      <c r="F139" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" t="s">
+        <v>239</v>
+      </c>
+      <c r="C140" t="s">
+        <v>315</v>
+      </c>
+      <c r="D140" t="s">
+        <v>452</v>
+      </c>
+      <c r="E140" t="s">
+        <v>592</v>
+      </c>
+      <c r="F140" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>142</v>
+      </c>
+      <c r="B141" t="s">
+        <v>166</v>
+      </c>
+      <c r="C141" t="s">
+        <v>324</v>
+      </c>
+      <c r="D141" t="s">
+        <v>453</v>
+      </c>
+      <c r="E141" t="s">
+        <v>593</v>
+      </c>
+      <c r="F141" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>143</v>
+      </c>
+      <c r="C142" t="s">
+        <v>299</v>
+      </c>
+      <c r="D142" t="s">
+        <v>454</v>
+      </c>
+      <c r="E142" t="s">
+        <v>594</v>
+      </c>
+      <c r="F142" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>144</v>
+      </c>
+      <c r="C143" t="s">
+        <v>299</v>
+      </c>
+      <c r="D143" t="s">
+        <v>454</v>
+      </c>
+      <c r="E143" t="s">
+        <v>595</v>
+      </c>
+      <c r="F143" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>145</v>
+      </c>
+      <c r="C144" t="s">
+        <v>299</v>
+      </c>
+      <c r="D144" t="s">
+        <v>454</v>
+      </c>
+      <c r="E144" t="s">
+        <v>596</v>
+      </c>
+      <c r="F144" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>146</v>
+      </c>
+      <c r="C145" t="s">
+        <v>299</v>
+      </c>
+      <c r="D145" t="s">
+        <v>454</v>
+      </c>
+      <c r="E145" t="s">
+        <v>597</v>
+      </c>
+      <c r="F145" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>147</v>
+      </c>
+      <c r="C146" t="s">
+        <v>299</v>
+      </c>
+      <c r="D146" t="s">
+        <v>454</v>
+      </c>
+      <c r="E146" t="s">
+        <v>598</v>
+      </c>
+      <c r="F146" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>148</v>
+      </c>
+      <c r="C147" t="s">
+        <v>299</v>
+      </c>
+      <c r="D147" t="s">
+        <v>454</v>
+      </c>
+      <c r="E147" t="s">
+        <v>599</v>
+      </c>
+      <c r="F147" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>149</v>
+      </c>
+      <c r="C148" t="s">
+        <v>299</v>
+      </c>
+      <c r="D148" t="s">
+        <v>454</v>
+      </c>
+      <c r="E148" t="s">
+        <v>600</v>
+      </c>
+      <c r="F148" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>150</v>
+      </c>
+      <c r="C149" t="s">
+        <v>299</v>
+      </c>
+      <c r="D149" t="s">
+        <v>454</v>
+      </c>
+      <c r="E149" t="s">
+        <v>601</v>
+      </c>
+      <c r="F149" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>151</v>
+      </c>
+      <c r="C150" t="s">
+        <v>299</v>
+      </c>
+      <c r="D150" t="s">
+        <v>454</v>
+      </c>
+      <c r="E150" t="s">
+        <v>602</v>
+      </c>
+      <c r="F150" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>152</v>
+      </c>
+      <c r="B151" t="s">
+        <v>183</v>
+      </c>
+      <c r="C151" t="s">
+        <v>325</v>
+      </c>
+      <c r="D151" t="s">
+        <v>455</v>
+      </c>
+      <c r="E151" t="s">
+        <v>603</v>
+      </c>
+      <c r="F151" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>153</v>
+      </c>
+      <c r="B152" t="s">
+        <v>240</v>
+      </c>
+      <c r="C152" t="s">
+        <v>325</v>
+      </c>
+      <c r="D152" t="s">
+        <v>456</v>
+      </c>
+      <c r="E152" t="s">
+        <v>604</v>
+      </c>
+      <c r="F152" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>